<commit_message>
moved subsets "Coal", "Lignite", "Gas", "SectorCoupling", and "HeatFuels" to file
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB5D89-8F63-43F4-AB1C-7FD3198787A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D28980-B6A8-46D8-9E2B-7E1C15FBE5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_TagTechnologyToSubsets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="239">
   <si>
     <t>Technology</t>
   </si>
@@ -730,6 +730,30 @@
   </si>
   <si>
     <t>PowerBiomass</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>SectorCoupling</t>
+  </si>
+  <si>
+    <t>Heat_Low_Industrial</t>
+  </si>
+  <si>
+    <t>Heat_Medium_Industrial</t>
+  </si>
+  <si>
+    <t>Heat_High_Industrial</t>
+  </si>
+  <si>
+    <t>Heat_Low_Residential</t>
+  </si>
+  <si>
+    <t>HeatFuels</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D866"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
-      <selection activeCell="F419" sqref="F419"/>
+    <sheetView topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="D460" sqref="D460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5847,8 +5871,11 @@
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A423" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="B423" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C423">
         <v>1</v>
@@ -5859,8 +5886,11 @@
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A424" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="B424" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C424">
         <v>1</v>
@@ -5871,8 +5901,11 @@
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A425" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="B425" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C425">
         <v>1</v>
@@ -5883,8 +5916,11 @@
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A426" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B426" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C426">
         <v>1</v>
@@ -5895,8 +5931,11 @@
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A427" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="B427" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C427">
         <v>1</v>
@@ -5907,8 +5946,11 @@
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A428" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="B428" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C428">
         <v>1</v>
@@ -5919,8 +5961,11 @@
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A429" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="B429" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C429">
         <v>1</v>
@@ -5931,8 +5976,11 @@
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A430" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="B430" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C430">
         <v>1</v>
@@ -5943,8 +5991,11 @@
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A431" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="B431" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C431">
         <v>1</v>
@@ -5955,8 +6006,11 @@
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A432" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="B432" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C432">
         <v>1</v>
@@ -5966,9 +6020,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="433" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A433" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="B433" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C433">
         <v>1</v>
@@ -5978,9 +6035,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="434" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A434" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="B434" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C434">
         <v>1</v>
@@ -5990,9 +6050,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="435" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A435" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="B435" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C435">
         <v>1</v>
@@ -6002,9 +6065,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="436" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A436" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="B436" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C436">
         <v>1</v>
@@ -6014,9 +6080,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="437" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A437" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="B437" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C437">
         <v>1</v>
@@ -6026,9 +6095,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="438" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A438" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="B438" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C438">
         <v>1</v>
@@ -6038,9 +6110,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="439" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A439" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="B439" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C439">
         <v>1</v>
@@ -6050,9 +6125,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="440" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A440" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="B440" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C440">
         <v>1</v>
@@ -6062,9 +6140,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="441" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A441" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="B441" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C441">
         <v>1</v>
@@ -6074,9 +6155,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="442" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A442" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B442" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C442">
         <v>1</v>
@@ -6086,9 +6170,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="443" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A443" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="B443" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C443">
         <v>1</v>
@@ -6098,9 +6185,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="444" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A444" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="B444" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C444">
         <v>1</v>
@@ -6110,9 +6200,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="445" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A445" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="B445" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C445">
         <v>1</v>
@@ -6122,9 +6215,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="446" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="B446" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C446">
         <v>1</v>
@@ -6134,9 +6230,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="447" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="B447" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C447">
         <v>1</v>
@@ -6146,9 +6245,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="448" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A448" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="B448" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C448">
         <v>1</v>
@@ -6158,9 +6260,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A449" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="B449" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C449">
         <v>1</v>
@@ -6170,9 +6275,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A450" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="B450" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C450">
         <v>1</v>
@@ -6182,9 +6290,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="B451" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C451">
         <v>1</v>
@@ -6194,9 +6305,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="B452" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C452">
         <v>1</v>
@@ -6206,9 +6320,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A453" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="B453" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C453">
         <v>1</v>
@@ -6218,9 +6335,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A454" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="B454" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C454">
         <v>1</v>
@@ -6230,9 +6350,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A455" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="B455" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C455">
         <v>1</v>
@@ -6242,9 +6365,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A456" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="B456" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C456">
         <v>1</v>
@@ -6254,9 +6380,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A457" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="B457" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C457">
         <v>1</v>
@@ -6266,9 +6395,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A458" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B458" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C458">
         <v>1</v>
@@ -6278,9 +6410,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A459" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="B459" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C459">
         <v>1</v>
@@ -6290,9 +6425,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A460" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="B460" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C460">
         <v>1</v>
@@ -6302,9 +6440,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A461" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="B461" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C461">
         <v>1</v>
@@ -6314,9 +6455,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A462" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="B462" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C462">
         <v>1</v>
@@ -6326,9 +6470,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A463" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="B463" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C463">
         <v>1</v>
@@ -6338,9 +6485,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A464" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="B464" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C464">
         <v>1</v>
@@ -6350,9 +6500,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="465" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A465" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="B465" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C465">
         <v>1</v>
@@ -6362,9 +6515,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="466" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A466" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="B466" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C466">
         <v>1</v>
@@ -6374,9 +6530,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="467" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A467" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="B467" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C467">
         <v>1</v>
@@ -6386,9 +6545,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="468" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A468" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="B468" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C468">
         <v>1</v>
@@ -6398,9 +6560,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="469" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C469">
         <v>1</v>
@@ -6410,9 +6572,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="470" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B470" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C470">
         <v>1</v>
@@ -6422,9 +6584,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="471" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B471" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C471">
         <v>1</v>
@@ -6434,9 +6596,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="472" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C472">
         <v>1</v>
@@ -6446,9 +6608,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="473" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C473">
         <v>1</v>
@@ -6458,9 +6620,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="474" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C474">
         <v>1</v>
@@ -6470,9 +6632,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="475" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C475">
         <v>1</v>
@@ -6482,9 +6644,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="476" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B476" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C476">
         <v>1</v>
@@ -6494,9 +6656,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="477" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B477" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C477">
         <v>1</v>
@@ -6506,9 +6668,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="478" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B478" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C478">
         <v>1</v>
@@ -6518,9 +6680,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="479" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B479" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C479">
         <v>1</v>
@@ -6530,9 +6692,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="480" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C480">
         <v>1</v>
@@ -6544,7 +6706,7 @@
     </row>
     <row r="481" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B481" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C481">
         <v>1</v>
@@ -6556,7 +6718,7 @@
     </row>
     <row r="482" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B482" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C482">
         <v>1</v>
@@ -6568,7 +6730,7 @@
     </row>
     <row r="483" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B483" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C483">
         <v>1</v>
@@ -6580,7 +6742,7 @@
     </row>
     <row r="484" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B484" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C484">
         <v>1</v>
@@ -6592,7 +6754,7 @@
     </row>
     <row r="485" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B485" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C485">
         <v>1</v>
@@ -6604,7 +6766,7 @@
     </row>
     <row r="486" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B486" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C486">
         <v>1</v>
@@ -6616,7 +6778,7 @@
     </row>
     <row r="487" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B487" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C487">
         <v>1</v>
@@ -6628,7 +6790,7 @@
     </row>
     <row r="488" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B488" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C488">
         <v>1</v>
@@ -6640,7 +6802,7 @@
     </row>
     <row r="489" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B489" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C489">
         <v>1</v>
@@ -6652,7 +6814,7 @@
     </row>
     <row r="490" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B490" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C490">
         <v>1</v>
@@ -6664,7 +6826,7 @@
     </row>
     <row r="491" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B491" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C491">
         <v>1</v>
@@ -6676,7 +6838,7 @@
     </row>
     <row r="492" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B492" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C492">
         <v>1</v>
@@ -6688,7 +6850,7 @@
     </row>
     <row r="493" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B493" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C493">
         <v>1</v>
@@ -6700,7 +6862,7 @@
     </row>
     <row r="494" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B494" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C494">
         <v>1</v>
@@ -6712,7 +6874,7 @@
     </row>
     <row r="495" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B495" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C495">
         <v>1</v>
@@ -6724,7 +6886,7 @@
     </row>
     <row r="496" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B496" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C496">
         <v>1</v>
@@ -6736,7 +6898,7 @@
     </row>
     <row r="497" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B497" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C497">
         <v>1</v>
@@ -6748,7 +6910,7 @@
     </row>
     <row r="498" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C498">
         <v>1</v>
@@ -6760,7 +6922,7 @@
     </row>
     <row r="499" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C499">
         <v>1</v>
@@ -6772,7 +6934,7 @@
     </row>
     <row r="500" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B500" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C500">
         <v>1</v>
@@ -6784,7 +6946,7 @@
     </row>
     <row r="501" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B501" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C501">
         <v>1</v>
@@ -6796,7 +6958,7 @@
     </row>
     <row r="502" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B502" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C502">
         <v>1</v>
@@ -6808,7 +6970,7 @@
     </row>
     <row r="503" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B503" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C503">
         <v>1</v>
@@ -6820,7 +6982,7 @@
     </row>
     <row r="504" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C504">
         <v>1</v>
@@ -6832,7 +6994,7 @@
     </row>
     <row r="505" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B505" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C505">
         <v>1</v>
@@ -6844,7 +7006,7 @@
     </row>
     <row r="506" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C506">
         <v>1</v>
@@ -6856,7 +7018,7 @@
     </row>
     <row r="507" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C507">
         <v>1</v>
@@ -6868,7 +7030,7 @@
     </row>
     <row r="508" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B508" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C508">
         <v>1</v>
@@ -6880,7 +7042,7 @@
     </row>
     <row r="509" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B509" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C509">
         <v>1</v>
@@ -6892,7 +7054,7 @@
     </row>
     <row r="510" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B510" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C510">
         <v>1</v>
@@ -6904,7 +7066,7 @@
     </row>
     <row r="511" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B511" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C511">
         <v>1</v>
@@ -6916,7 +7078,7 @@
     </row>
     <row r="512" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B512" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C512">
         <v>1</v>
@@ -6928,7 +7090,7 @@
     </row>
     <row r="513" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B513" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C513">
         <v>1</v>
@@ -6940,7 +7102,7 @@
     </row>
     <row r="514" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B514" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C514">
         <v>1</v>
@@ -6952,7 +7114,7 @@
     </row>
     <row r="515" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B515" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C515">
         <v>1</v>
@@ -6964,7 +7126,7 @@
     </row>
     <row r="516" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B516" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C516">
         <v>1</v>
@@ -6976,7 +7138,7 @@
     </row>
     <row r="517" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B517" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C517">
         <v>1</v>
@@ -6988,7 +7150,7 @@
     </row>
     <row r="518" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B518" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C518">
         <v>1</v>
@@ -7000,7 +7162,7 @@
     </row>
     <row r="519" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B519" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C519">
         <v>1</v>
@@ -7012,7 +7174,7 @@
     </row>
     <row r="520" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B520" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C520">
         <v>1</v>
@@ -7024,7 +7186,7 @@
     </row>
     <row r="521" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B521" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C521">
         <v>1</v>
@@ -7036,7 +7198,7 @@
     </row>
     <row r="522" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B522" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C522">
         <v>1</v>
@@ -7048,7 +7210,7 @@
     </row>
     <row r="523" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B523" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C523">
         <v>1</v>
@@ -7060,7 +7222,7 @@
     </row>
     <row r="524" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B524" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C524">
         <v>1</v>
@@ -7072,7 +7234,7 @@
     </row>
     <row r="525" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B525" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C525">
         <v>1</v>
@@ -7084,7 +7246,7 @@
     </row>
     <row r="526" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B526" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C526">
         <v>1</v>
@@ -7096,7 +7258,7 @@
     </row>
     <row r="527" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B527" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C527">
         <v>1</v>
@@ -7108,7 +7270,7 @@
     </row>
     <row r="528" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B528" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C528">
         <v>1</v>
@@ -7120,7 +7282,7 @@
     </row>
     <row r="529" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B529" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C529">
         <v>1</v>
@@ -7132,7 +7294,7 @@
     </row>
     <row r="530" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B530" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C530">
         <v>1</v>
@@ -7144,7 +7306,7 @@
     </row>
     <row r="531" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B531" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C531">
         <v>1</v>
@@ -7156,7 +7318,7 @@
     </row>
     <row r="532" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B532" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C532">
         <v>1</v>
@@ -7168,7 +7330,7 @@
     </row>
     <row r="533" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B533" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C533">
         <v>1</v>
@@ -7180,7 +7342,7 @@
     </row>
     <row r="534" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B534" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C534">
         <v>1</v>
@@ -7192,7 +7354,7 @@
     </row>
     <row r="535" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B535" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C535">
         <v>1</v>
@@ -7204,7 +7366,7 @@
     </row>
     <row r="536" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B536" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C536">
         <v>1</v>
@@ -7216,7 +7378,7 @@
     </row>
     <row r="537" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B537" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C537">
         <v>1</v>
@@ -7228,7 +7390,7 @@
     </row>
     <row r="538" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B538" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C538">
         <v>1</v>
@@ -7240,7 +7402,7 @@
     </row>
     <row r="539" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B539" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C539">
         <v>1</v>
@@ -7252,7 +7414,7 @@
     </row>
     <row r="540" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B540" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C540">
         <v>1</v>
@@ -7264,7 +7426,7 @@
     </row>
     <row r="541" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B541" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C541">
         <v>1</v>
@@ -7276,7 +7438,7 @@
     </row>
     <row r="542" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B542" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C542">
         <v>1</v>
@@ -7288,7 +7450,7 @@
     </row>
     <row r="543" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B543" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C543">
         <v>1</v>
@@ -7300,7 +7462,7 @@
     </row>
     <row r="544" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B544" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C544">
         <v>1</v>
@@ -7312,7 +7474,7 @@
     </row>
     <row r="545" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B545" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C545">
         <v>1</v>
@@ -7324,7 +7486,7 @@
     </row>
     <row r="546" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B546" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C546">
         <v>1</v>
@@ -7336,7 +7498,7 @@
     </row>
     <row r="547" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B547" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C547">
         <v>1</v>
@@ -7348,7 +7510,7 @@
     </row>
     <row r="548" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B548" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C548">
         <v>1</v>
@@ -7360,7 +7522,7 @@
     </row>
     <row r="549" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B549" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C549">
         <v>1</v>
@@ -7372,7 +7534,7 @@
     </row>
     <row r="550" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B550" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C550">
         <v>1</v>
@@ -7384,7 +7546,7 @@
     </row>
     <row r="551" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B551" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C551">
         <v>1</v>
@@ -7396,7 +7558,7 @@
     </row>
     <row r="552" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B552" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C552">
         <v>1</v>
@@ -7408,7 +7570,7 @@
     </row>
     <row r="553" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B553" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C553">
         <v>1</v>
@@ -7420,7 +7582,7 @@
     </row>
     <row r="554" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B554" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C554">
         <v>1</v>
@@ -7432,7 +7594,7 @@
     </row>
     <row r="555" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B555" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C555">
         <v>1</v>
@@ -7444,7 +7606,7 @@
     </row>
     <row r="556" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B556" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C556">
         <v>1</v>
@@ -7456,7 +7618,7 @@
     </row>
     <row r="557" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B557" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C557">
         <v>1</v>
@@ -7468,7 +7630,7 @@
     </row>
     <row r="558" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B558" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C558">
         <v>1</v>
@@ -7480,7 +7642,7 @@
     </row>
     <row r="559" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B559" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C559">
         <v>1</v>
@@ -7492,7 +7654,7 @@
     </row>
     <row r="560" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B560" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C560">
         <v>1</v>
@@ -7504,7 +7666,7 @@
     </row>
     <row r="561" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B561" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C561">
         <v>1</v>
@@ -7516,7 +7678,7 @@
     </row>
     <row r="562" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B562" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C562">
         <v>1</v>
@@ -7528,7 +7690,7 @@
     </row>
     <row r="563" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B563" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C563">
         <v>1</v>
@@ -7540,7 +7702,7 @@
     </row>
     <row r="564" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B564" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C564">
         <v>1</v>
@@ -7552,7 +7714,7 @@
     </row>
     <row r="565" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B565" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C565">
         <v>1</v>
@@ -7564,7 +7726,7 @@
     </row>
     <row r="566" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B566" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C566">
         <v>1</v>
@@ -7576,7 +7738,7 @@
     </row>
     <row r="567" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B567" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C567">
         <v>1</v>
@@ -7588,7 +7750,7 @@
     </row>
     <row r="568" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B568" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C568">
         <v>1</v>
@@ -7600,7 +7762,7 @@
     </row>
     <row r="569" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B569" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C569">
         <v>1</v>
@@ -7612,7 +7774,7 @@
     </row>
     <row r="570" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B570" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C570">
         <v>1</v>
@@ -7624,7 +7786,7 @@
     </row>
     <row r="571" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B571" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C571">
         <v>1</v>
@@ -7636,7 +7798,7 @@
     </row>
     <row r="572" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B572" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C572">
         <v>1</v>
@@ -7648,7 +7810,7 @@
     </row>
     <row r="573" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B573" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C573">
         <v>1</v>
@@ -7660,7 +7822,7 @@
     </row>
     <row r="574" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B574" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C574">
         <v>1</v>
@@ -7672,7 +7834,7 @@
     </row>
     <row r="575" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B575" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C575">
         <v>1</v>
@@ -7684,7 +7846,7 @@
     </row>
     <row r="576" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B576" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C576">
         <v>1</v>
@@ -7696,7 +7858,7 @@
     </row>
     <row r="577" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B577" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C577">
         <v>1</v>
@@ -7708,7 +7870,7 @@
     </row>
     <row r="578" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B578" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C578">
         <v>1</v>
@@ -7720,7 +7882,7 @@
     </row>
     <row r="579" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B579" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C579">
         <v>1</v>
@@ -7732,7 +7894,7 @@
     </row>
     <row r="580" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B580" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C580">
         <v>1</v>
@@ -7744,7 +7906,7 @@
     </row>
     <row r="581" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B581" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C581">
         <v>1</v>
@@ -7756,7 +7918,7 @@
     </row>
     <row r="582" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B582" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C582">
         <v>1</v>
@@ -7768,7 +7930,7 @@
     </row>
     <row r="583" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B583" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C583">
         <v>1</v>
@@ -7780,7 +7942,7 @@
     </row>
     <row r="584" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B584" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C584">
         <v>1</v>
@@ -7792,7 +7954,7 @@
     </row>
     <row r="585" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B585" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C585">
         <v>1</v>
@@ -7804,7 +7966,7 @@
     </row>
     <row r="586" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B586" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C586">
         <v>1</v>
@@ -7816,7 +7978,7 @@
     </row>
     <row r="587" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B587" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C587">
         <v>1</v>
@@ -7828,7 +7990,7 @@
     </row>
     <row r="588" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B588" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C588">
         <v>1</v>
@@ -7840,7 +8002,7 @@
     </row>
     <row r="589" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B589" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C589">
         <v>1</v>
@@ -7852,7 +8014,7 @@
     </row>
     <row r="590" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B590" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C590">
         <v>1</v>
@@ -7864,7 +8026,7 @@
     </row>
     <row r="591" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B591" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C591">
         <v>1</v>
@@ -7876,7 +8038,7 @@
     </row>
     <row r="592" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B592" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C592">
         <v>1</v>
@@ -7888,7 +8050,7 @@
     </row>
     <row r="593" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B593" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C593">
         <v>1</v>
@@ -7900,7 +8062,7 @@
     </row>
     <row r="594" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B594" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C594">
         <v>1</v>
@@ -7912,7 +8074,7 @@
     </row>
     <row r="595" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B595" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C595">
         <v>1</v>
@@ -7924,7 +8086,7 @@
     </row>
     <row r="596" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B596" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C596">
         <v>1</v>
@@ -7936,7 +8098,7 @@
     </row>
     <row r="597" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B597" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C597">
         <v>1</v>
@@ -7948,7 +8110,7 @@
     </row>
     <row r="598" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B598" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C598">
         <v>1</v>
@@ -7960,7 +8122,7 @@
     </row>
     <row r="599" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B599" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C599">
         <v>1</v>
@@ -7972,7 +8134,7 @@
     </row>
     <row r="600" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B600" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C600">
         <v>1</v>
@@ -7984,7 +8146,7 @@
     </row>
     <row r="601" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B601" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C601">
         <v>1</v>
@@ -7996,7 +8158,7 @@
     </row>
     <row r="602" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B602" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C602">
         <v>1</v>
@@ -8008,7 +8170,7 @@
     </row>
     <row r="603" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B603" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C603">
         <v>1</v>
@@ -8020,7 +8182,7 @@
     </row>
     <row r="604" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B604" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C604">
         <v>1</v>
@@ -8032,7 +8194,7 @@
     </row>
     <row r="605" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B605" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C605">
         <v>1</v>
@@ -8044,7 +8206,7 @@
     </row>
     <row r="606" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B606" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C606">
         <v>1</v>
@@ -8056,7 +8218,7 @@
     </row>
     <row r="607" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B607" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C607">
         <v>1</v>
@@ -8068,7 +8230,7 @@
     </row>
     <row r="608" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B608" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C608">
         <v>1</v>
@@ -8080,7 +8242,7 @@
     </row>
     <row r="609" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B609" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C609">
         <v>1</v>
@@ -8092,7 +8254,7 @@
     </row>
     <row r="610" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B610" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C610">
         <v>1</v>
@@ -8104,7 +8266,7 @@
     </row>
     <row r="611" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B611" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C611">
         <v>1</v>
@@ -8116,7 +8278,7 @@
     </row>
     <row r="612" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B612" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C612">
         <v>1</v>
@@ -8128,7 +8290,7 @@
     </row>
     <row r="613" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B613" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C613">
         <v>1</v>
@@ -8140,7 +8302,7 @@
     </row>
     <row r="614" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B614" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C614">
         <v>1</v>
@@ -8152,7 +8314,7 @@
     </row>
     <row r="615" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B615" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C615">
         <v>1</v>
@@ -8164,7 +8326,7 @@
     </row>
     <row r="616" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B616" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C616">
         <v>1</v>
@@ -8176,7 +8338,7 @@
     </row>
     <row r="617" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B617" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C617">
         <v>1</v>
@@ -8188,7 +8350,7 @@
     </row>
     <row r="618" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B618" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C618">
         <v>1</v>
@@ -8200,7 +8362,7 @@
     </row>
     <row r="619" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B619" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C619">
         <v>1</v>
@@ -8212,7 +8374,7 @@
     </row>
     <row r="620" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B620" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C620">
         <v>1</v>
@@ -8224,7 +8386,7 @@
     </row>
     <row r="621" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B621" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C621">
         <v>1</v>
@@ -8236,7 +8398,7 @@
     </row>
     <row r="622" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B622" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C622">
         <v>1</v>
@@ -8248,7 +8410,7 @@
     </row>
     <row r="623" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B623" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C623">
         <v>1</v>
@@ -8260,7 +8422,7 @@
     </row>
     <row r="624" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B624" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C624">
         <v>1</v>
@@ -8272,7 +8434,7 @@
     </row>
     <row r="625" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B625" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C625">
         <v>1</v>
@@ -8284,7 +8446,7 @@
     </row>
     <row r="626" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B626" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C626">
         <v>1</v>
@@ -8296,7 +8458,7 @@
     </row>
     <row r="627" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B627" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C627">
         <v>1</v>
@@ -8308,7 +8470,7 @@
     </row>
     <row r="628" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B628" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C628">
         <v>1</v>
@@ -8320,7 +8482,7 @@
     </row>
     <row r="629" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B629" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C629">
         <v>1</v>
@@ -8332,7 +8494,7 @@
     </row>
     <row r="630" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B630" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C630">
         <v>1</v>
@@ -8344,7 +8506,7 @@
     </row>
     <row r="631" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B631" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C631">
         <v>1</v>
@@ -8356,7 +8518,7 @@
     </row>
     <row r="632" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B632" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C632">
         <v>1</v>
@@ -8368,7 +8530,7 @@
     </row>
     <row r="633" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B633" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C633">
         <v>1</v>
@@ -8380,7 +8542,7 @@
     </row>
     <row r="634" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B634" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C634">
         <v>1</v>
@@ -8392,7 +8554,7 @@
     </row>
     <row r="635" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B635" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C635">
         <v>1</v>
@@ -8404,7 +8566,7 @@
     </row>
     <row r="636" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B636" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C636">
         <v>1</v>
@@ -8416,7 +8578,7 @@
     </row>
     <row r="637" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B637" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C637">
         <v>1</v>
@@ -8428,7 +8590,7 @@
     </row>
     <row r="638" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B638" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C638">
         <v>1</v>
@@ -8440,7 +8602,7 @@
     </row>
     <row r="639" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B639" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C639">
         <v>1</v>
@@ -8452,7 +8614,7 @@
     </row>
     <row r="640" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B640" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C640">
         <v>1</v>
@@ -8464,7 +8626,7 @@
     </row>
     <row r="641" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B641" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C641">
         <v>1</v>
@@ -8476,7 +8638,7 @@
     </row>
     <row r="642" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B642" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C642">
         <v>1</v>
@@ -8488,7 +8650,7 @@
     </row>
     <row r="643" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B643" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C643">
         <v>1</v>
@@ -8500,7 +8662,7 @@
     </row>
     <row r="644" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B644" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C644">
         <v>1</v>
@@ -8512,7 +8674,7 @@
     </row>
     <row r="645" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B645" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C645">
         <v>1</v>
@@ -8524,7 +8686,7 @@
     </row>
     <row r="646" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B646" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C646">
         <v>1</v>
@@ -8536,7 +8698,7 @@
     </row>
     <row r="647" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B647" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C647">
         <v>1</v>
@@ -8548,7 +8710,7 @@
     </row>
     <row r="648" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B648" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C648">
         <v>1</v>
@@ -8560,7 +8722,7 @@
     </row>
     <row r="649" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B649" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C649">
         <v>1</v>
@@ -8572,7 +8734,7 @@
     </row>
     <row r="650" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B650" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C650">
         <v>1</v>
@@ -8584,7 +8746,7 @@
     </row>
     <row r="651" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B651" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C651">
         <v>1</v>
@@ -8596,7 +8758,7 @@
     </row>
     <row r="652" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B652" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C652">
         <v>1</v>
@@ -8608,7 +8770,7 @@
     </row>
     <row r="653" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B653" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C653">
         <v>1</v>
@@ -8620,7 +8782,7 @@
     </row>
     <row r="654" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B654" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C654">
         <v>1</v>
@@ -8632,7 +8794,7 @@
     </row>
     <row r="655" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B655" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C655">
         <v>1</v>
@@ -8644,7 +8806,7 @@
     </row>
     <row r="656" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B656" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C656">
         <v>1</v>
@@ -8656,7 +8818,7 @@
     </row>
     <row r="657" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B657" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C657">
         <v>1</v>
@@ -8668,7 +8830,7 @@
     </row>
     <row r="658" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B658" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C658">
         <v>1</v>
@@ -8680,7 +8842,7 @@
     </row>
     <row r="659" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B659" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C659">
         <v>1</v>
@@ -8692,7 +8854,7 @@
     </row>
     <row r="660" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B660" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C660">
         <v>1</v>
@@ -8704,7 +8866,7 @@
     </row>
     <row r="661" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B661" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C661">
         <v>1</v>
@@ -8716,7 +8878,7 @@
     </row>
     <row r="662" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B662" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C662">
         <v>1</v>
@@ -8728,7 +8890,7 @@
     </row>
     <row r="663" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B663" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C663">
         <v>1</v>
@@ -8740,7 +8902,7 @@
     </row>
     <row r="664" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B664" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C664">
         <v>1</v>
@@ -8752,7 +8914,7 @@
     </row>
     <row r="665" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B665" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C665">
         <v>1</v>
@@ -8764,7 +8926,7 @@
     </row>
     <row r="666" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B666" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C666">
         <v>1</v>
@@ -8776,7 +8938,7 @@
     </row>
     <row r="667" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B667" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C667">
         <v>1</v>
@@ -8788,7 +8950,7 @@
     </row>
     <row r="668" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B668" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C668">
         <v>1</v>
@@ -8800,7 +8962,7 @@
     </row>
     <row r="669" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B669" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C669">
         <v>1</v>
@@ -8812,7 +8974,7 @@
     </row>
     <row r="670" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B670" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C670">
         <v>1</v>
@@ -8824,7 +8986,7 @@
     </row>
     <row r="671" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B671" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C671">
         <v>1</v>
@@ -8836,7 +8998,7 @@
     </row>
     <row r="672" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B672" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C672">
         <v>1</v>
@@ -8848,7 +9010,7 @@
     </row>
     <row r="673" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B673" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C673">
         <v>1</v>
@@ -8860,7 +9022,7 @@
     </row>
     <row r="674" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B674" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C674">
         <v>1</v>
@@ -8872,7 +9034,7 @@
     </row>
     <row r="675" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B675" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C675">
         <v>1</v>
@@ -8884,7 +9046,7 @@
     </row>
     <row r="676" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B676" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C676">
         <v>1</v>
@@ -8896,7 +9058,7 @@
     </row>
     <row r="677" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B677" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C677">
         <v>1</v>
@@ -8908,7 +9070,7 @@
     </row>
     <row r="678" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B678" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C678">
         <v>1</v>
@@ -8920,7 +9082,7 @@
     </row>
     <row r="679" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B679" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C679">
         <v>1</v>
@@ -8932,7 +9094,7 @@
     </row>
     <row r="680" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B680" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C680">
         <v>1</v>
@@ -8944,7 +9106,7 @@
     </row>
     <row r="681" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B681" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C681">
         <v>1</v>
@@ -8956,7 +9118,7 @@
     </row>
     <row r="682" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B682" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C682">
         <v>1</v>
@@ -8968,7 +9130,7 @@
     </row>
     <row r="683" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B683" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C683">
         <v>1</v>
@@ -8980,7 +9142,7 @@
     </row>
     <row r="684" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B684" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C684">
         <v>1</v>
@@ -8992,7 +9154,7 @@
     </row>
     <row r="685" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B685" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C685">
         <v>1</v>
@@ -9004,7 +9166,7 @@
     </row>
     <row r="686" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B686" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C686">
         <v>1</v>
@@ -9016,7 +9178,7 @@
     </row>
     <row r="687" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B687" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C687">
         <v>1</v>
@@ -9028,7 +9190,7 @@
     </row>
     <row r="688" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B688" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C688">
         <v>1</v>
@@ -9040,7 +9202,7 @@
     </row>
     <row r="689" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B689" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C689">
         <v>1</v>
@@ -9052,7 +9214,7 @@
     </row>
     <row r="690" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B690" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C690">
         <v>1</v>
@@ -9064,7 +9226,7 @@
     </row>
     <row r="691" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B691" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C691">
         <v>1</v>
@@ -9076,7 +9238,7 @@
     </row>
     <row r="692" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B692" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C692">
         <v>1</v>
@@ -9088,7 +9250,7 @@
     </row>
     <row r="693" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B693" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C693">
         <v>1</v>
@@ -9100,7 +9262,7 @@
     </row>
     <row r="694" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B694" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C694">
         <v>1</v>
@@ -9112,7 +9274,7 @@
     </row>
     <row r="695" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B695" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C695">
         <v>1</v>
@@ -9124,7 +9286,7 @@
     </row>
     <row r="696" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B696" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C696">
         <v>1</v>
@@ -9136,7 +9298,7 @@
     </row>
     <row r="697" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B697" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C697">
         <v>1</v>
@@ -9148,7 +9310,7 @@
     </row>
     <row r="698" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B698" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C698">
         <v>1</v>
@@ -9160,7 +9322,7 @@
     </row>
     <row r="699" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B699" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C699">
         <v>1</v>
@@ -9172,7 +9334,7 @@
     </row>
     <row r="700" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B700" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C700">
         <v>1</v>
@@ -9184,7 +9346,7 @@
     </row>
     <row r="701" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B701" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C701">
         <v>1</v>
@@ -9196,7 +9358,7 @@
     </row>
     <row r="702" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B702" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C702">
         <v>1</v>
@@ -9208,7 +9370,7 @@
     </row>
     <row r="703" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B703" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C703">
         <v>1</v>
@@ -9220,7 +9382,7 @@
     </row>
     <row r="704" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B704" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C704">
         <v>1</v>
@@ -9232,7 +9394,7 @@
     </row>
     <row r="705" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B705" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C705">
         <v>1</v>
@@ -9244,7 +9406,7 @@
     </row>
     <row r="706" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B706" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C706">
         <v>1</v>
@@ -9256,7 +9418,7 @@
     </row>
     <row r="707" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B707" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C707">
         <v>1</v>
@@ -9268,7 +9430,7 @@
     </row>
     <row r="708" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B708" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C708">
         <v>1</v>
@@ -9280,7 +9442,7 @@
     </row>
     <row r="709" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B709" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C709">
         <v>1</v>
@@ -9292,7 +9454,7 @@
     </row>
     <row r="710" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B710" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C710">
         <v>1</v>
@@ -9304,7 +9466,7 @@
     </row>
     <row r="711" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B711" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C711">
         <v>1</v>
@@ -9316,7 +9478,7 @@
     </row>
     <row r="712" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B712" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C712">
         <v>1</v>
@@ -9328,7 +9490,7 @@
     </row>
     <row r="713" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B713" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C713">
         <v>1</v>
@@ -9340,7 +9502,7 @@
     </row>
     <row r="714" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B714" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C714">
         <v>1</v>
@@ -9352,7 +9514,7 @@
     </row>
     <row r="715" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B715" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C715">
         <v>1</v>
@@ -9364,7 +9526,7 @@
     </row>
     <row r="716" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B716" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C716">
         <v>1</v>
@@ -9376,7 +9538,7 @@
     </row>
     <row r="717" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B717" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C717">
         <v>1</v>
@@ -9388,7 +9550,7 @@
     </row>
     <row r="718" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B718" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C718">
         <v>1</v>
@@ -9400,7 +9562,7 @@
     </row>
     <row r="719" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B719" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C719">
         <v>1</v>
@@ -9412,7 +9574,7 @@
     </row>
     <row r="720" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B720" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C720">
         <v>1</v>
@@ -9424,7 +9586,7 @@
     </row>
     <row r="721" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B721" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C721">
         <v>1</v>
@@ -9436,7 +9598,7 @@
     </row>
     <row r="722" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B722" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C722">
         <v>1</v>
@@ -9448,7 +9610,7 @@
     </row>
     <row r="723" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B723" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C723">
         <v>1</v>
@@ -9460,7 +9622,7 @@
     </row>
     <row r="724" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B724" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C724">
         <v>1</v>
@@ -9472,7 +9634,7 @@
     </row>
     <row r="725" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B725" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C725">
         <v>1</v>
@@ -9484,7 +9646,7 @@
     </row>
     <row r="726" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B726" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C726">
         <v>1</v>
@@ -9496,7 +9658,7 @@
     </row>
     <row r="727" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B727" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C727">
         <v>1</v>
@@ -9508,7 +9670,7 @@
     </row>
     <row r="728" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B728" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C728">
         <v>1</v>
@@ -9520,7 +9682,7 @@
     </row>
     <row r="729" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B729" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C729">
         <v>1</v>
@@ -9532,7 +9694,7 @@
     </row>
     <row r="730" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B730" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C730">
         <v>1</v>
@@ -9544,7 +9706,7 @@
     </row>
     <row r="731" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B731" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C731">
         <v>1</v>
@@ -9556,7 +9718,7 @@
     </row>
     <row r="732" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B732" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C732">
         <v>1</v>
@@ -9568,7 +9730,7 @@
     </row>
     <row r="733" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B733" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C733">
         <v>1</v>
@@ -9580,7 +9742,7 @@
     </row>
     <row r="734" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B734" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C734">
         <v>1</v>
@@ -9592,7 +9754,7 @@
     </row>
     <row r="735" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B735" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C735">
         <v>1</v>
@@ -9604,7 +9766,7 @@
     </row>
     <row r="736" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B736" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C736">
         <v>1</v>
@@ -9616,7 +9778,7 @@
     </row>
     <row r="737" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B737" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C737">
         <v>1</v>
@@ -9628,7 +9790,7 @@
     </row>
     <row r="738" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B738" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C738">
         <v>1</v>
@@ -9640,7 +9802,7 @@
     </row>
     <row r="739" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B739" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C739">
         <v>1</v>
@@ -9652,7 +9814,7 @@
     </row>
     <row r="740" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B740" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C740">
         <v>1</v>
@@ -9664,7 +9826,7 @@
     </row>
     <row r="741" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B741" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C741">
         <v>1</v>
@@ -9676,7 +9838,7 @@
     </row>
     <row r="742" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B742" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C742">
         <v>1</v>
@@ -9688,7 +9850,7 @@
     </row>
     <row r="743" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B743" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C743">
         <v>1</v>
@@ -9700,7 +9862,7 @@
     </row>
     <row r="744" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B744" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C744">
         <v>1</v>
@@ -9712,7 +9874,7 @@
     </row>
     <row r="745" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B745" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C745">
         <v>1</v>
@@ -9724,7 +9886,7 @@
     </row>
     <row r="746" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B746" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C746">
         <v>1</v>
@@ -9736,7 +9898,7 @@
     </row>
     <row r="747" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B747" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C747">
         <v>1</v>
@@ -9748,7 +9910,7 @@
     </row>
     <row r="748" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B748" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C748">
         <v>1</v>
@@ -9760,7 +9922,7 @@
     </row>
     <row r="749" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B749" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C749">
         <v>1</v>
@@ -9772,7 +9934,7 @@
     </row>
     <row r="750" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B750" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C750">
         <v>1</v>
@@ -9784,7 +9946,7 @@
     </row>
     <row r="751" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B751" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C751">
         <v>1</v>
@@ -9796,7 +9958,7 @@
     </row>
     <row r="752" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B752" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C752">
         <v>1</v>
@@ -9808,7 +9970,7 @@
     </row>
     <row r="753" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B753" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C753">
         <v>1</v>
@@ -9820,7 +9982,7 @@
     </row>
     <row r="754" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B754" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C754">
         <v>1</v>
@@ -9832,7 +9994,7 @@
     </row>
     <row r="755" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B755" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C755">
         <v>1</v>
@@ -9844,7 +10006,7 @@
     </row>
     <row r="756" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B756" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C756">
         <v>1</v>
@@ -9856,7 +10018,7 @@
     </row>
     <row r="757" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B757" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C757">
         <v>1</v>
@@ -9868,7 +10030,7 @@
     </row>
     <row r="758" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B758" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C758">
         <v>1</v>
@@ -9880,7 +10042,7 @@
     </row>
     <row r="759" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B759" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C759">
         <v>1</v>
@@ -9892,7 +10054,7 @@
     </row>
     <row r="760" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B760" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C760">
         <v>1</v>
@@ -9904,7 +10066,7 @@
     </row>
     <row r="761" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B761" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C761">
         <v>1</v>
@@ -9916,7 +10078,7 @@
     </row>
     <row r="762" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B762" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C762">
         <v>1</v>
@@ -9928,7 +10090,7 @@
     </row>
     <row r="763" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B763" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C763">
         <v>1</v>
@@ -9940,7 +10102,7 @@
     </row>
     <row r="764" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B764" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C764">
         <v>1</v>
@@ -9952,7 +10114,7 @@
     </row>
     <row r="765" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B765" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C765">
         <v>1</v>
@@ -9964,7 +10126,7 @@
     </row>
     <row r="766" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B766" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C766">
         <v>1</v>
@@ -9976,7 +10138,7 @@
     </row>
     <row r="767" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B767" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C767">
         <v>1</v>
@@ -9988,7 +10150,7 @@
     </row>
     <row r="768" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B768" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C768">
         <v>1</v>
@@ -10000,7 +10162,7 @@
     </row>
     <row r="769" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B769" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C769">
         <v>1</v>
@@ -10012,7 +10174,7 @@
     </row>
     <row r="770" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B770" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C770">
         <v>1</v>
@@ -10024,7 +10186,7 @@
     </row>
     <row r="771" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B771" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C771">
         <v>1</v>
@@ -10036,7 +10198,7 @@
     </row>
     <row r="772" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B772" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C772">
         <v>1</v>
@@ -10048,7 +10210,7 @@
     </row>
     <row r="773" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B773" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C773">
         <v>1</v>
@@ -10060,7 +10222,7 @@
     </row>
     <row r="774" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B774" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C774">
         <v>1</v>
@@ -10072,7 +10234,7 @@
     </row>
     <row r="775" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B775" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C775">
         <v>1</v>
@@ -10084,7 +10246,7 @@
     </row>
     <row r="776" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B776" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C776">
         <v>1</v>
@@ -10096,7 +10258,7 @@
     </row>
     <row r="777" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B777" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C777">
         <v>1</v>
@@ -10108,7 +10270,7 @@
     </row>
     <row r="778" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B778" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C778">
         <v>1</v>
@@ -10120,7 +10282,7 @@
     </row>
     <row r="779" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B779" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C779">
         <v>1</v>
@@ -10132,7 +10294,7 @@
     </row>
     <row r="780" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B780" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C780">
         <v>1</v>
@@ -10144,7 +10306,7 @@
     </row>
     <row r="781" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B781" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C781">
         <v>1</v>
@@ -10156,7 +10318,7 @@
     </row>
     <row r="782" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B782" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C782">
         <v>1</v>
@@ -10168,7 +10330,7 @@
     </row>
     <row r="783" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B783" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C783">
         <v>1</v>
@@ -10180,7 +10342,7 @@
     </row>
     <row r="784" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B784" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C784">
         <v>1</v>
@@ -10192,7 +10354,7 @@
     </row>
     <row r="785" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B785" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C785">
         <v>1</v>
@@ -10204,7 +10366,7 @@
     </row>
     <row r="786" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B786" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C786">
         <v>1</v>
@@ -10216,7 +10378,7 @@
     </row>
     <row r="787" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B787" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C787">
         <v>1</v>
@@ -10228,7 +10390,7 @@
     </row>
     <row r="788" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B788" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C788">
         <v>1</v>
@@ -10240,7 +10402,7 @@
     </row>
     <row r="789" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B789" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C789">
         <v>1</v>
@@ -10252,7 +10414,7 @@
     </row>
     <row r="790" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B790" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C790">
         <v>1</v>
@@ -10264,7 +10426,7 @@
     </row>
     <row r="791" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B791" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C791">
         <v>1</v>
@@ -10276,7 +10438,7 @@
     </row>
     <row r="792" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B792" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C792">
         <v>1</v>
@@ -10288,7 +10450,7 @@
     </row>
     <row r="793" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B793" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C793">
         <v>1</v>
@@ -10300,7 +10462,7 @@
     </row>
     <row r="794" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B794" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C794">
         <v>1</v>
@@ -10312,7 +10474,7 @@
     </row>
     <row r="795" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B795" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C795">
         <v>1</v>
@@ -10324,7 +10486,7 @@
     </row>
     <row r="796" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B796" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C796">
         <v>1</v>
@@ -10336,7 +10498,7 @@
     </row>
     <row r="797" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B797" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C797">
         <v>1</v>
@@ -10348,7 +10510,7 @@
     </row>
     <row r="798" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B798" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C798">
         <v>1</v>
@@ -10360,7 +10522,7 @@
     </row>
     <row r="799" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B799" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C799">
         <v>1</v>
@@ -10372,7 +10534,7 @@
     </row>
     <row r="800" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B800" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C800">
         <v>1</v>
@@ -10384,7 +10546,7 @@
     </row>
     <row r="801" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B801" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C801">
         <v>1</v>
@@ -10396,7 +10558,7 @@
     </row>
     <row r="802" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B802" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C802">
         <v>1</v>
@@ -10408,7 +10570,7 @@
     </row>
     <row r="803" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B803" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C803">
         <v>1</v>
@@ -10420,7 +10582,7 @@
     </row>
     <row r="804" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B804" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C804">
         <v>1</v>
@@ -10432,7 +10594,7 @@
     </row>
     <row r="805" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B805" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C805">
         <v>1</v>
@@ -10444,7 +10606,7 @@
     </row>
     <row r="806" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B806" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C806">
         <v>1</v>
@@ -10456,7 +10618,7 @@
     </row>
     <row r="807" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B807" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C807">
         <v>1</v>
@@ -10468,7 +10630,7 @@
     </row>
     <row r="808" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B808" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C808">
         <v>1</v>
@@ -10480,7 +10642,7 @@
     </row>
     <row r="809" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B809" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C809">
         <v>1</v>
@@ -10492,7 +10654,7 @@
     </row>
     <row r="810" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B810" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C810">
         <v>1</v>
@@ -10504,7 +10666,7 @@
     </row>
     <row r="811" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B811" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C811">
         <v>1</v>
@@ -10516,7 +10678,7 @@
     </row>
     <row r="812" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B812" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C812">
         <v>1</v>
@@ -10528,7 +10690,7 @@
     </row>
     <row r="813" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B813" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C813">
         <v>1</v>
@@ -10540,7 +10702,7 @@
     </row>
     <row r="814" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B814" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C814">
         <v>1</v>
@@ -10552,7 +10714,7 @@
     </row>
     <row r="815" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B815" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C815">
         <v>1</v>
@@ -10564,7 +10726,7 @@
     </row>
     <row r="816" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B816" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C816">
         <v>1</v>
@@ -10576,7 +10738,7 @@
     </row>
     <row r="817" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B817" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C817">
         <v>1</v>
@@ -10588,7 +10750,7 @@
     </row>
     <row r="818" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B818" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C818">
         <v>1</v>
@@ -10600,7 +10762,7 @@
     </row>
     <row r="819" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B819" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C819">
         <v>1</v>
@@ -10612,7 +10774,7 @@
     </row>
     <row r="820" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B820" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C820">
         <v>1</v>
@@ -10624,7 +10786,7 @@
     </row>
     <row r="821" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B821" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C821">
         <v>1</v>
@@ -10636,7 +10798,7 @@
     </row>
     <row r="822" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B822" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C822">
         <v>1</v>
@@ -10648,7 +10810,7 @@
     </row>
     <row r="823" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B823" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C823">
         <v>1</v>
@@ -10660,7 +10822,7 @@
     </row>
     <row r="824" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B824" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C824">
         <v>1</v>
@@ -10672,7 +10834,7 @@
     </row>
     <row r="825" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B825" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C825">
         <v>1</v>
@@ -10684,7 +10846,7 @@
     </row>
     <row r="826" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B826" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C826">
         <v>1</v>
@@ -10696,7 +10858,7 @@
     </row>
     <row r="827" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B827" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C827">
         <v>1</v>
@@ -10708,7 +10870,7 @@
     </row>
     <row r="828" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B828" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C828">
         <v>1</v>
@@ -10720,7 +10882,7 @@
     </row>
     <row r="829" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B829" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C829">
         <v>1</v>
@@ -10732,7 +10894,7 @@
     </row>
     <row r="830" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B830" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C830">
         <v>1</v>
@@ -10744,7 +10906,7 @@
     </row>
     <row r="831" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B831" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C831">
         <v>1</v>
@@ -10756,7 +10918,7 @@
     </row>
     <row r="832" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B832" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C832">
         <v>1</v>
@@ -10768,7 +10930,7 @@
     </row>
     <row r="833" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B833" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C833">
         <v>1</v>
@@ -10780,7 +10942,7 @@
     </row>
     <row r="834" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B834" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C834">
         <v>1</v>
@@ -10792,7 +10954,7 @@
     </row>
     <row r="835" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B835" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C835">
         <v>1</v>
@@ -10804,7 +10966,7 @@
     </row>
     <row r="836" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B836" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C836">
         <v>1</v>
@@ -10816,7 +10978,7 @@
     </row>
     <row r="837" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B837" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C837">
         <v>1</v>
@@ -10828,7 +10990,7 @@
     </row>
     <row r="838" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B838" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C838">
         <v>1</v>
@@ -10840,7 +11002,7 @@
     </row>
     <row r="839" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B839" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C839">
         <v>1</v>
@@ -10852,7 +11014,7 @@
     </row>
     <row r="840" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B840" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C840">
         <v>1</v>
@@ -10864,7 +11026,7 @@
     </row>
     <row r="841" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B841" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C841">
         <v>1</v>
@@ -10876,7 +11038,7 @@
     </row>
     <row r="842" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B842" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C842">
         <v>1</v>
@@ -10888,7 +11050,7 @@
     </row>
     <row r="843" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B843" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C843">
         <v>1</v>
@@ -10900,7 +11062,7 @@
     </row>
     <row r="844" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B844" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C844">
         <v>1</v>
@@ -10912,7 +11074,7 @@
     </row>
     <row r="845" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B845" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C845">
         <v>1</v>
@@ -10924,7 +11086,7 @@
     </row>
     <row r="846" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B846" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C846">
         <v>1</v>
@@ -10936,7 +11098,7 @@
     </row>
     <row r="847" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B847" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C847">
         <v>1</v>
@@ -10948,7 +11110,7 @@
     </row>
     <row r="848" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B848" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C848">
         <v>1</v>
@@ -10960,7 +11122,7 @@
     </row>
     <row r="849" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B849" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C849">
         <v>1</v>
@@ -10972,7 +11134,7 @@
     </row>
     <row r="850" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B850" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C850">
         <v>1</v>
@@ -10984,7 +11146,7 @@
     </row>
     <row r="851" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B851" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C851">
         <v>1</v>
@@ -10996,7 +11158,7 @@
     </row>
     <row r="852" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B852" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C852">
         <v>1</v>
@@ -11008,7 +11170,7 @@
     </row>
     <row r="853" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B853" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C853">
         <v>1</v>
@@ -11020,7 +11182,7 @@
     </row>
     <row r="854" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B854" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C854">
         <v>1</v>
@@ -11032,7 +11194,7 @@
     </row>
     <row r="855" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B855" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C855">
         <v>1</v>
@@ -11044,7 +11206,7 @@
     </row>
     <row r="856" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B856" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C856">
         <v>1</v>
@@ -11056,7 +11218,7 @@
     </row>
     <row r="857" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B857" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C857">
         <v>1</v>
@@ -11068,7 +11230,7 @@
     </row>
     <row r="858" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B858" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C858">
         <v>1</v>
@@ -11080,7 +11242,7 @@
     </row>
     <row r="859" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B859" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C859">
         <v>1</v>
@@ -11092,7 +11254,7 @@
     </row>
     <row r="860" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B860" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C860">
         <v>1</v>
@@ -11104,7 +11266,7 @@
     </row>
     <row r="861" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B861" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C861">
         <v>1</v>
@@ -11116,7 +11278,7 @@
     </row>
     <row r="862" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B862" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C862">
         <v>1</v>
@@ -11128,7 +11290,7 @@
     </row>
     <row r="863" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B863" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C863">
         <v>1</v>
@@ -11140,7 +11302,7 @@
     </row>
     <row r="864" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B864" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C864">
         <v>1</v>
@@ -11152,7 +11314,7 @@
     </row>
     <row r="865" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B865" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C865">
         <v>1</v>
@@ -11164,7 +11326,7 @@
     </row>
     <row r="866" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B866" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C866">
         <v>1</v>
@@ -11182,10 +11344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1479B4DB-1D01-41F4-A419-27AD6B416698}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11194,7 +11356,7 @@
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -11205,7 +11367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>153</v>
       </c>
@@ -11216,7 +11378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>154</v>
       </c>
@@ -11227,7 +11389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>155</v>
       </c>
@@ -11238,7 +11400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>156</v>
       </c>
@@ -11249,7 +11411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>157</v>
       </c>
@@ -11260,7 +11422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>195</v>
       </c>
@@ -11271,7 +11433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>196</v>
       </c>
@@ -11282,7 +11444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>157</v>
       </c>
@@ -11293,7 +11455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>226</v>
       </c>
@@ -11304,7 +11466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -11315,7 +11477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>228</v>
       </c>
@@ -11324,6 +11486,276 @@
       </c>
       <c r="C12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="e">
+        <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A13, "'"), "'")</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="e">
+        <f t="shared" ref="D14:D42" si="0">_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A14, "'"), "'")</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved subsets "HeatSlowRamper", "HeatQuickRamper", "Hydro", and "Biomass" to file. deleted subsets "Offshore", "Onshore", and "Oil", since not used
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D28980-B6A8-46D8-9E2B-7E1C15FBE5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD17EF0-3080-4AB2-8D43-D08AE387393B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_TagTechnologyToSubsets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="251">
   <si>
     <t>Technology</t>
   </si>
@@ -754,6 +754,42 @@
   </si>
   <si>
     <t>HeatFuels</t>
+  </si>
+  <si>
+    <t>HeatSlowRamper</t>
+  </si>
+  <si>
+    <t>HeatQuickRamper</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>Res_Hydro_large</t>
+  </si>
+  <si>
+    <t>Res_Hydro_small</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>RES_Grass</t>
+  </si>
+  <si>
+    <t>RES_Wood</t>
+  </si>
+  <si>
+    <t>RES_Residues</t>
+  </si>
+  <si>
+    <t>RES_Paper_Cardboard</t>
+  </si>
+  <si>
+    <t>RES_Roundwood</t>
+  </si>
+  <si>
+    <t>RES_Biogas</t>
   </si>
 </sst>
 </file>
@@ -1082,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D866"/>
   <sheetViews>
-    <sheetView topLeftCell="A446" workbookViewId="0">
-      <selection activeCell="D460" sqref="D460"/>
+    <sheetView tabSelected="1" topLeftCell="A477" workbookViewId="0">
+      <selection activeCell="H497" sqref="H497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6561,8 +6597,11 @@
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A469" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="B469" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C469">
         <v>1</v>
@@ -6573,8 +6612,11 @@
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A470" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="B470" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C470">
         <v>1</v>
@@ -6585,8 +6627,11 @@
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="B471" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C471">
         <v>1</v>
@@ -6597,8 +6642,11 @@
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="B472" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C472">
         <v>1</v>
@@ -6609,8 +6657,11 @@
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="B473" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C473">
         <v>1</v>
@@ -6621,8 +6672,11 @@
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="B474" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C474">
         <v>1</v>
@@ -6633,8 +6687,11 @@
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A475" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="B475" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C475">
         <v>1</v>
@@ -6645,8 +6702,11 @@
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A476" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="B476" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C476">
         <v>1</v>
@@ -6657,8 +6717,11 @@
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A477" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="B477" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C477">
         <v>1</v>
@@ -6669,8 +6732,11 @@
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="B478" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="C478">
         <v>1</v>
@@ -6681,8 +6747,11 @@
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A479" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="B479" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C479">
         <v>1</v>
@@ -6693,8 +6762,11 @@
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A480" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B480" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C480">
         <v>1</v>
@@ -6704,9 +6776,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="481" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A481" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="B481" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C481">
         <v>1</v>
@@ -6716,9 +6791,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="482" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A482" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="B482" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C482">
         <v>1</v>
@@ -6728,9 +6806,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="483" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A483" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="B483" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C483">
         <v>1</v>
@@ -6740,9 +6821,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="484" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A484" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="B484" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C484">
         <v>1</v>
@@ -6752,9 +6836,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="485" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A485" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="B485" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C485">
         <v>1</v>
@@ -6764,9 +6851,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="486" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A486" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="B486" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C486">
         <v>1</v>
@@ -6776,9 +6866,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="487" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A487" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="B487" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C487">
         <v>1</v>
@@ -6788,9 +6881,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="488" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A488" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="B488" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C488">
         <v>1</v>
@@ -6800,9 +6896,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="489" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A489" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B489" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C489">
         <v>1</v>
@@ -6812,9 +6911,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="490" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A490" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="B490" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C490">
         <v>1</v>
@@ -6824,9 +6926,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="491" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A491" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="B491" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C491">
         <v>1</v>
@@ -6836,9 +6941,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="492" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A492" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="B492" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C492">
         <v>1</v>
@@ -6848,9 +6956,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="493" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A493" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="B493" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C493">
         <v>1</v>
@@ -6860,9 +6971,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="494" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A494" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="B494" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C494">
         <v>1</v>
@@ -6872,9 +6986,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="495" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A495" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="B495" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C495">
         <v>1</v>
@@ -6884,9 +7001,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="496" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A496" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="B496" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C496">
         <v>1</v>
@@ -6896,9 +7016,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="497" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A497" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="B497" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
       <c r="C497">
         <v>1</v>
@@ -6908,9 +7031,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="498" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A498" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="B498" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="C498">
         <v>1</v>
@@ -6920,9 +7046,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="499" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A499" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="B499" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="C499">
         <v>1</v>
@@ -6932,9 +7061,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="500" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A500" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="B500" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C500">
         <v>1</v>
@@ -6944,9 +7076,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="501" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A501" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="B501" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C501">
         <v>1</v>
@@ -6956,9 +7091,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="502" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A502" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="B502" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C502">
         <v>1</v>
@@ -6968,9 +7106,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="503" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A503" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="B503" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C503">
         <v>1</v>
@@ -6980,9 +7121,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="504" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A504" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="B504" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C504">
         <v>1</v>
@@ -6992,9 +7136,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="505" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A505" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="B505" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C505">
         <v>1</v>
@@ -7004,9 +7151,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="506" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C506">
         <v>1</v>
@@ -7016,9 +7163,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="507" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C507">
         <v>1</v>
@@ -7028,9 +7175,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="508" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B508" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C508">
         <v>1</v>
@@ -7040,9 +7187,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="509" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B509" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C509">
         <v>1</v>
@@ -7052,9 +7199,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="510" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B510" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C510">
         <v>1</v>
@@ -7064,9 +7211,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="511" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B511" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C511">
         <v>1</v>
@@ -7076,9 +7223,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="512" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B512" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C512">
         <v>1</v>
@@ -7090,7 +7237,7 @@
     </row>
     <row r="513" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B513" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C513">
         <v>1</v>
@@ -7102,7 +7249,7 @@
     </row>
     <row r="514" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B514" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C514">
         <v>1</v>
@@ -7114,7 +7261,7 @@
     </row>
     <row r="515" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B515" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C515">
         <v>1</v>
@@ -7126,7 +7273,7 @@
     </row>
     <row r="516" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B516" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C516">
         <v>1</v>
@@ -7138,7 +7285,7 @@
     </row>
     <row r="517" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B517" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C517">
         <v>1</v>
@@ -7150,7 +7297,7 @@
     </row>
     <row r="518" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B518" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C518">
         <v>1</v>
@@ -7162,7 +7309,7 @@
     </row>
     <row r="519" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B519" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C519">
         <v>1</v>
@@ -7174,7 +7321,7 @@
     </row>
     <row r="520" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B520" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C520">
         <v>1</v>
@@ -7186,7 +7333,7 @@
     </row>
     <row r="521" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B521" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C521">
         <v>1</v>
@@ -7198,7 +7345,7 @@
     </row>
     <row r="522" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B522" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C522">
         <v>1</v>
@@ -7210,7 +7357,7 @@
     </row>
     <row r="523" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B523" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C523">
         <v>1</v>
@@ -7222,7 +7369,7 @@
     </row>
     <row r="524" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B524" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C524">
         <v>1</v>
@@ -7234,7 +7381,7 @@
     </row>
     <row r="525" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B525" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C525">
         <v>1</v>
@@ -7246,7 +7393,7 @@
     </row>
     <row r="526" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B526" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C526">
         <v>1</v>
@@ -7258,7 +7405,7 @@
     </row>
     <row r="527" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B527" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C527">
         <v>1</v>
@@ -7270,7 +7417,7 @@
     </row>
     <row r="528" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B528" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C528">
         <v>1</v>
@@ -7282,7 +7429,7 @@
     </row>
     <row r="529" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B529" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C529">
         <v>1</v>
@@ -7294,7 +7441,7 @@
     </row>
     <row r="530" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B530" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C530">
         <v>1</v>
@@ -7306,7 +7453,7 @@
     </row>
     <row r="531" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B531" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C531">
         <v>1</v>
@@ -7318,7 +7465,7 @@
     </row>
     <row r="532" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B532" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C532">
         <v>1</v>
@@ -7330,7 +7477,7 @@
     </row>
     <row r="533" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B533" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C533">
         <v>1</v>
@@ -7342,7 +7489,7 @@
     </row>
     <row r="534" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B534" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C534">
         <v>1</v>
@@ -7354,7 +7501,7 @@
     </row>
     <row r="535" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B535" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C535">
         <v>1</v>
@@ -7366,7 +7513,7 @@
     </row>
     <row r="536" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B536" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C536">
         <v>1</v>
@@ -7378,7 +7525,7 @@
     </row>
     <row r="537" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B537" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C537">
         <v>1</v>
@@ -7390,7 +7537,7 @@
     </row>
     <row r="538" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B538" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C538">
         <v>1</v>
@@ -7402,7 +7549,7 @@
     </row>
     <row r="539" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B539" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C539">
         <v>1</v>
@@ -7414,7 +7561,7 @@
     </row>
     <row r="540" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B540" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C540">
         <v>1</v>
@@ -7426,7 +7573,7 @@
     </row>
     <row r="541" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B541" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C541">
         <v>1</v>
@@ -7438,7 +7585,7 @@
     </row>
     <row r="542" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B542" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C542">
         <v>1</v>
@@ -7450,7 +7597,7 @@
     </row>
     <row r="543" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B543" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C543">
         <v>1</v>
@@ -7462,7 +7609,7 @@
     </row>
     <row r="544" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B544" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C544">
         <v>1</v>
@@ -7474,7 +7621,7 @@
     </row>
     <row r="545" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B545" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C545">
         <v>1</v>
@@ -7486,7 +7633,7 @@
     </row>
     <row r="546" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B546" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C546">
         <v>1</v>
@@ -7498,7 +7645,7 @@
     </row>
     <row r="547" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B547" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C547">
         <v>1</v>
@@ -7510,7 +7657,7 @@
     </row>
     <row r="548" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B548" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C548">
         <v>1</v>
@@ -7522,7 +7669,7 @@
     </row>
     <row r="549" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B549" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C549">
         <v>1</v>
@@ -7534,7 +7681,7 @@
     </row>
     <row r="550" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B550" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C550">
         <v>1</v>
@@ -7546,7 +7693,7 @@
     </row>
     <row r="551" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B551" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C551">
         <v>1</v>
@@ -7558,7 +7705,7 @@
     </row>
     <row r="552" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B552" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C552">
         <v>1</v>
@@ -7570,7 +7717,7 @@
     </row>
     <row r="553" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B553" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C553">
         <v>1</v>
@@ -7582,7 +7729,7 @@
     </row>
     <row r="554" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B554" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C554">
         <v>1</v>
@@ -7594,7 +7741,7 @@
     </row>
     <row r="555" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B555" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C555">
         <v>1</v>
@@ -7606,7 +7753,7 @@
     </row>
     <row r="556" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B556" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C556">
         <v>1</v>
@@ -7618,7 +7765,7 @@
     </row>
     <row r="557" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B557" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C557">
         <v>1</v>
@@ -7630,7 +7777,7 @@
     </row>
     <row r="558" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B558" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C558">
         <v>1</v>
@@ -7642,7 +7789,7 @@
     </row>
     <row r="559" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B559" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C559">
         <v>1</v>
@@ -7654,7 +7801,7 @@
     </row>
     <row r="560" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B560" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C560">
         <v>1</v>
@@ -7666,7 +7813,7 @@
     </row>
     <row r="561" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B561" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C561">
         <v>1</v>
@@ -7678,7 +7825,7 @@
     </row>
     <row r="562" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B562" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C562">
         <v>1</v>
@@ -7690,7 +7837,7 @@
     </row>
     <row r="563" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B563" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C563">
         <v>1</v>
@@ -7702,7 +7849,7 @@
     </row>
     <row r="564" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B564" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C564">
         <v>1</v>
@@ -7714,7 +7861,7 @@
     </row>
     <row r="565" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B565" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C565">
         <v>1</v>
@@ -7726,7 +7873,7 @@
     </row>
     <row r="566" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B566" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C566">
         <v>1</v>
@@ -7738,7 +7885,7 @@
     </row>
     <row r="567" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B567" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C567">
         <v>1</v>
@@ -7750,7 +7897,7 @@
     </row>
     <row r="568" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B568" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C568">
         <v>1</v>
@@ -7762,7 +7909,7 @@
     </row>
     <row r="569" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B569" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C569">
         <v>1</v>
@@ -7774,7 +7921,7 @@
     </row>
     <row r="570" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B570" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C570">
         <v>1</v>
@@ -7786,7 +7933,7 @@
     </row>
     <row r="571" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B571" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C571">
         <v>1</v>
@@ -7798,7 +7945,7 @@
     </row>
     <row r="572" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B572" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C572">
         <v>1</v>
@@ -7810,7 +7957,7 @@
     </row>
     <row r="573" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B573" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C573">
         <v>1</v>
@@ -7822,7 +7969,7 @@
     </row>
     <row r="574" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B574" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C574">
         <v>1</v>
@@ -7834,7 +7981,7 @@
     </row>
     <row r="575" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B575" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C575">
         <v>1</v>
@@ -7846,7 +7993,7 @@
     </row>
     <row r="576" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B576" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C576">
         <v>1</v>
@@ -7858,7 +8005,7 @@
     </row>
     <row r="577" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B577" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C577">
         <v>1</v>
@@ -7870,7 +8017,7 @@
     </row>
     <row r="578" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B578" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C578">
         <v>1</v>
@@ -7882,7 +8029,7 @@
     </row>
     <row r="579" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B579" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C579">
         <v>1</v>
@@ -7894,7 +8041,7 @@
     </row>
     <row r="580" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B580" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C580">
         <v>1</v>
@@ -7906,7 +8053,7 @@
     </row>
     <row r="581" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B581" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C581">
         <v>1</v>
@@ -7918,7 +8065,7 @@
     </row>
     <row r="582" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B582" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C582">
         <v>1</v>
@@ -7930,7 +8077,7 @@
     </row>
     <row r="583" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B583" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C583">
         <v>1</v>
@@ -7942,7 +8089,7 @@
     </row>
     <row r="584" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B584" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C584">
         <v>1</v>
@@ -7954,7 +8101,7 @@
     </row>
     <row r="585" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B585" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C585">
         <v>1</v>
@@ -7966,7 +8113,7 @@
     </row>
     <row r="586" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B586" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C586">
         <v>1</v>
@@ -7978,7 +8125,7 @@
     </row>
     <row r="587" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B587" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C587">
         <v>1</v>
@@ -7990,7 +8137,7 @@
     </row>
     <row r="588" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B588" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C588">
         <v>1</v>
@@ -8002,7 +8149,7 @@
     </row>
     <row r="589" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B589" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C589">
         <v>1</v>
@@ -8014,7 +8161,7 @@
     </row>
     <row r="590" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B590" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C590">
         <v>1</v>
@@ -8026,7 +8173,7 @@
     </row>
     <row r="591" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B591" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C591">
         <v>1</v>
@@ -8038,7 +8185,7 @@
     </row>
     <row r="592" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B592" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C592">
         <v>1</v>
@@ -8050,7 +8197,7 @@
     </row>
     <row r="593" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B593" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C593">
         <v>1</v>
@@ -8062,7 +8209,7 @@
     </row>
     <row r="594" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B594" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C594">
         <v>1</v>
@@ -8074,7 +8221,7 @@
     </row>
     <row r="595" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B595" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C595">
         <v>1</v>
@@ -8086,7 +8233,7 @@
     </row>
     <row r="596" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B596" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C596">
         <v>1</v>
@@ -8098,7 +8245,7 @@
     </row>
     <row r="597" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B597" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C597">
         <v>1</v>
@@ -8110,7 +8257,7 @@
     </row>
     <row r="598" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B598" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C598">
         <v>1</v>
@@ -8122,7 +8269,7 @@
     </row>
     <row r="599" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B599" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C599">
         <v>1</v>
@@ -8134,7 +8281,7 @@
     </row>
     <row r="600" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B600" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C600">
         <v>1</v>
@@ -8146,7 +8293,7 @@
     </row>
     <row r="601" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B601" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C601">
         <v>1</v>
@@ -8158,7 +8305,7 @@
     </row>
     <row r="602" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B602" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C602">
         <v>1</v>
@@ -8170,7 +8317,7 @@
     </row>
     <row r="603" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B603" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C603">
         <v>1</v>
@@ -8182,7 +8329,7 @@
     </row>
     <row r="604" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B604" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C604">
         <v>1</v>
@@ -8194,7 +8341,7 @@
     </row>
     <row r="605" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B605" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C605">
         <v>1</v>
@@ -8206,7 +8353,7 @@
     </row>
     <row r="606" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B606" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C606">
         <v>1</v>
@@ -8218,7 +8365,7 @@
     </row>
     <row r="607" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B607" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C607">
         <v>1</v>
@@ -8230,7 +8377,7 @@
     </row>
     <row r="608" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B608" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C608">
         <v>1</v>
@@ -8242,7 +8389,7 @@
     </row>
     <row r="609" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B609" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C609">
         <v>1</v>
@@ -8254,7 +8401,7 @@
     </row>
     <row r="610" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B610" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C610">
         <v>1</v>
@@ -8266,7 +8413,7 @@
     </row>
     <row r="611" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B611" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C611">
         <v>1</v>
@@ -8278,7 +8425,7 @@
     </row>
     <row r="612" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B612" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C612">
         <v>1</v>
@@ -8290,7 +8437,7 @@
     </row>
     <row r="613" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B613" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C613">
         <v>1</v>
@@ -8302,7 +8449,7 @@
     </row>
     <row r="614" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B614" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C614">
         <v>1</v>
@@ -8314,7 +8461,7 @@
     </row>
     <row r="615" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B615" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C615">
         <v>1</v>
@@ -8326,7 +8473,7 @@
     </row>
     <row r="616" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B616" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C616">
         <v>1</v>
@@ -8338,7 +8485,7 @@
     </row>
     <row r="617" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B617" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C617">
         <v>1</v>
@@ -8350,7 +8497,7 @@
     </row>
     <row r="618" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B618" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C618">
         <v>1</v>
@@ -8362,7 +8509,7 @@
     </row>
     <row r="619" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B619" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C619">
         <v>1</v>
@@ -8374,7 +8521,7 @@
     </row>
     <row r="620" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B620" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C620">
         <v>1</v>
@@ -8386,7 +8533,7 @@
     </row>
     <row r="621" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B621" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C621">
         <v>1</v>
@@ -8398,7 +8545,7 @@
     </row>
     <row r="622" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B622" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C622">
         <v>1</v>
@@ -8410,7 +8557,7 @@
     </row>
     <row r="623" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B623" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C623">
         <v>1</v>
@@ -8422,7 +8569,7 @@
     </row>
     <row r="624" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B624" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C624">
         <v>1</v>
@@ -8434,7 +8581,7 @@
     </row>
     <row r="625" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B625" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C625">
         <v>1</v>
@@ -8446,7 +8593,7 @@
     </row>
     <row r="626" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B626" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C626">
         <v>1</v>
@@ -8458,7 +8605,7 @@
     </row>
     <row r="627" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B627" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C627">
         <v>1</v>
@@ -8470,7 +8617,7 @@
     </row>
     <row r="628" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B628" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C628">
         <v>1</v>
@@ -8482,7 +8629,7 @@
     </row>
     <row r="629" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B629" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C629">
         <v>1</v>
@@ -8494,7 +8641,7 @@
     </row>
     <row r="630" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B630" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C630">
         <v>1</v>
@@ -8506,7 +8653,7 @@
     </row>
     <row r="631" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B631" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C631">
         <v>1</v>
@@ -8518,7 +8665,7 @@
     </row>
     <row r="632" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B632" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C632">
         <v>1</v>
@@ -8530,7 +8677,7 @@
     </row>
     <row r="633" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B633" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C633">
         <v>1</v>
@@ -8542,7 +8689,7 @@
     </row>
     <row r="634" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B634" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C634">
         <v>1</v>
@@ -8554,7 +8701,7 @@
     </row>
     <row r="635" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B635" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C635">
         <v>1</v>
@@ -8566,7 +8713,7 @@
     </row>
     <row r="636" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B636" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C636">
         <v>1</v>
@@ -8578,7 +8725,7 @@
     </row>
     <row r="637" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B637" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C637">
         <v>1</v>
@@ -8590,7 +8737,7 @@
     </row>
     <row r="638" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B638" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C638">
         <v>1</v>
@@ -8602,7 +8749,7 @@
     </row>
     <row r="639" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B639" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C639">
         <v>1</v>
@@ -8614,7 +8761,7 @@
     </row>
     <row r="640" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B640" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C640">
         <v>1</v>
@@ -8626,7 +8773,7 @@
     </row>
     <row r="641" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B641" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C641">
         <v>1</v>
@@ -8638,7 +8785,7 @@
     </row>
     <row r="642" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B642" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C642">
         <v>1</v>
@@ -8650,7 +8797,7 @@
     </row>
     <row r="643" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B643" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C643">
         <v>1</v>
@@ -8662,7 +8809,7 @@
     </row>
     <row r="644" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B644" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C644">
         <v>1</v>
@@ -8674,7 +8821,7 @@
     </row>
     <row r="645" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B645" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C645">
         <v>1</v>
@@ -8686,7 +8833,7 @@
     </row>
     <row r="646" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B646" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C646">
         <v>1</v>
@@ -8698,7 +8845,7 @@
     </row>
     <row r="647" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B647" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C647">
         <v>1</v>
@@ -8710,7 +8857,7 @@
     </row>
     <row r="648" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B648" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C648">
         <v>1</v>
@@ -8722,7 +8869,7 @@
     </row>
     <row r="649" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B649" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C649">
         <v>1</v>
@@ -8734,7 +8881,7 @@
     </row>
     <row r="650" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B650" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C650">
         <v>1</v>
@@ -8746,7 +8893,7 @@
     </row>
     <row r="651" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B651" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C651">
         <v>1</v>
@@ -8758,7 +8905,7 @@
     </row>
     <row r="652" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B652" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C652">
         <v>1</v>
@@ -8770,7 +8917,7 @@
     </row>
     <row r="653" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B653" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C653">
         <v>1</v>
@@ -8782,7 +8929,7 @@
     </row>
     <row r="654" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B654" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C654">
         <v>1</v>
@@ -8794,7 +8941,7 @@
     </row>
     <row r="655" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B655" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C655">
         <v>1</v>
@@ -8806,7 +8953,7 @@
     </row>
     <row r="656" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B656" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C656">
         <v>1</v>
@@ -8818,7 +8965,7 @@
     </row>
     <row r="657" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B657" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C657">
         <v>1</v>
@@ -8830,7 +8977,7 @@
     </row>
     <row r="658" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B658" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C658">
         <v>1</v>
@@ -8842,7 +8989,7 @@
     </row>
     <row r="659" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B659" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C659">
         <v>1</v>
@@ -8854,7 +9001,7 @@
     </row>
     <row r="660" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B660" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C660">
         <v>1</v>
@@ -8866,7 +9013,7 @@
     </row>
     <row r="661" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B661" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C661">
         <v>1</v>
@@ -8878,7 +9025,7 @@
     </row>
     <row r="662" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B662" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C662">
         <v>1</v>
@@ -8890,7 +9037,7 @@
     </row>
     <row r="663" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B663" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C663">
         <v>1</v>
@@ -8902,7 +9049,7 @@
     </row>
     <row r="664" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B664" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C664">
         <v>1</v>
@@ -8914,7 +9061,7 @@
     </row>
     <row r="665" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B665" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C665">
         <v>1</v>
@@ -8926,7 +9073,7 @@
     </row>
     <row r="666" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B666" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C666">
         <v>1</v>
@@ -8938,7 +9085,7 @@
     </row>
     <row r="667" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B667" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C667">
         <v>1</v>
@@ -8950,7 +9097,7 @@
     </row>
     <row r="668" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B668" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C668">
         <v>1</v>
@@ -8962,7 +9109,7 @@
     </row>
     <row r="669" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B669" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C669">
         <v>1</v>
@@ -8974,7 +9121,7 @@
     </row>
     <row r="670" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B670" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C670">
         <v>1</v>
@@ -8986,7 +9133,7 @@
     </row>
     <row r="671" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B671" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C671">
         <v>1</v>
@@ -8998,7 +9145,7 @@
     </row>
     <row r="672" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B672" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C672">
         <v>1</v>
@@ -9010,7 +9157,7 @@
     </row>
     <row r="673" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B673" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C673">
         <v>1</v>
@@ -9022,7 +9169,7 @@
     </row>
     <row r="674" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B674" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C674">
         <v>1</v>
@@ -9034,7 +9181,7 @@
     </row>
     <row r="675" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B675" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C675">
         <v>1</v>
@@ -9046,7 +9193,7 @@
     </row>
     <row r="676" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B676" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C676">
         <v>1</v>
@@ -9058,7 +9205,7 @@
     </row>
     <row r="677" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B677" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C677">
         <v>1</v>
@@ -9070,7 +9217,7 @@
     </row>
     <row r="678" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B678" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C678">
         <v>1</v>
@@ -9082,7 +9229,7 @@
     </row>
     <row r="679" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B679" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C679">
         <v>1</v>
@@ -9094,7 +9241,7 @@
     </row>
     <row r="680" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B680" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C680">
         <v>1</v>
@@ -9106,7 +9253,7 @@
     </row>
     <row r="681" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B681" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C681">
         <v>1</v>
@@ -9118,7 +9265,7 @@
     </row>
     <row r="682" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B682" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C682">
         <v>1</v>
@@ -9130,7 +9277,7 @@
     </row>
     <row r="683" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B683" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C683">
         <v>1</v>
@@ -9142,7 +9289,7 @@
     </row>
     <row r="684" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B684" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C684">
         <v>1</v>
@@ -9154,7 +9301,7 @@
     </row>
     <row r="685" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B685" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C685">
         <v>1</v>
@@ -9166,7 +9313,7 @@
     </row>
     <row r="686" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B686" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C686">
         <v>1</v>
@@ -9178,7 +9325,7 @@
     </row>
     <row r="687" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B687" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C687">
         <v>1</v>
@@ -9190,7 +9337,7 @@
     </row>
     <row r="688" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B688" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C688">
         <v>1</v>
@@ -9202,7 +9349,7 @@
     </row>
     <row r="689" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B689" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C689">
         <v>1</v>
@@ -9214,7 +9361,7 @@
     </row>
     <row r="690" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B690" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C690">
         <v>1</v>
@@ -9226,7 +9373,7 @@
     </row>
     <row r="691" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B691" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C691">
         <v>1</v>
@@ -9238,7 +9385,7 @@
     </row>
     <row r="692" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B692" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C692">
         <v>1</v>
@@ -9250,7 +9397,7 @@
     </row>
     <row r="693" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B693" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C693">
         <v>1</v>
@@ -9262,7 +9409,7 @@
     </row>
     <row r="694" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B694" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C694">
         <v>1</v>
@@ -9274,7 +9421,7 @@
     </row>
     <row r="695" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B695" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C695">
         <v>1</v>
@@ -9286,7 +9433,7 @@
     </row>
     <row r="696" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B696" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C696">
         <v>1</v>
@@ -9298,7 +9445,7 @@
     </row>
     <row r="697" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B697" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C697">
         <v>1</v>
@@ -9310,7 +9457,7 @@
     </row>
     <row r="698" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B698" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C698">
         <v>1</v>
@@ -9322,7 +9469,7 @@
     </row>
     <row r="699" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B699" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C699">
         <v>1</v>
@@ -9334,7 +9481,7 @@
     </row>
     <row r="700" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B700" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C700">
         <v>1</v>
@@ -9346,7 +9493,7 @@
     </row>
     <row r="701" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B701" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C701">
         <v>1</v>
@@ -9358,7 +9505,7 @@
     </row>
     <row r="702" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B702" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C702">
         <v>1</v>
@@ -9370,7 +9517,7 @@
     </row>
     <row r="703" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B703" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C703">
         <v>1</v>
@@ -9382,7 +9529,7 @@
     </row>
     <row r="704" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B704" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C704">
         <v>1</v>
@@ -9394,7 +9541,7 @@
     </row>
     <row r="705" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B705" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C705">
         <v>1</v>
@@ -9406,7 +9553,7 @@
     </row>
     <row r="706" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B706" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C706">
         <v>1</v>
@@ -9418,7 +9565,7 @@
     </row>
     <row r="707" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B707" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C707">
         <v>1</v>
@@ -9430,7 +9577,7 @@
     </row>
     <row r="708" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B708" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C708">
         <v>1</v>
@@ -9442,7 +9589,7 @@
     </row>
     <row r="709" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B709" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C709">
         <v>1</v>
@@ -9454,7 +9601,7 @@
     </row>
     <row r="710" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B710" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C710">
         <v>1</v>
@@ -9466,7 +9613,7 @@
     </row>
     <row r="711" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B711" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C711">
         <v>1</v>
@@ -9478,7 +9625,7 @@
     </row>
     <row r="712" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B712" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C712">
         <v>1</v>
@@ -9490,7 +9637,7 @@
     </row>
     <row r="713" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B713" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C713">
         <v>1</v>
@@ -9502,7 +9649,7 @@
     </row>
     <row r="714" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B714" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C714">
         <v>1</v>
@@ -9514,7 +9661,7 @@
     </row>
     <row r="715" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B715" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C715">
         <v>1</v>
@@ -9526,7 +9673,7 @@
     </row>
     <row r="716" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B716" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C716">
         <v>1</v>
@@ -9538,7 +9685,7 @@
     </row>
     <row r="717" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B717" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C717">
         <v>1</v>
@@ -9550,7 +9697,7 @@
     </row>
     <row r="718" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B718" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C718">
         <v>1</v>
@@ -9562,7 +9709,7 @@
     </row>
     <row r="719" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B719" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C719">
         <v>1</v>
@@ -9574,7 +9721,7 @@
     </row>
     <row r="720" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B720" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C720">
         <v>1</v>
@@ -9586,7 +9733,7 @@
     </row>
     <row r="721" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B721" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C721">
         <v>1</v>
@@ -9598,7 +9745,7 @@
     </row>
     <row r="722" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B722" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C722">
         <v>1</v>
@@ -9610,7 +9757,7 @@
     </row>
     <row r="723" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B723" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C723">
         <v>1</v>
@@ -9622,7 +9769,7 @@
     </row>
     <row r="724" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B724" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C724">
         <v>1</v>
@@ -9634,7 +9781,7 @@
     </row>
     <row r="725" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B725" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C725">
         <v>1</v>
@@ -9646,7 +9793,7 @@
     </row>
     <row r="726" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B726" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C726">
         <v>1</v>
@@ -9658,7 +9805,7 @@
     </row>
     <row r="727" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B727" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C727">
         <v>1</v>
@@ -9670,7 +9817,7 @@
     </row>
     <row r="728" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B728" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C728">
         <v>1</v>
@@ -9682,7 +9829,7 @@
     </row>
     <row r="729" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B729" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C729">
         <v>1</v>
@@ -9694,7 +9841,7 @@
     </row>
     <row r="730" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B730" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C730">
         <v>1</v>
@@ -9706,7 +9853,7 @@
     </row>
     <row r="731" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B731" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C731">
         <v>1</v>
@@ -9718,7 +9865,7 @@
     </row>
     <row r="732" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B732" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C732">
         <v>1</v>
@@ -9730,7 +9877,7 @@
     </row>
     <row r="733" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B733" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C733">
         <v>1</v>
@@ -9742,7 +9889,7 @@
     </row>
     <row r="734" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B734" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C734">
         <v>1</v>
@@ -9754,7 +9901,7 @@
     </row>
     <row r="735" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B735" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C735">
         <v>1</v>
@@ -9766,7 +9913,7 @@
     </row>
     <row r="736" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B736" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C736">
         <v>1</v>
@@ -9778,7 +9925,7 @@
     </row>
     <row r="737" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B737" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C737">
         <v>1</v>
@@ -9790,7 +9937,7 @@
     </row>
     <row r="738" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B738" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C738">
         <v>1</v>
@@ -9802,7 +9949,7 @@
     </row>
     <row r="739" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B739" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C739">
         <v>1</v>
@@ -9814,7 +9961,7 @@
     </row>
     <row r="740" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B740" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C740">
         <v>1</v>
@@ -9826,7 +9973,7 @@
     </row>
     <row r="741" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B741" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C741">
         <v>1</v>
@@ -9838,7 +9985,7 @@
     </row>
     <row r="742" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B742" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C742">
         <v>1</v>
@@ -9850,7 +9997,7 @@
     </row>
     <row r="743" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B743" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C743">
         <v>1</v>
@@ -9862,7 +10009,7 @@
     </row>
     <row r="744" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B744" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C744">
         <v>1</v>
@@ -9874,7 +10021,7 @@
     </row>
     <row r="745" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B745" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C745">
         <v>1</v>
@@ -9886,7 +10033,7 @@
     </row>
     <row r="746" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B746" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C746">
         <v>1</v>
@@ -9898,7 +10045,7 @@
     </row>
     <row r="747" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B747" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C747">
         <v>1</v>
@@ -9910,7 +10057,7 @@
     </row>
     <row r="748" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B748" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C748">
         <v>1</v>
@@ -9922,7 +10069,7 @@
     </row>
     <row r="749" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B749" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C749">
         <v>1</v>
@@ -9934,7 +10081,7 @@
     </row>
     <row r="750" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B750" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C750">
         <v>1</v>
@@ -9946,7 +10093,7 @@
     </row>
     <row r="751" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B751" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C751">
         <v>1</v>
@@ -9958,7 +10105,7 @@
     </row>
     <row r="752" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B752" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C752">
         <v>1</v>
@@ -9970,7 +10117,7 @@
     </row>
     <row r="753" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B753" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C753">
         <v>1</v>
@@ -9982,7 +10129,7 @@
     </row>
     <row r="754" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B754" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C754">
         <v>1</v>
@@ -9994,7 +10141,7 @@
     </row>
     <row r="755" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B755" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C755">
         <v>1</v>
@@ -10006,7 +10153,7 @@
     </row>
     <row r="756" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B756" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C756">
         <v>1</v>
@@ -10018,7 +10165,7 @@
     </row>
     <row r="757" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B757" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C757">
         <v>1</v>
@@ -10030,7 +10177,7 @@
     </row>
     <row r="758" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B758" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C758">
         <v>1</v>
@@ -10042,7 +10189,7 @@
     </row>
     <row r="759" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B759" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C759">
         <v>1</v>
@@ -10054,7 +10201,7 @@
     </row>
     <row r="760" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B760" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C760">
         <v>1</v>
@@ -10066,7 +10213,7 @@
     </row>
     <row r="761" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B761" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C761">
         <v>1</v>
@@ -10078,7 +10225,7 @@
     </row>
     <row r="762" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B762" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C762">
         <v>1</v>
@@ -10090,7 +10237,7 @@
     </row>
     <row r="763" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B763" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C763">
         <v>1</v>
@@ -10102,7 +10249,7 @@
     </row>
     <row r="764" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B764" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C764">
         <v>1</v>
@@ -10114,7 +10261,7 @@
     </row>
     <row r="765" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B765" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C765">
         <v>1</v>
@@ -10126,7 +10273,7 @@
     </row>
     <row r="766" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B766" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C766">
         <v>1</v>
@@ -10138,7 +10285,7 @@
     </row>
     <row r="767" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B767" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C767">
         <v>1</v>
@@ -10150,7 +10297,7 @@
     </row>
     <row r="768" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B768" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C768">
         <v>1</v>
@@ -10162,7 +10309,7 @@
     </row>
     <row r="769" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B769" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C769">
         <v>1</v>
@@ -10174,7 +10321,7 @@
     </row>
     <row r="770" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B770" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C770">
         <v>1</v>
@@ -10186,7 +10333,7 @@
     </row>
     <row r="771" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B771" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C771">
         <v>1</v>
@@ -10198,7 +10345,7 @@
     </row>
     <row r="772" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B772" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C772">
         <v>1</v>
@@ -10210,7 +10357,7 @@
     </row>
     <row r="773" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B773" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C773">
         <v>1</v>
@@ -10222,7 +10369,7 @@
     </row>
     <row r="774" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B774" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C774">
         <v>1</v>
@@ -10234,7 +10381,7 @@
     </row>
     <row r="775" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B775" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C775">
         <v>1</v>
@@ -10246,7 +10393,7 @@
     </row>
     <row r="776" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B776" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C776">
         <v>1</v>
@@ -10258,7 +10405,7 @@
     </row>
     <row r="777" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B777" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C777">
         <v>1</v>
@@ -10270,7 +10417,7 @@
     </row>
     <row r="778" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B778" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C778">
         <v>1</v>
@@ -10282,7 +10429,7 @@
     </row>
     <row r="779" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B779" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C779">
         <v>1</v>
@@ -10294,7 +10441,7 @@
     </row>
     <row r="780" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B780" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C780">
         <v>1</v>
@@ -10306,7 +10453,7 @@
     </row>
     <row r="781" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B781" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C781">
         <v>1</v>
@@ -10318,7 +10465,7 @@
     </row>
     <row r="782" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B782" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C782">
         <v>1</v>
@@ -10330,7 +10477,7 @@
     </row>
     <row r="783" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B783" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C783">
         <v>1</v>
@@ -10342,7 +10489,7 @@
     </row>
     <row r="784" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B784" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C784">
         <v>1</v>
@@ -10354,7 +10501,7 @@
     </row>
     <row r="785" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B785" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C785">
         <v>1</v>
@@ -10366,7 +10513,7 @@
     </row>
     <row r="786" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B786" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C786">
         <v>1</v>
@@ -10378,7 +10525,7 @@
     </row>
     <row r="787" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B787" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C787">
         <v>1</v>
@@ -10390,7 +10537,7 @@
     </row>
     <row r="788" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B788" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C788">
         <v>1</v>
@@ -10402,7 +10549,7 @@
     </row>
     <row r="789" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B789" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C789">
         <v>1</v>
@@ -10414,7 +10561,7 @@
     </row>
     <row r="790" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B790" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C790">
         <v>1</v>
@@ -10426,7 +10573,7 @@
     </row>
     <row r="791" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B791" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C791">
         <v>1</v>
@@ -10438,7 +10585,7 @@
     </row>
     <row r="792" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B792" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C792">
         <v>1</v>
@@ -10450,7 +10597,7 @@
     </row>
     <row r="793" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B793" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C793">
         <v>1</v>
@@ -10462,7 +10609,7 @@
     </row>
     <row r="794" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B794" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C794">
         <v>1</v>
@@ -10474,7 +10621,7 @@
     </row>
     <row r="795" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B795" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C795">
         <v>1</v>
@@ -10486,7 +10633,7 @@
     </row>
     <row r="796" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B796" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C796">
         <v>1</v>
@@ -10498,7 +10645,7 @@
     </row>
     <row r="797" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B797" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C797">
         <v>1</v>
@@ -10510,7 +10657,7 @@
     </row>
     <row r="798" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B798" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C798">
         <v>1</v>
@@ -10522,7 +10669,7 @@
     </row>
     <row r="799" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B799" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C799">
         <v>1</v>
@@ -10534,7 +10681,7 @@
     </row>
     <row r="800" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B800" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C800">
         <v>1</v>
@@ -10546,7 +10693,7 @@
     </row>
     <row r="801" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B801" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C801">
         <v>1</v>
@@ -10558,7 +10705,7 @@
     </row>
     <row r="802" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B802" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C802">
         <v>1</v>
@@ -10570,7 +10717,7 @@
     </row>
     <row r="803" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B803" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C803">
         <v>1</v>
@@ -10582,7 +10729,7 @@
     </row>
     <row r="804" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B804" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C804">
         <v>1</v>
@@ -10594,7 +10741,7 @@
     </row>
     <row r="805" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B805" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C805">
         <v>1</v>
@@ -10606,7 +10753,7 @@
     </row>
     <row r="806" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B806" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C806">
         <v>1</v>
@@ -10618,7 +10765,7 @@
     </row>
     <row r="807" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B807" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C807">
         <v>1</v>
@@ -10630,7 +10777,7 @@
     </row>
     <row r="808" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B808" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C808">
         <v>1</v>
@@ -10642,7 +10789,7 @@
     </row>
     <row r="809" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B809" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C809">
         <v>1</v>
@@ -10654,7 +10801,7 @@
     </row>
     <row r="810" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B810" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C810">
         <v>1</v>
@@ -10666,7 +10813,7 @@
     </row>
     <row r="811" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B811" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C811">
         <v>1</v>
@@ -10678,7 +10825,7 @@
     </row>
     <row r="812" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B812" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C812">
         <v>1</v>
@@ -10690,7 +10837,7 @@
     </row>
     <row r="813" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B813" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C813">
         <v>1</v>
@@ -10702,7 +10849,7 @@
     </row>
     <row r="814" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B814" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C814">
         <v>1</v>
@@ -10714,7 +10861,7 @@
     </row>
     <row r="815" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B815" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C815">
         <v>1</v>
@@ -10726,7 +10873,7 @@
     </row>
     <row r="816" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B816" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C816">
         <v>1</v>
@@ -10738,7 +10885,7 @@
     </row>
     <row r="817" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B817" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C817">
         <v>1</v>
@@ -10750,7 +10897,7 @@
     </row>
     <row r="818" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B818" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C818">
         <v>1</v>
@@ -10762,7 +10909,7 @@
     </row>
     <row r="819" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B819" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C819">
         <v>1</v>
@@ -10774,7 +10921,7 @@
     </row>
     <row r="820" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B820" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C820">
         <v>1</v>
@@ -10786,7 +10933,7 @@
     </row>
     <row r="821" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B821" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C821">
         <v>1</v>
@@ -10798,7 +10945,7 @@
     </row>
     <row r="822" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B822" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C822">
         <v>1</v>
@@ -10810,7 +10957,7 @@
     </row>
     <row r="823" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B823" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C823">
         <v>1</v>
@@ -10822,7 +10969,7 @@
     </row>
     <row r="824" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B824" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C824">
         <v>1</v>
@@ -10834,7 +10981,7 @@
     </row>
     <row r="825" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B825" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C825">
         <v>1</v>
@@ -10846,7 +10993,7 @@
     </row>
     <row r="826" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B826" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C826">
         <v>1</v>
@@ -10858,7 +11005,7 @@
     </row>
     <row r="827" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B827" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C827">
         <v>1</v>
@@ -10870,7 +11017,7 @@
     </row>
     <row r="828" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B828" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C828">
         <v>1</v>
@@ -10882,7 +11029,7 @@
     </row>
     <row r="829" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B829" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C829">
         <v>1</v>
@@ -10894,7 +11041,7 @@
     </row>
     <row r="830" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B830" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C830">
         <v>1</v>
@@ -10906,7 +11053,7 @@
     </row>
     <row r="831" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B831" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C831">
         <v>1</v>
@@ -10918,7 +11065,7 @@
     </row>
     <row r="832" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B832" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C832">
         <v>1</v>
@@ -10930,7 +11077,7 @@
     </row>
     <row r="833" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B833" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C833">
         <v>1</v>
@@ -10942,7 +11089,7 @@
     </row>
     <row r="834" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B834" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C834">
         <v>1</v>
@@ -10954,7 +11101,7 @@
     </row>
     <row r="835" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B835" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C835">
         <v>1</v>
@@ -10966,7 +11113,7 @@
     </row>
     <row r="836" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B836" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C836">
         <v>1</v>
@@ -10978,7 +11125,7 @@
     </row>
     <row r="837" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B837" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C837">
         <v>1</v>
@@ -10990,7 +11137,7 @@
     </row>
     <row r="838" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B838" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C838">
         <v>1</v>
@@ -11002,7 +11149,7 @@
     </row>
     <row r="839" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B839" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C839">
         <v>1</v>
@@ -11014,7 +11161,7 @@
     </row>
     <row r="840" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B840" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C840">
         <v>1</v>
@@ -11026,7 +11173,7 @@
     </row>
     <row r="841" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B841" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C841">
         <v>1</v>
@@ -11038,7 +11185,7 @@
     </row>
     <row r="842" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B842" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C842">
         <v>1</v>
@@ -11050,7 +11197,7 @@
     </row>
     <row r="843" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B843" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C843">
         <v>1</v>
@@ -11062,7 +11209,7 @@
     </row>
     <row r="844" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B844" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C844">
         <v>1</v>
@@ -11074,7 +11221,7 @@
     </row>
     <row r="845" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B845" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C845">
         <v>1</v>
@@ -11086,7 +11233,7 @@
     </row>
     <row r="846" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B846" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C846">
         <v>1</v>
@@ -11098,7 +11245,7 @@
     </row>
     <row r="847" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B847" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C847">
         <v>1</v>
@@ -11110,7 +11257,7 @@
     </row>
     <row r="848" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B848" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C848">
         <v>1</v>
@@ -11122,7 +11269,7 @@
     </row>
     <row r="849" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B849" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C849">
         <v>1</v>
@@ -11134,7 +11281,7 @@
     </row>
     <row r="850" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B850" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C850">
         <v>1</v>
@@ -11146,7 +11293,7 @@
     </row>
     <row r="851" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B851" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C851">
         <v>1</v>
@@ -11158,7 +11305,7 @@
     </row>
     <row r="852" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B852" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C852">
         <v>1</v>
@@ -11170,7 +11317,7 @@
     </row>
     <row r="853" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B853" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C853">
         <v>1</v>
@@ -11182,7 +11329,7 @@
     </row>
     <row r="854" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B854" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C854">
         <v>1</v>
@@ -11194,7 +11341,7 @@
     </row>
     <row r="855" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B855" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C855">
         <v>1</v>
@@ -11206,7 +11353,7 @@
     </row>
     <row r="856" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B856" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C856">
         <v>1</v>
@@ -11218,7 +11365,7 @@
     </row>
     <row r="857" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B857" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C857">
         <v>1</v>
@@ -11230,7 +11377,7 @@
     </row>
     <row r="858" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B858" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C858">
         <v>1</v>
@@ -11242,7 +11389,7 @@
     </row>
     <row r="859" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B859" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C859">
         <v>1</v>
@@ -11254,7 +11401,7 @@
     </row>
     <row r="860" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B860" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C860">
         <v>1</v>
@@ -11266,7 +11413,7 @@
     </row>
     <row r="861" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B861" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C861">
         <v>1</v>
@@ -11278,7 +11425,7 @@
     </row>
     <row r="862" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B862" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C862">
         <v>1</v>
@@ -11290,7 +11437,7 @@
     </row>
     <row r="863" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B863" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C863">
         <v>1</v>
@@ -11302,7 +11449,7 @@
     </row>
     <row r="864" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B864" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C864">
         <v>1</v>
@@ -11314,7 +11461,7 @@
     </row>
     <row r="865" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B865" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C865">
         <v>1</v>
@@ -11326,7 +11473,7 @@
     </row>
     <row r="866" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B866" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="C866">
         <v>1</v>
@@ -11346,7 +11493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1479B4DB-1D01-41F4-A419-27AD6B416698}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C12" sqref="C12:C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
moved ramping code to input data file and dataload; deleted subsets "Lignite", "FossilFuels", "PowerBiomass", "Coal", "Gas", "HeatSlowRamper", "HeatQuickRamper"
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35E9F70-66D8-46A0-A529-E946CD213CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F94203B-52A3-49BE-A31C-C310A03A98B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="242">
   <si>
     <t>Technology</t>
   </si>
@@ -495,21 +495,6 @@
     <t>FossilFuelGeneration</t>
   </si>
   <si>
-    <t xml:space="preserve">FossilFuels </t>
-  </si>
-  <si>
-    <t>Hardcoal</t>
-  </si>
-  <si>
-    <t>Lignite</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
-    <t>Oil</t>
-  </si>
-  <si>
     <t>Gas_Natural</t>
   </si>
   <si>
@@ -729,15 +714,6 @@
     <t>PowerSupply</t>
   </si>
   <si>
-    <t>PowerBiomass</t>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
     <t>SectorCoupling</t>
   </si>
   <si>
@@ -754,12 +730,6 @@
   </si>
   <si>
     <t>HeatFuels</t>
-  </si>
-  <si>
-    <t>HeatSlowRamper</t>
-  </si>
-  <si>
-    <t>HeatQuickRamper</t>
   </si>
   <si>
     <t>Hydro</t>
@@ -1119,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C514"/>
+  <dimension ref="A1:C444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A499" workbookViewId="0">
-      <selection activeCell="E510" sqref="E510"/>
+    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="E417" sqref="E417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,10 +2753,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B151" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -2794,10 +2764,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B152" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -2805,10 +2775,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -2816,10 +2786,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B154" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -2827,10 +2797,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B155" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -2838,10 +2808,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B156" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -2849,10 +2819,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B157" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -2860,10 +2830,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B158" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -2871,10 +2841,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -2882,10 +2852,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B160" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -2896,7 +2866,7 @@
         <v>132</v>
       </c>
       <c r="B161" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -2907,7 +2877,7 @@
         <v>133</v>
       </c>
       <c r="B162" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -2918,7 +2888,7 @@
         <v>134</v>
       </c>
       <c r="B163" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -2929,7 +2899,7 @@
         <v>138</v>
       </c>
       <c r="B164" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -2940,7 +2910,7 @@
         <v>139</v>
       </c>
       <c r="B165" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -2951,7 +2921,7 @@
         <v>77</v>
       </c>
       <c r="B166" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C166">
         <v>1</v>
@@ -2962,7 +2932,7 @@
         <v>142</v>
       </c>
       <c r="B167" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -2973,7 +2943,7 @@
         <v>131</v>
       </c>
       <c r="B168" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C168">
         <v>1</v>
@@ -2984,7 +2954,7 @@
         <v>132</v>
       </c>
       <c r="B169" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -2995,7 +2965,7 @@
         <v>133</v>
       </c>
       <c r="B170" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -3006,7 +2976,7 @@
         <v>134</v>
       </c>
       <c r="B171" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -3017,7 +2987,7 @@
         <v>135</v>
       </c>
       <c r="B172" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -3028,7 +2998,7 @@
         <v>136</v>
       </c>
       <c r="B173" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -3039,7 +3009,7 @@
         <v>137</v>
       </c>
       <c r="B174" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C174">
         <v>1</v>
@@ -3050,7 +3020,7 @@
         <v>138</v>
       </c>
       <c r="B175" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -3061,7 +3031,7 @@
         <v>139</v>
       </c>
       <c r="B176" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -3072,7 +3042,7 @@
         <v>77</v>
       </c>
       <c r="B177" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -3083,7 +3053,7 @@
         <v>140</v>
       </c>
       <c r="B178" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -3094,7 +3064,7 @@
         <v>141</v>
       </c>
       <c r="B179" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -3105,7 +3075,7 @@
         <v>142</v>
       </c>
       <c r="B180" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -3113,10 +3083,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B181" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -3124,10 +3094,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B182" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -3135,10 +3105,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -3146,10 +3116,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B184" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -3157,10 +3127,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B185" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -3168,10 +3138,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B186" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -3179,10 +3149,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B187" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -3190,10 +3160,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B188" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -3201,10 +3171,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B189" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C189">
         <v>1</v>
@@ -3212,10 +3182,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B190" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -3223,10 +3193,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B191" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C191">
         <v>1</v>
@@ -3234,10 +3204,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B192" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C192">
         <v>1</v>
@@ -3245,10 +3215,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B193" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -3256,10 +3226,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B194" t="s">
         <v>180</v>
-      </c>
-      <c r="B194" t="s">
-        <v>185</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -3267,10 +3237,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B195" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C195">
         <v>1</v>
@@ -3278,10 +3248,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B196" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C196">
         <v>1</v>
@@ -3289,10 +3259,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B197" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -3300,10 +3270,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B198" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -3311,10 +3281,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B199" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -3322,10 +3292,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B200" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -3333,10 +3303,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B201" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -3344,10 +3314,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B202" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -3355,10 +3325,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B203" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C203">
         <v>1</v>
@@ -3366,10 +3336,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B204" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -3377,10 +3347,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B205" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -3388,10 +3358,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B206" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -3399,10 +3369,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B207" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -3410,10 +3380,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B208" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -3421,10 +3391,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B209" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C209">
         <v>1</v>
@@ -3432,10 +3402,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B210" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -3443,10 +3413,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B211" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -3454,10 +3424,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B212" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C212">
         <v>1</v>
@@ -3465,10 +3435,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B213" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C213">
         <v>1</v>
@@ -3476,10 +3446,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B214" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C214">
         <v>1</v>
@@ -3487,10 +3457,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B215" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -3498,10 +3468,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B216" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -3509,10 +3479,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B217" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C217">
         <v>1</v>
@@ -3520,10 +3490,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B218" t="s">
         <v>188</v>
-      </c>
-      <c r="B218" t="s">
-        <v>193</v>
       </c>
       <c r="C218">
         <v>1</v>
@@ -3534,7 +3504,7 @@
         <v>94</v>
       </c>
       <c r="B219" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -3545,7 +3515,7 @@
         <v>95</v>
       </c>
       <c r="B220" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -3556,7 +3526,7 @@
         <v>96</v>
       </c>
       <c r="B221" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -3567,7 +3537,7 @@
         <v>97</v>
       </c>
       <c r="B222" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -3578,7 +3548,7 @@
         <v>98</v>
       </c>
       <c r="B223" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -3589,7 +3559,7 @@
         <v>4</v>
       </c>
       <c r="B224" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -3600,7 +3570,7 @@
         <v>99</v>
       </c>
       <c r="B225" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -3611,7 +3581,7 @@
         <v>100</v>
       </c>
       <c r="B226" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -3622,7 +3592,7 @@
         <v>101</v>
       </c>
       <c r="B227" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -3633,7 +3603,7 @@
         <v>102</v>
       </c>
       <c r="B228" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -3644,7 +3614,7 @@
         <v>104</v>
       </c>
       <c r="B229" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -3655,7 +3625,7 @@
         <v>105</v>
       </c>
       <c r="B230" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -3666,7 +3636,7 @@
         <v>106</v>
       </c>
       <c r="B231" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C231">
         <v>1</v>
@@ -3677,7 +3647,7 @@
         <v>107</v>
       </c>
       <c r="B232" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C232">
         <v>1</v>
@@ -3688,7 +3658,7 @@
         <v>108</v>
       </c>
       <c r="B233" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C233">
         <v>1</v>
@@ -3699,7 +3669,7 @@
         <v>5</v>
       </c>
       <c r="B234" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C234">
         <v>1</v>
@@ -3710,7 +3680,7 @@
         <v>109</v>
       </c>
       <c r="B235" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C235">
         <v>1</v>
@@ -3721,7 +3691,7 @@
         <v>110</v>
       </c>
       <c r="B236" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C236">
         <v>1</v>
@@ -3732,7 +3702,7 @@
         <v>111</v>
       </c>
       <c r="B237" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C237">
         <v>1</v>
@@ -3743,7 +3713,7 @@
         <v>113</v>
       </c>
       <c r="B238" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C238">
         <v>1</v>
@@ -3754,7 +3724,7 @@
         <v>114</v>
       </c>
       <c r="B239" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C239">
         <v>1</v>
@@ -3765,7 +3735,7 @@
         <v>115</v>
       </c>
       <c r="B240" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C240">
         <v>1</v>
@@ -3776,7 +3746,7 @@
         <v>116</v>
       </c>
       <c r="B241" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C241">
         <v>1</v>
@@ -3787,7 +3757,7 @@
         <v>117</v>
       </c>
       <c r="B242" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C242">
         <v>1</v>
@@ -3798,7 +3768,7 @@
         <v>118</v>
       </c>
       <c r="B243" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -3809,7 +3779,7 @@
         <v>119</v>
       </c>
       <c r="B244" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -3820,7 +3790,7 @@
         <v>120</v>
       </c>
       <c r="B245" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C245">
         <v>1</v>
@@ -3831,7 +3801,7 @@
         <v>121</v>
       </c>
       <c r="B246" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -3842,7 +3812,7 @@
         <v>122</v>
       </c>
       <c r="B247" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -3853,7 +3823,7 @@
         <v>123</v>
       </c>
       <c r="B248" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -3864,7 +3834,7 @@
         <v>124</v>
       </c>
       <c r="B249" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -3875,7 +3845,7 @@
         <v>125</v>
       </c>
       <c r="B250" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -3886,7 +3856,7 @@
         <v>126</v>
       </c>
       <c r="B251" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -3897,7 +3867,7 @@
         <v>127</v>
       </c>
       <c r="B252" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -3908,7 +3878,7 @@
         <v>103</v>
       </c>
       <c r="B253" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -3919,7 +3889,7 @@
         <v>112</v>
       </c>
       <c r="B254" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C254">
         <v>1</v>
@@ -3930,7 +3900,7 @@
         <v>131</v>
       </c>
       <c r="B255" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -3941,7 +3911,7 @@
         <v>132</v>
       </c>
       <c r="B256" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -3952,7 +3922,7 @@
         <v>133</v>
       </c>
       <c r="B257" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -3963,7 +3933,7 @@
         <v>134</v>
       </c>
       <c r="B258" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -3974,7 +3944,7 @@
         <v>135</v>
       </c>
       <c r="B259" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C259">
         <v>1</v>
@@ -3985,7 +3955,7 @@
         <v>136</v>
       </c>
       <c r="B260" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C260">
         <v>1</v>
@@ -3996,7 +3966,7 @@
         <v>137</v>
       </c>
       <c r="B261" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -4007,7 +3977,7 @@
         <v>138</v>
       </c>
       <c r="B262" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C262">
         <v>1</v>
@@ -4018,7 +3988,7 @@
         <v>139</v>
       </c>
       <c r="B263" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C263">
         <v>1</v>
@@ -4029,7 +3999,7 @@
         <v>77</v>
       </c>
       <c r="B264" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C264">
         <v>1</v>
@@ -4040,7 +4010,7 @@
         <v>140</v>
       </c>
       <c r="B265" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C265">
         <v>1</v>
@@ -4051,7 +4021,7 @@
         <v>141</v>
       </c>
       <c r="B266" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C266">
         <v>1</v>
@@ -4062,7 +4032,7 @@
         <v>142</v>
       </c>
       <c r="B267" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C267">
         <v>1</v>
@@ -4070,10 +4040,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B268" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C268">
         <v>1</v>
@@ -4081,10 +4051,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B269" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -4095,7 +4065,7 @@
         <v>150</v>
       </c>
       <c r="B270" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C270">
         <v>1</v>
@@ -4106,7 +4076,7 @@
         <v>149</v>
       </c>
       <c r="B271" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C271">
         <v>1</v>
@@ -4117,7 +4087,7 @@
         <v>148</v>
       </c>
       <c r="B272" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C272">
         <v>1</v>
@@ -4125,10 +4095,10 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B273" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C273">
         <v>1</v>
@@ -4136,10 +4106,10 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B274" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C274">
         <v>1</v>
@@ -4150,7 +4120,7 @@
         <v>86</v>
       </c>
       <c r="B275" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C275">
         <v>1</v>
@@ -4161,7 +4131,7 @@
         <v>87</v>
       </c>
       <c r="B276" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C276">
         <v>1</v>
@@ -4172,7 +4142,7 @@
         <v>88</v>
       </c>
       <c r="B277" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C277">
         <v>1</v>
@@ -4183,7 +4153,7 @@
         <v>89</v>
       </c>
       <c r="B278" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C278">
         <v>1</v>
@@ -4194,7 +4164,7 @@
         <v>91</v>
       </c>
       <c r="B279" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C279">
         <v>1</v>
@@ -4205,7 +4175,7 @@
         <v>92</v>
       </c>
       <c r="B280" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C280">
         <v>1</v>
@@ -4216,7 +4186,7 @@
         <v>93</v>
       </c>
       <c r="B281" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C281">
         <v>1</v>
@@ -4224,10 +4194,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B282" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C282">
         <v>1</v>
@@ -4238,7 +4208,7 @@
         <v>90</v>
       </c>
       <c r="B283" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C283">
         <v>1</v>
@@ -4249,7 +4219,7 @@
         <v>82</v>
       </c>
       <c r="B284" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C284">
         <v>1</v>
@@ -4260,7 +4230,7 @@
         <v>84</v>
       </c>
       <c r="B285" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C285">
         <v>1</v>
@@ -4271,7 +4241,7 @@
         <v>86</v>
       </c>
       <c r="B286" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C286">
         <v>1</v>
@@ -4282,7 +4252,7 @@
         <v>87</v>
       </c>
       <c r="B287" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C287">
         <v>1</v>
@@ -4293,7 +4263,7 @@
         <v>88</v>
       </c>
       <c r="B288" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C288">
         <v>1</v>
@@ -4304,7 +4274,7 @@
         <v>89</v>
       </c>
       <c r="B289" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -4315,7 +4285,7 @@
         <v>90</v>
       </c>
       <c r="B290" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C290">
         <v>1</v>
@@ -4326,7 +4296,7 @@
         <v>92</v>
       </c>
       <c r="B291" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C291">
         <v>1</v>
@@ -4337,7 +4307,7 @@
         <v>91</v>
       </c>
       <c r="B292" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C292">
         <v>1</v>
@@ -4348,7 +4318,7 @@
         <v>93</v>
       </c>
       <c r="B293" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C293">
         <v>1</v>
@@ -4359,7 +4329,7 @@
         <v>95</v>
       </c>
       <c r="B294" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C294">
         <v>1</v>
@@ -4370,7 +4340,7 @@
         <v>98</v>
       </c>
       <c r="B295" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C295">
         <v>1</v>
@@ -4381,7 +4351,7 @@
         <v>4</v>
       </c>
       <c r="B296" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C296">
         <v>1</v>
@@ -4392,7 +4362,7 @@
         <v>99</v>
       </c>
       <c r="B297" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C297">
         <v>1</v>
@@ -4403,7 +4373,7 @@
         <v>100</v>
       </c>
       <c r="B298" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C298">
         <v>1</v>
@@ -4414,7 +4384,7 @@
         <v>101</v>
       </c>
       <c r="B299" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C299">
         <v>1</v>
@@ -4425,7 +4395,7 @@
         <v>105</v>
       </c>
       <c r="B300" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C300">
         <v>1</v>
@@ -4436,7 +4406,7 @@
         <v>108</v>
       </c>
       <c r="B301" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C301">
         <v>1</v>
@@ -4447,7 +4417,7 @@
         <v>5</v>
       </c>
       <c r="B302" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C302">
         <v>1</v>
@@ -4458,7 +4428,7 @@
         <v>109</v>
       </c>
       <c r="B303" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C303">
         <v>1</v>
@@ -4469,7 +4439,7 @@
         <v>110</v>
       </c>
       <c r="B304" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C304">
         <v>1</v>
@@ -4480,7 +4450,7 @@
         <v>114</v>
       </c>
       <c r="B305" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C305">
         <v>1</v>
@@ -4491,7 +4461,7 @@
         <v>116</v>
       </c>
       <c r="B306" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C306">
         <v>1</v>
@@ -4502,7 +4472,7 @@
         <v>121</v>
       </c>
       <c r="B307" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C307">
         <v>1</v>
@@ -4513,7 +4483,7 @@
         <v>120</v>
       </c>
       <c r="B308" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C308">
         <v>1</v>
@@ -4524,7 +4494,7 @@
         <v>122</v>
       </c>
       <c r="B309" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C309">
         <v>1</v>
@@ -4535,7 +4505,7 @@
         <v>123</v>
       </c>
       <c r="B310" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C310">
         <v>1</v>
@@ -4543,10 +4513,10 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B311" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C311">
         <v>1</v>
@@ -4554,10 +4524,10 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B312" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C312">
         <v>1</v>
@@ -4565,10 +4535,10 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B313" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C313">
         <v>1</v>
@@ -4576,10 +4546,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B314" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C314">
         <v>1</v>
@@ -4587,10 +4557,10 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B315" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C315">
         <v>1</v>
@@ -4598,10 +4568,10 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B316" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C316">
         <v>1</v>
@@ -4609,10 +4579,10 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B317" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C317">
         <v>1</v>
@@ -4620,10 +4590,10 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B318" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C318">
         <v>1</v>
@@ -4631,10 +4601,10 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B319" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C319">
         <v>1</v>
@@ -4642,10 +4612,10 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B320" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C320">
         <v>1</v>
@@ -4653,10 +4623,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B321" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C321">
         <v>1</v>
@@ -4667,7 +4637,7 @@
         <v>6</v>
       </c>
       <c r="B322" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C322">
         <v>1</v>
@@ -4675,10 +4645,10 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B323" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C323">
         <v>1</v>
@@ -4686,10 +4656,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B324" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C324">
         <v>1</v>
@@ -4697,10 +4667,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B325" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C325">
         <v>1</v>
@@ -4708,10 +4678,10 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B326" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C326">
         <v>1</v>
@@ -4719,10 +4689,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B327" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C327">
         <v>1</v>
@@ -4730,10 +4700,10 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B328" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C328">
         <v>1</v>
@@ -4741,10 +4711,10 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B329" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C329">
         <v>1</v>
@@ -4755,7 +4725,7 @@
         <v>129</v>
       </c>
       <c r="B330" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C330">
         <v>1</v>
@@ -4763,10 +4733,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B331" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C331">
         <v>1</v>
@@ -4774,10 +4744,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B332" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C332">
         <v>1</v>
@@ -4788,7 +4758,7 @@
         <v>103</v>
       </c>
       <c r="B333" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C333">
         <v>1</v>
@@ -4799,7 +4769,7 @@
         <v>112</v>
       </c>
       <c r="B334" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C334">
         <v>1</v>
@@ -4807,10 +4777,10 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B335" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C335">
         <v>1</v>
@@ -4818,10 +4788,10 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B336" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C336">
         <v>1</v>
@@ -4829,10 +4799,10 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B337" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C337">
         <v>1</v>
@@ -4840,10 +4810,10 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B338" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C338">
         <v>1</v>
@@ -4851,10 +4821,10 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B339" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C339">
         <v>1</v>
@@ -4862,10 +4832,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B340" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C340">
         <v>1</v>
@@ -4873,10 +4843,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B341" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C341">
         <v>1</v>
@@ -4884,10 +4854,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B342" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C342">
         <v>1</v>
@@ -4895,10 +4865,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B343" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C343">
         <v>1</v>
@@ -4906,10 +4876,10 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B344" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C344">
         <v>1</v>
@@ -4920,7 +4890,7 @@
         <v>130</v>
       </c>
       <c r="B345" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C345">
         <v>1</v>
@@ -4931,7 +4901,7 @@
         <v>131</v>
       </c>
       <c r="B346" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C346">
         <v>1</v>
@@ -4942,7 +4912,7 @@
         <v>135</v>
       </c>
       <c r="B347" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C347">
         <v>1</v>
@@ -4953,7 +4923,7 @@
         <v>136</v>
       </c>
       <c r="B348" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C348">
         <v>1</v>
@@ -4964,7 +4934,7 @@
         <v>137</v>
       </c>
       <c r="B349" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C349">
         <v>1</v>
@@ -4975,7 +4945,7 @@
         <v>138</v>
       </c>
       <c r="B350" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C350">
         <v>1</v>
@@ -4986,7 +4956,7 @@
         <v>139</v>
       </c>
       <c r="B351" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C351">
         <v>1</v>
@@ -4997,7 +4967,7 @@
         <v>77</v>
       </c>
       <c r="B352" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C352">
         <v>1</v>
@@ -5008,7 +4978,7 @@
         <v>140</v>
       </c>
       <c r="B353" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C353">
         <v>1</v>
@@ -5019,7 +4989,7 @@
         <v>141</v>
       </c>
       <c r="B354" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C354">
         <v>1</v>
@@ -5030,7 +5000,7 @@
         <v>63</v>
       </c>
       <c r="B355" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C355">
         <v>1</v>
@@ -5041,7 +5011,7 @@
         <v>64</v>
       </c>
       <c r="B356" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C356">
         <v>1</v>
@@ -5052,7 +5022,7 @@
         <v>65</v>
       </c>
       <c r="B357" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C357">
         <v>1</v>
@@ -5063,7 +5033,7 @@
         <v>66</v>
       </c>
       <c r="B358" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C358">
         <v>1</v>
@@ -5074,7 +5044,7 @@
         <v>67</v>
       </c>
       <c r="B359" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C359">
         <v>1</v>
@@ -5085,7 +5055,7 @@
         <v>68</v>
       </c>
       <c r="B360" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C360">
         <v>1</v>
@@ -5096,7 +5066,7 @@
         <v>69</v>
       </c>
       <c r="B361" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C361">
         <v>1</v>
@@ -5107,7 +5077,7 @@
         <v>70</v>
       </c>
       <c r="B362" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C362">
         <v>1</v>
@@ -5118,7 +5088,7 @@
         <v>71</v>
       </c>
       <c r="B363" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C363">
         <v>1</v>
@@ -5129,7 +5099,7 @@
         <v>72</v>
       </c>
       <c r="B364" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C364">
         <v>1</v>
@@ -5140,7 +5110,7 @@
         <v>73</v>
       </c>
       <c r="B365" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C365">
         <v>1</v>
@@ -5151,7 +5121,7 @@
         <v>74</v>
       </c>
       <c r="B366" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C366">
         <v>1</v>
@@ -5162,7 +5132,7 @@
         <v>75</v>
       </c>
       <c r="B367" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C367">
         <v>1</v>
@@ -5173,7 +5143,7 @@
         <v>76</v>
       </c>
       <c r="B368" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C368">
         <v>1</v>
@@ -5184,7 +5154,7 @@
         <v>77</v>
       </c>
       <c r="B369" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C369">
         <v>1</v>
@@ -5195,7 +5165,7 @@
         <v>78</v>
       </c>
       <c r="B370" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C370">
         <v>1</v>
@@ -5203,10 +5173,10 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B371" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C371">
         <v>1</v>
@@ -5214,10 +5184,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B372" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C372">
         <v>1</v>
@@ -5225,10 +5195,10 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B373" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C373">
         <v>1</v>
@@ -5239,7 +5209,7 @@
         <v>94</v>
       </c>
       <c r="B374" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C374">
         <v>1</v>
@@ -5250,7 +5220,7 @@
         <v>96</v>
       </c>
       <c r="B375" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C375">
         <v>1</v>
@@ -5261,7 +5231,7 @@
         <v>97</v>
       </c>
       <c r="B376" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C376">
         <v>1</v>
@@ -5272,7 +5242,7 @@
         <v>102</v>
       </c>
       <c r="B377" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C377">
         <v>1</v>
@@ -5283,7 +5253,7 @@
         <v>104</v>
       </c>
       <c r="B378" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C378">
         <v>1</v>
@@ -5294,7 +5264,7 @@
         <v>106</v>
       </c>
       <c r="B379" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C379">
         <v>1</v>
@@ -5305,7 +5275,7 @@
         <v>107</v>
       </c>
       <c r="B380" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C380">
         <v>1</v>
@@ -5316,7 +5286,7 @@
         <v>111</v>
       </c>
       <c r="B381" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C381">
         <v>1</v>
@@ -5327,7 +5297,7 @@
         <v>113</v>
       </c>
       <c r="B382" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C382">
         <v>1</v>
@@ -5338,7 +5308,7 @@
         <v>115</v>
       </c>
       <c r="B383" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C383">
         <v>1</v>
@@ -5349,7 +5319,7 @@
         <v>117</v>
       </c>
       <c r="B384" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C384">
         <v>1</v>
@@ -5360,7 +5330,7 @@
         <v>118</v>
       </c>
       <c r="B385" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C385">
         <v>1</v>
@@ -5371,7 +5341,7 @@
         <v>132</v>
       </c>
       <c r="B386" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C386">
         <v>1</v>
@@ -5382,7 +5352,7 @@
         <v>133</v>
       </c>
       <c r="B387" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C387">
         <v>1</v>
@@ -5393,7 +5363,7 @@
         <v>142</v>
       </c>
       <c r="B388" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C388">
         <v>1</v>
@@ -5401,10 +5371,10 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B389" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C389">
         <v>1</v>
@@ -5412,10 +5382,10 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B390" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C390">
         <v>1</v>
@@ -5423,10 +5393,10 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B391" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C391">
         <v>1</v>
@@ -5434,10 +5404,10 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B392" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C392">
         <v>1</v>
@@ -5445,10 +5415,10 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B393" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C393">
         <v>1</v>
@@ -5456,10 +5426,10 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B394" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C394">
         <v>1</v>
@@ -5467,10 +5437,10 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B395" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C395">
         <v>1</v>
@@ -5478,10 +5448,10 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B396" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C396">
         <v>1</v>
@@ -5489,10 +5459,10 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B397" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C397">
         <v>1</v>
@@ -5500,10 +5470,10 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B398" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C398">
         <v>1</v>
@@ -5511,10 +5481,10 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B399" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C399">
         <v>1</v>
@@ -5525,7 +5495,7 @@
         <v>6</v>
       </c>
       <c r="B400" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C400">
         <v>1</v>
@@ -5533,10 +5503,10 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B401" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C401">
         <v>1</v>
@@ -5544,10 +5514,10 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B402" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C402">
         <v>1</v>
@@ -5555,10 +5525,10 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B403" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C403">
         <v>1</v>
@@ -5566,10 +5536,10 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B404" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -5577,10 +5547,10 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B405" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C405">
         <v>1</v>
@@ -5588,10 +5558,10 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B406" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C406">
         <v>1</v>
@@ -5599,10 +5569,10 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B407" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C407">
         <v>1</v>
@@ -5610,10 +5580,10 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B408" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C408">
         <v>1</v>
@@ -5621,10 +5591,10 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B409" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C409">
         <v>1</v>
@@ -5632,10 +5602,10 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B410" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C410">
         <v>1</v>
@@ -5643,10 +5613,10 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B411" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C411">
         <v>1</v>
@@ -5654,10 +5624,10 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B412" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C412">
         <v>1</v>
@@ -5665,10 +5635,10 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B413" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C413">
         <v>1</v>
@@ -5676,10 +5646,10 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B414" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C414">
         <v>1</v>
@@ -5690,7 +5660,7 @@
         <v>130</v>
       </c>
       <c r="B415" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C415">
         <v>1</v>
@@ -5698,10 +5668,10 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B416" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C416">
         <v>1</v>
@@ -5709,10 +5679,10 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B417" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C417">
         <v>1</v>
@@ -5720,10 +5690,10 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B418" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C418">
         <v>1</v>
@@ -5731,10 +5701,10 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>220</v>
+        <v>81</v>
       </c>
       <c r="B419" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C419">
         <v>1</v>
@@ -5742,10 +5712,10 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>221</v>
+        <v>82</v>
       </c>
       <c r="B420" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C420">
         <v>1</v>
@@ -5753,10 +5723,10 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="B421" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C421">
         <v>1</v>
@@ -5764,10 +5734,10 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="B422" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C422">
         <v>1</v>
@@ -5775,10 +5745,10 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="B423" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C423">
         <v>1</v>
@@ -5786,10 +5756,10 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="B424" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C424">
         <v>1</v>
@@ -5797,10 +5767,10 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B425" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C425">
         <v>1</v>
@@ -5808,10 +5778,10 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B426" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C426">
         <v>1</v>
@@ -5819,10 +5789,10 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="B427" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C427">
         <v>1</v>
@@ -5830,7 +5800,7 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>107</v>
+        <v>232</v>
       </c>
       <c r="B428" t="s">
         <v>231</v>
@@ -5841,7 +5811,7 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
-        <v>115</v>
+        <v>233</v>
       </c>
       <c r="B429" t="s">
         <v>231</v>
@@ -5852,10 +5822,10 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>118</v>
+        <v>235</v>
       </c>
       <c r="B430" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C430">
         <v>1</v>
@@ -5863,10 +5833,10 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>124</v>
+        <v>236</v>
       </c>
       <c r="B431" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C431">
         <v>1</v>
@@ -5874,10 +5844,10 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>127</v>
+        <v>237</v>
       </c>
       <c r="B432" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C432">
         <v>1</v>
@@ -5885,10 +5855,10 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
       <c r="B433" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C433">
         <v>1</v>
@@ -5896,10 +5866,10 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
-        <v>165</v>
+        <v>239</v>
       </c>
       <c r="B434" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C434">
         <v>1</v>
@@ -5907,10 +5877,10 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
-        <v>132</v>
+        <v>240</v>
       </c>
       <c r="B435" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C435">
         <v>1</v>
@@ -5918,10 +5888,10 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="B436" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C436">
         <v>1</v>
@@ -5929,10 +5899,10 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="B437" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C437">
         <v>1</v>
@@ -5940,10 +5910,10 @@
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="B438" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C438">
         <v>1</v>
@@ -5951,10 +5921,10 @@
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="B439" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C439">
         <v>1</v>
@@ -5962,10 +5932,10 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="B440" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C440">
         <v>1</v>
@@ -5973,10 +5943,10 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
-        <v>161</v>
+        <v>4</v>
       </c>
       <c r="B441" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="C441">
         <v>1</v>
@@ -5984,10 +5954,10 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B442" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="C442">
         <v>1</v>
@@ -5995,10 +5965,10 @@
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B443" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="C443">
         <v>1</v>
@@ -6006,782 +5976,12 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
-        <v>165</v>
+        <v>102</v>
       </c>
       <c r="B444" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="C444">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A445" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B445" t="s">
-        <v>232</v>
-      </c>
-      <c r="C445">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A446" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B446" t="s">
-        <v>232</v>
-      </c>
-      <c r="C446">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A447" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B447" t="s">
-        <v>232</v>
-      </c>
-      <c r="C447">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A448" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B448" t="s">
-        <v>232</v>
-      </c>
-      <c r="C448">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A449" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B449" t="s">
-        <v>232</v>
-      </c>
-      <c r="C449">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A450" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B450" t="s">
-        <v>232</v>
-      </c>
-      <c r="C450">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A451" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B451" t="s">
-        <v>232</v>
-      </c>
-      <c r="C451">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A452" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B452" t="s">
-        <v>232</v>
-      </c>
-      <c r="C452">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A453" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B453" t="s">
-        <v>232</v>
-      </c>
-      <c r="C453">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A454" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B454" t="s">
-        <v>232</v>
-      </c>
-      <c r="C454">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A455" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B455" t="s">
-        <v>232</v>
-      </c>
-      <c r="C455">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A456" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B456" t="s">
-        <v>232</v>
-      </c>
-      <c r="C456">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A457" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B457" t="s">
-        <v>232</v>
-      </c>
-      <c r="C457">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A458" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B458" t="s">
-        <v>232</v>
-      </c>
-      <c r="C458">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A459" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B459" t="s">
-        <v>232</v>
-      </c>
-      <c r="C459">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A460" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B460" t="s">
-        <v>233</v>
-      </c>
-      <c r="C460">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A461" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B461" t="s">
-        <v>233</v>
-      </c>
-      <c r="C461">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A462" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B462" t="s">
-        <v>233</v>
-      </c>
-      <c r="C462">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A463" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B463" t="s">
-        <v>233</v>
-      </c>
-      <c r="C463">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A464" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B464" t="s">
-        <v>233</v>
-      </c>
-      <c r="C464">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A465" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B465" t="s">
-        <v>233</v>
-      </c>
-      <c r="C465">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A466" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B466" t="s">
-        <v>233</v>
-      </c>
-      <c r="C466">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A467" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B467" t="s">
-        <v>233</v>
-      </c>
-      <c r="C467">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A468" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B468" t="s">
-        <v>233</v>
-      </c>
-      <c r="C468">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A469" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B469" t="s">
-        <v>239</v>
-      </c>
-      <c r="C469">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A470" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B470" t="s">
-        <v>239</v>
-      </c>
-      <c r="C470">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A471" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B471" t="s">
-        <v>239</v>
-      </c>
-      <c r="C471">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A472" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B472" t="s">
-        <v>239</v>
-      </c>
-      <c r="C472">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A473" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B473" t="s">
-        <v>239</v>
-      </c>
-      <c r="C473">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A474" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B474" t="s">
-        <v>239</v>
-      </c>
-      <c r="C474">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A475" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B475" t="s">
-        <v>239</v>
-      </c>
-      <c r="C475">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A476" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B476" t="s">
-        <v>239</v>
-      </c>
-      <c r="C476">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A477" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B477" t="s">
-        <v>239</v>
-      </c>
-      <c r="C477">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A478" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B478" t="s">
-        <v>239</v>
-      </c>
-      <c r="C478">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A479" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B479" t="s">
-        <v>240</v>
-      </c>
-      <c r="C479">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A480" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B480" t="s">
-        <v>240</v>
-      </c>
-      <c r="C480">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A481" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B481" t="s">
-        <v>240</v>
-      </c>
-      <c r="C481">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A482" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B482" t="s">
-        <v>240</v>
-      </c>
-      <c r="C482">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A483" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B483" t="s">
-        <v>240</v>
-      </c>
-      <c r="C483">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A484" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B484" t="s">
-        <v>240</v>
-      </c>
-      <c r="C484">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A485" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B485" t="s">
-        <v>240</v>
-      </c>
-      <c r="C485">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A486" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B486" t="s">
-        <v>240</v>
-      </c>
-      <c r="C486">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A487" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B487" t="s">
-        <v>240</v>
-      </c>
-      <c r="C487">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A488" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B488" t="s">
-        <v>240</v>
-      </c>
-      <c r="C488">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A489" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B489" t="s">
-        <v>240</v>
-      </c>
-      <c r="C489">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A490" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B490" t="s">
-        <v>240</v>
-      </c>
-      <c r="C490">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A491" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B491" t="s">
-        <v>240</v>
-      </c>
-      <c r="C491">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A492" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B492" t="s">
-        <v>240</v>
-      </c>
-      <c r="C492">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A493" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B493" t="s">
-        <v>240</v>
-      </c>
-      <c r="C493">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A494" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B494" t="s">
-        <v>240</v>
-      </c>
-      <c r="C494">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A495" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B495" t="s">
-        <v>240</v>
-      </c>
-      <c r="C495">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A496" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B496" t="s">
-        <v>240</v>
-      </c>
-      <c r="C496">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A497" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B497" t="s">
-        <v>240</v>
-      </c>
-      <c r="C497">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A498" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B498" t="s">
-        <v>241</v>
-      </c>
-      <c r="C498">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A499" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B499" t="s">
-        <v>241</v>
-      </c>
-      <c r="C499">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A500" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B500" t="s">
-        <v>244</v>
-      </c>
-      <c r="C500">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A501" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B501" t="s">
-        <v>244</v>
-      </c>
-      <c r="C501">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A502" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B502" t="s">
-        <v>244</v>
-      </c>
-      <c r="C502">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A503" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B503" t="s">
-        <v>244</v>
-      </c>
-      <c r="C503">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A504" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B504" t="s">
-        <v>244</v>
-      </c>
-      <c r="C504">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A505" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B505" t="s">
-        <v>244</v>
-      </c>
-      <c r="C505">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A506" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B506" t="s">
-        <v>251</v>
-      </c>
-      <c r="C506">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A507" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B507" t="s">
-        <v>251</v>
-      </c>
-      <c r="C507">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A508" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B508" t="s">
-        <v>251</v>
-      </c>
-      <c r="C508">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A509" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B509" t="s">
-        <v>251</v>
-      </c>
-      <c r="C509">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A510" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B510" t="s">
-        <v>251</v>
-      </c>
-      <c r="C510">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A511" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B511" t="s">
-        <v>251</v>
-      </c>
-      <c r="C511">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A512" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B512" t="s">
-        <v>251</v>
-      </c>
-      <c r="C512">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A513" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B513" t="s">
-        <v>251</v>
-      </c>
-      <c r="C513">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A514" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B514" t="s">
-        <v>251</v>
-      </c>
-      <c r="C514">
         <v>1</v>
       </c>
     </row>
@@ -6793,10 +5993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1479B4DB-1D01-41F4-A419-27AD6B416698}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6807,7 +6007,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -6818,10 +6018,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6829,10 +6029,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6840,10 +6040,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6851,32 +6051,32 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>156</v>
+        <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>157</v>
+      <c r="A6" t="s">
+        <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>195</v>
+      <c r="A7" t="s">
+        <v>223</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6884,10 +6084,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6895,10 +6095,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>157</v>
+        <v>227</v>
       </c>
       <c r="B9" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6906,78 +6106,23 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>227</v>
+      <c r="A11" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>228</v>
-      </c>
-      <c r="B12" t="s">
-        <v>225</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B13" t="s">
-        <v>238</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B14" t="s">
-        <v>238</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B15" t="s">
-        <v>238</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B16" t="s">
-        <v>238</v>
-      </c>
-      <c r="C16">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replaced X_SMR_CCS with X_ATR_CCS in Tag_Subsets
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimitrip\GENeSYS-MOD\GENeSYS_MOD.data\Output\output_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C989F4-EB7B-4974-A6FC-DD186AC9E345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753B6B18-2BF4-4C7F-86C8-9E9BAEDC0DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5625" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_TagTechnologyToSubsets" sheetId="1" r:id="rId1"/>
@@ -234,9 +234,6 @@
     <t>X_SMR</t>
   </si>
   <si>
-    <t>X_SMR_CCS</t>
-  </si>
-  <si>
     <t>P_H2_OCGT</t>
   </si>
   <si>
@@ -553,6 +550,9 @@
   </si>
   <si>
     <t>RES_Ocean</t>
+  </si>
+  <si>
+    <t>X_ATR_CCS</t>
   </si>
 </sst>
 </file>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
-      <selection activeCell="E421" sqref="E421"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +915,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
         <v>15</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
         <v>15</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="B68" t="s">
         <v>15</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
         <v>15</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
         <v>15</v>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
         <v>15</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
         <v>15</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>15</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
         <v>16</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77" t="s">
         <v>16</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" t="s">
         <v>16</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B80" t="s">
         <v>16</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" t="s">
         <v>16</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B82" t="s">
         <v>16</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B83" t="s">
         <v>16</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B84" t="s">
         <v>16</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
         <v>16</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B87" t="s">
         <v>16</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
         <v>16</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B133" t="s">
         <v>16</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B136" t="s">
         <v>16</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="B140" t="s">
         <v>16</v>
@@ -2433,10 +2433,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B141" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -2444,10 +2444,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -2455,10 +2455,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B143" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -2466,10 +2466,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B144" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -2477,10 +2477,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B145" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -2488,10 +2488,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B146" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -2499,10 +2499,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B147" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -2510,10 +2510,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B148" t="s">
         <v>85</v>
-      </c>
-      <c r="B148" t="s">
-        <v>86</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -2521,10 +2521,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B149" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -2532,10 +2532,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B150" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -2543,10 +2543,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B151" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -2554,10 +2554,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B152" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -2565,10 +2565,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B153" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -2576,10 +2576,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B154" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -2587,10 +2587,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B155" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -2598,10 +2598,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B156" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -2609,10 +2609,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B157" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -2620,10 +2620,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B158" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -2631,10 +2631,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B159" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -2642,10 +2642,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B160" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -2653,10 +2653,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B161" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -2664,10 +2664,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B162" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -2675,10 +2675,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B163" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -2689,7 +2689,7 @@
         <v>14</v>
       </c>
       <c r="B164" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -2697,10 +2697,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B165" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B166" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C166">
         <v>1</v>
@@ -2719,10 +2719,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B167" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -2730,10 +2730,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B168" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C168">
         <v>1</v>
@@ -2741,10 +2741,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B169" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -2752,10 +2752,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B170" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -2763,10 +2763,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B171" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B172" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -2785,10 +2785,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B173" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -2796,10 +2796,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B174" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C174">
         <v>1</v>
@@ -2810,7 +2810,7 @@
         <v>14</v>
       </c>
       <c r="B175" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -2818,10 +2818,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B176" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -2829,10 +2829,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B177" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -2840,10 +2840,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B178" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -2851,10 +2851,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B179" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -2862,10 +2862,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B180" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -2873,10 +2873,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B181" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -2884,10 +2884,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B182" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -2895,10 +2895,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B183" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -2906,10 +2906,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B184" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -2917,10 +2917,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B185" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -2928,10 +2928,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B186" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -2939,10 +2939,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B187" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -2950,10 +2950,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B188" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -2961,10 +2961,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B189" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C189">
         <v>1</v>
@@ -2972,10 +2972,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B190" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -2983,10 +2983,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B191" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C191">
         <v>1</v>
@@ -2994,10 +2994,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B192" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C192">
         <v>1</v>
@@ -3005,10 +3005,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B193" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -3016,10 +3016,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B194" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -3027,10 +3027,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B195" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C195">
         <v>1</v>
@@ -3038,10 +3038,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B196" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C196">
         <v>1</v>
@@ -3049,10 +3049,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B197" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B198" t="s">
         <v>114</v>
-      </c>
-      <c r="B198" t="s">
-        <v>115</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -3071,10 +3071,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B199" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -3082,10 +3082,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B200" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -3093,10 +3093,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B201" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -3104,10 +3104,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B202" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -3115,10 +3115,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B203" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C203">
         <v>1</v>
@@ -3126,10 +3126,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B204" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -3137,10 +3137,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B205" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B206" t="s">
         <v>121</v>
-      </c>
-      <c r="B206" t="s">
-        <v>122</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -3159,10 +3159,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B207" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B208" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B209" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C209">
         <v>1</v>
@@ -3192,10 +3192,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B210" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -3203,10 +3203,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B211" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -3214,10 +3214,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B212" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C212">
         <v>1</v>
@@ -3225,10 +3225,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B213" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C213">
         <v>1</v>
@@ -3236,10 +3236,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B214" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C214">
         <v>1</v>
@@ -3247,10 +3247,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B215" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -3258,10 +3258,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B216" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -3272,7 +3272,7 @@
         <v>29</v>
       </c>
       <c r="B217" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C217">
         <v>1</v>
@@ -3283,7 +3283,7 @@
         <v>30</v>
       </c>
       <c r="B218" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C218">
         <v>1</v>
@@ -3294,7 +3294,7 @@
         <v>31</v>
       </c>
       <c r="B219" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -3305,7 +3305,7 @@
         <v>32</v>
       </c>
       <c r="B220" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -3316,7 +3316,7 @@
         <v>33</v>
       </c>
       <c r="B221" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -3327,7 +3327,7 @@
         <v>4</v>
       </c>
       <c r="B222" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -3338,7 +3338,7 @@
         <v>34</v>
       </c>
       <c r="B223" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -3349,7 +3349,7 @@
         <v>35</v>
       </c>
       <c r="B224" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -3360,7 +3360,7 @@
         <v>36</v>
       </c>
       <c r="B225" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -3371,7 +3371,7 @@
         <v>37</v>
       </c>
       <c r="B226" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -3382,7 +3382,7 @@
         <v>39</v>
       </c>
       <c r="B227" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -3393,7 +3393,7 @@
         <v>40</v>
       </c>
       <c r="B228" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -3404,7 +3404,7 @@
         <v>41</v>
       </c>
       <c r="B229" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -3415,7 +3415,7 @@
         <v>42</v>
       </c>
       <c r="B230" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -3426,7 +3426,7 @@
         <v>43</v>
       </c>
       <c r="B231" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C231">
         <v>1</v>
@@ -3437,7 +3437,7 @@
         <v>5</v>
       </c>
       <c r="B232" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C232">
         <v>1</v>
@@ -3448,7 +3448,7 @@
         <v>44</v>
       </c>
       <c r="B233" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C233">
         <v>1</v>
@@ -3459,7 +3459,7 @@
         <v>45</v>
       </c>
       <c r="B234" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C234">
         <v>1</v>
@@ -3470,7 +3470,7 @@
         <v>46</v>
       </c>
       <c r="B235" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C235">
         <v>1</v>
@@ -3481,7 +3481,7 @@
         <v>48</v>
       </c>
       <c r="B236" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C236">
         <v>1</v>
@@ -3492,7 +3492,7 @@
         <v>49</v>
       </c>
       <c r="B237" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C237">
         <v>1</v>
@@ -3503,7 +3503,7 @@
         <v>50</v>
       </c>
       <c r="B238" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C238">
         <v>1</v>
@@ -3514,7 +3514,7 @@
         <v>51</v>
       </c>
       <c r="B239" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C239">
         <v>1</v>
@@ -3525,7 +3525,7 @@
         <v>52</v>
       </c>
       <c r="B240" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C240">
         <v>1</v>
@@ -3536,7 +3536,7 @@
         <v>53</v>
       </c>
       <c r="B241" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C241">
         <v>1</v>
@@ -3547,7 +3547,7 @@
         <v>54</v>
       </c>
       <c r="B242" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C242">
         <v>1</v>
@@ -3558,7 +3558,7 @@
         <v>55</v>
       </c>
       <c r="B243" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -3569,7 +3569,7 @@
         <v>56</v>
       </c>
       <c r="B244" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -3580,7 +3580,7 @@
         <v>57</v>
       </c>
       <c r="B245" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C245">
         <v>1</v>
@@ -3591,7 +3591,7 @@
         <v>58</v>
       </c>
       <c r="B246" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -3602,7 +3602,7 @@
         <v>59</v>
       </c>
       <c r="B247" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         <v>60</v>
       </c>
       <c r="B248" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -3624,7 +3624,7 @@
         <v>61</v>
       </c>
       <c r="B249" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -3635,7 +3635,7 @@
         <v>62</v>
       </c>
       <c r="B250" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -3646,7 +3646,7 @@
         <v>38</v>
       </c>
       <c r="B251" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -3657,7 +3657,7 @@
         <v>47</v>
       </c>
       <c r="B252" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -3665,10 +3665,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B253" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -3676,10 +3676,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B254" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C254">
         <v>1</v>
@@ -3687,10 +3687,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B255" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -3698,10 +3698,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B256" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -3709,10 +3709,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B257" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -3720,10 +3720,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B258" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -3731,10 +3731,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B259" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C259">
         <v>1</v>
@@ -3742,10 +3742,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B260" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C260">
         <v>1</v>
@@ -3753,10 +3753,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B261" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -3767,7 +3767,7 @@
         <v>14</v>
       </c>
       <c r="B262" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C262">
         <v>1</v>
@@ -3775,10 +3775,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B263" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C263">
         <v>1</v>
@@ -3786,10 +3786,10 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B264" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C264">
         <v>1</v>
@@ -3797,10 +3797,10 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B265" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C265">
         <v>1</v>
@@ -3808,10 +3808,10 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B266" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C266">
         <v>1</v>
@@ -3819,10 +3819,10 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B267" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C267">
         <v>1</v>
@@ -3830,10 +3830,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B268" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C268">
         <v>1</v>
@@ -3841,10 +3841,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B269" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -3852,10 +3852,10 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B270" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C270">
         <v>1</v>
@@ -3863,10 +3863,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B271" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C271">
         <v>1</v>
@@ -3874,10 +3874,10 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B272" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C272">
         <v>1</v>
@@ -3888,7 +3888,7 @@
         <v>21</v>
       </c>
       <c r="B273" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C273">
         <v>1</v>
@@ -3899,7 +3899,7 @@
         <v>22</v>
       </c>
       <c r="B274" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C274">
         <v>1</v>
@@ -3910,7 +3910,7 @@
         <v>23</v>
       </c>
       <c r="B275" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C275">
         <v>1</v>
@@ -3921,7 +3921,7 @@
         <v>24</v>
       </c>
       <c r="B276" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C276">
         <v>1</v>
@@ -3932,7 +3932,7 @@
         <v>26</v>
       </c>
       <c r="B277" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C277">
         <v>1</v>
@@ -3943,7 +3943,7 @@
         <v>27</v>
       </c>
       <c r="B278" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C278">
         <v>1</v>
@@ -3954,7 +3954,7 @@
         <v>28</v>
       </c>
       <c r="B279" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C279">
         <v>1</v>
@@ -3962,10 +3962,10 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B280" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C280">
         <v>1</v>
@@ -3976,7 +3976,7 @@
         <v>25</v>
       </c>
       <c r="B281" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C281">
         <v>1</v>
@@ -3984,10 +3984,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B282" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C282">
         <v>1</v>
@@ -3995,10 +3995,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B283" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C283">
         <v>1</v>
@@ -4006,10 +4006,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B284" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C284">
         <v>1</v>
@@ -4017,10 +4017,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B285" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C285">
         <v>1</v>
@@ -4028,10 +4028,10 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B286" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C286">
         <v>1</v>
@@ -4039,10 +4039,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B287" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C287">
         <v>1</v>
@@ -4053,7 +4053,7 @@
         <v>14</v>
       </c>
       <c r="B288" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C288">
         <v>1</v>
@@ -4061,10 +4061,10 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B289" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -4072,10 +4072,10 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B290" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C290">
         <v>1</v>
@@ -4086,7 +4086,7 @@
         <v>21</v>
       </c>
       <c r="B291" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C291">
         <v>1</v>
@@ -4097,7 +4097,7 @@
         <v>22</v>
       </c>
       <c r="B292" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C292">
         <v>1</v>
@@ -4108,7 +4108,7 @@
         <v>25</v>
       </c>
       <c r="B293" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C293">
         <v>1</v>
@@ -4119,7 +4119,7 @@
         <v>24</v>
       </c>
       <c r="B294" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C294">
         <v>1</v>
@@ -4130,7 +4130,7 @@
         <v>23</v>
       </c>
       <c r="B295" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C295">
         <v>1</v>
@@ -4141,7 +4141,7 @@
         <v>26</v>
       </c>
       <c r="B296" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C296">
         <v>1</v>
@@ -4152,7 +4152,7 @@
         <v>27</v>
       </c>
       <c r="B297" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C297">
         <v>1</v>
@@ -4163,7 +4163,7 @@
         <v>28</v>
       </c>
       <c r="B298" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C298">
         <v>1</v>
@@ -4171,10 +4171,10 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B299" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C299">
         <v>1</v>
@@ -4182,10 +4182,10 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B300" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C300">
         <v>1</v>
@@ -4193,10 +4193,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B301" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C301">
         <v>1</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B302" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C302">
         <v>1</v>
@@ -4215,10 +4215,10 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B303" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C303">
         <v>1</v>
@@ -4229,7 +4229,7 @@
         <v>59</v>
       </c>
       <c r="B304" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C304">
         <v>1</v>
@@ -4240,7 +4240,7 @@
         <v>58</v>
       </c>
       <c r="B305" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C305">
         <v>1</v>
@@ -4251,7 +4251,7 @@
         <v>60</v>
       </c>
       <c r="B306" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C306">
         <v>1</v>
@@ -4262,7 +4262,7 @@
         <v>56</v>
       </c>
       <c r="B307" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C307">
         <v>1</v>
@@ -4273,7 +4273,7 @@
         <v>57</v>
       </c>
       <c r="B308" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C308">
         <v>1</v>
@@ -4284,7 +4284,7 @@
         <v>55</v>
       </c>
       <c r="B309" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C309">
         <v>1</v>
@@ -4295,7 +4295,7 @@
         <v>40</v>
       </c>
       <c r="B310" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C310">
         <v>1</v>
@@ -4306,7 +4306,7 @@
         <v>43</v>
       </c>
       <c r="B311" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C311">
         <v>1</v>
@@ -4317,7 +4317,7 @@
         <v>44</v>
       </c>
       <c r="B312" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C312">
         <v>1</v>
@@ -4328,7 +4328,7 @@
         <v>45</v>
       </c>
       <c r="B313" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C313">
         <v>1</v>
@@ -4339,7 +4339,7 @@
         <v>47</v>
       </c>
       <c r="B314" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C314">
         <v>1</v>
@@ -4350,7 +4350,7 @@
         <v>5</v>
       </c>
       <c r="B315" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C315">
         <v>1</v>
@@ -4361,7 +4361,7 @@
         <v>30</v>
       </c>
       <c r="B316" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C316">
         <v>1</v>
@@ -4372,7 +4372,7 @@
         <v>33</v>
       </c>
       <c r="B317" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C317">
         <v>1</v>
@@ -4383,7 +4383,7 @@
         <v>36</v>
       </c>
       <c r="B318" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C318">
         <v>1</v>
@@ -4394,7 +4394,7 @@
         <v>38</v>
       </c>
       <c r="B319" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C319">
         <v>1</v>
@@ -4405,7 +4405,7 @@
         <v>34</v>
       </c>
       <c r="B320" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C320">
         <v>1</v>
@@ -4416,7 +4416,7 @@
         <v>35</v>
       </c>
       <c r="B321" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C321">
         <v>1</v>
@@ -4427,7 +4427,7 @@
         <v>4</v>
       </c>
       <c r="B322" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C322">
         <v>1</v>
@@ -4438,7 +4438,7 @@
         <v>49</v>
       </c>
       <c r="B323" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C323">
         <v>1</v>
@@ -4449,7 +4449,7 @@
         <v>61</v>
       </c>
       <c r="B324" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C324">
         <v>1</v>
@@ -4460,7 +4460,7 @@
         <v>62</v>
       </c>
       <c r="B325" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C325">
         <v>1</v>
@@ -4471,7 +4471,7 @@
         <v>51</v>
       </c>
       <c r="B326" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C326">
         <v>1</v>
@@ -4479,10 +4479,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B327" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C327">
         <v>1</v>
@@ -4490,10 +4490,10 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B328" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C328">
         <v>1</v>
@@ -4501,10 +4501,10 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B329" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C329">
         <v>1</v>
@@ -4512,10 +4512,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B330" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C330">
         <v>1</v>
@@ -4523,10 +4523,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B331" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C331">
         <v>1</v>
@@ -4534,10 +4534,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B332" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C332">
         <v>1</v>
@@ -4545,10 +4545,10 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B333" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C333">
         <v>1</v>
@@ -4556,10 +4556,10 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B334" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C334">
         <v>1</v>
@@ -4567,10 +4567,10 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B335" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C335">
         <v>1</v>
@@ -4578,10 +4578,10 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B336" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C336">
         <v>1</v>
@@ -4589,10 +4589,10 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B337" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C337">
         <v>1</v>
@@ -4603,7 +4603,7 @@
         <v>8</v>
       </c>
       <c r="B338" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C338">
         <v>1</v>
@@ -4611,10 +4611,10 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B339" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C339">
         <v>1</v>
@@ -4622,10 +4622,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B340" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C340">
         <v>1</v>
@@ -4633,10 +4633,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B341" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C341">
         <v>1</v>
@@ -4644,10 +4644,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B342" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C342">
         <v>1</v>
@@ -4655,10 +4655,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B343" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C343">
         <v>1</v>
@@ -4669,7 +4669,7 @@
         <v>7</v>
       </c>
       <c r="B344" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C344">
         <v>1</v>
@@ -4677,10 +4677,10 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B345" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C345">
         <v>1</v>
@@ -4688,10 +4688,10 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B346" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C346">
         <v>1</v>
@@ -4699,10 +4699,10 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B347" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C347">
         <v>1</v>
@@ -4713,7 +4713,7 @@
         <v>6</v>
       </c>
       <c r="B348" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C348">
         <v>1</v>
@@ -4724,7 +4724,7 @@
         <v>10</v>
       </c>
       <c r="B349" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C349">
         <v>1</v>
@@ -4735,7 +4735,7 @@
         <v>11</v>
       </c>
       <c r="B350" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C350">
         <v>1</v>
@@ -4746,7 +4746,7 @@
         <v>12</v>
       </c>
       <c r="B351" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C351">
         <v>1</v>
@@ -4754,10 +4754,10 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B352" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C352">
         <v>1</v>
@@ -4765,10 +4765,10 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B353" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C353">
         <v>1</v>
@@ -4776,10 +4776,10 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B354" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C354">
         <v>1</v>
@@ -4790,7 +4790,7 @@
         <v>19</v>
       </c>
       <c r="B355" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C355">
         <v>1</v>
@@ -4798,10 +4798,10 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B356" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C356">
         <v>1</v>
@@ -4809,10 +4809,10 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B357" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C357">
         <v>1</v>
@@ -4823,7 +4823,7 @@
         <v>17</v>
       </c>
       <c r="B358" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C358">
         <v>1</v>
@@ -4831,10 +4831,10 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="B359" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C359">
         <v>1</v>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B360" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C360">
         <v>1</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B361" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C361">
         <v>1</v>
@@ -4864,10 +4864,10 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B362" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C362">
         <v>1</v>
@@ -4878,7 +4878,7 @@
         <v>29</v>
       </c>
       <c r="B363" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C363">
         <v>1</v>
@@ -4889,7 +4889,7 @@
         <v>31</v>
       </c>
       <c r="B364" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C364">
         <v>1</v>
@@ -4900,7 +4900,7 @@
         <v>32</v>
       </c>
       <c r="B365" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C365">
         <v>1</v>
@@ -4911,7 +4911,7 @@
         <v>37</v>
       </c>
       <c r="B366" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C366">
         <v>1</v>
@@ -4922,7 +4922,7 @@
         <v>39</v>
       </c>
       <c r="B367" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C367">
         <v>1</v>
@@ -4933,7 +4933,7 @@
         <v>41</v>
       </c>
       <c r="B368" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C368">
         <v>1</v>
@@ -4944,7 +4944,7 @@
         <v>42</v>
       </c>
       <c r="B369" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C369">
         <v>1</v>
@@ -4955,7 +4955,7 @@
         <v>46</v>
       </c>
       <c r="B370" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C370">
         <v>1</v>
@@ -4966,7 +4966,7 @@
         <v>48</v>
       </c>
       <c r="B371" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C371">
         <v>1</v>
@@ -4977,7 +4977,7 @@
         <v>50</v>
       </c>
       <c r="B372" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C372">
         <v>1</v>
@@ -4988,7 +4988,7 @@
         <v>52</v>
       </c>
       <c r="B373" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C373">
         <v>1</v>
@@ -4999,7 +4999,7 @@
         <v>53</v>
       </c>
       <c r="B374" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C374">
         <v>1</v>
@@ -5007,10 +5007,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B375" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C375">
         <v>1</v>
@@ -5018,10 +5018,10 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B376" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C376">
         <v>1</v>
@@ -5029,10 +5029,10 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B377" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C377">
         <v>1</v>
@@ -5043,7 +5043,7 @@
         <v>10</v>
       </c>
       <c r="B378" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C378">
         <v>1</v>
@@ -5054,7 +5054,7 @@
         <v>11</v>
       </c>
       <c r="B379" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C379">
         <v>1</v>
@@ -5065,7 +5065,7 @@
         <v>12</v>
       </c>
       <c r="B380" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C380">
         <v>1</v>
@@ -5073,10 +5073,10 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B381" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C381">
         <v>1</v>
@@ -5084,10 +5084,10 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B382" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C382">
         <v>1</v>
@@ -5095,10 +5095,10 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B383" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C383">
         <v>1</v>
@@ -5109,7 +5109,7 @@
         <v>7</v>
       </c>
       <c r="B384" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C384">
         <v>1</v>
@@ -5117,10 +5117,10 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B385" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C385">
         <v>1</v>
@@ -5128,10 +5128,10 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B386" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C386">
         <v>1</v>
@@ -5139,10 +5139,10 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B387" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C387">
         <v>1</v>
@@ -5150,10 +5150,10 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B388" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C388">
         <v>1</v>
@@ -5164,7 +5164,7 @@
         <v>6</v>
       </c>
       <c r="B389" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C389">
         <v>1</v>
@@ -5175,7 +5175,7 @@
         <v>8</v>
       </c>
       <c r="B390" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C390">
         <v>1</v>
@@ -5183,10 +5183,10 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B391" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C391">
         <v>1</v>
@@ -5194,10 +5194,10 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B392" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C392">
         <v>1</v>
@@ -5205,10 +5205,10 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B393" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C393">
         <v>1</v>
@@ -5216,10 +5216,10 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B394" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C394">
         <v>1</v>
@@ -5227,10 +5227,10 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B395" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C395">
         <v>1</v>
@@ -5238,10 +5238,10 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B396" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C396">
         <v>1</v>
@@ -5249,10 +5249,10 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B397" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C397">
         <v>1</v>
@@ -5260,10 +5260,10 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B398" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C398">
         <v>1</v>
@@ -5271,10 +5271,10 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B399" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C399">
         <v>1</v>
@@ -5282,10 +5282,10 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B400" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C400">
         <v>1</v>
@@ -5293,10 +5293,10 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B401" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C401">
         <v>1</v>
@@ -5304,10 +5304,10 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B402" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C402">
         <v>1</v>
@@ -5315,10 +5315,10 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B403" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C403">
         <v>1</v>
@@ -5326,10 +5326,10 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B404" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -5337,10 +5337,10 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B405" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C405">
         <v>1</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B406" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C406">
         <v>1</v>
@@ -5359,10 +5359,10 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B407" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C407">
         <v>1</v>
@@ -5370,10 +5370,10 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B408" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C408">
         <v>1</v>
@@ -5384,7 +5384,7 @@
         <v>17</v>
       </c>
       <c r="B409" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C409">
         <v>1</v>
@@ -5395,7 +5395,7 @@
         <v>18</v>
       </c>
       <c r="B410" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C410">
         <v>1</v>
@@ -5406,7 +5406,7 @@
         <v>44</v>
       </c>
       <c r="B411" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C411">
         <v>1</v>
@@ -5417,7 +5417,7 @@
         <v>63</v>
       </c>
       <c r="B412" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C412">
         <v>1</v>
@@ -5425,10 +5425,10 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="B413" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C413">
         <v>1</v>
@@ -5439,7 +5439,7 @@
         <v>19</v>
       </c>
       <c r="B414" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C414">
         <v>1</v>
@@ -5450,7 +5450,7 @@
         <v>20</v>
       </c>
       <c r="B415" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C415">
         <v>1</v>
@@ -5458,10 +5458,10 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B416" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C416">
         <v>1</v>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B417" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C417">
         <v>1</v>
@@ -5480,10 +5480,10 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B418" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C418">
         <v>1</v>
@@ -5491,10 +5491,10 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B419" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C419">
         <v>1</v>
@@ -5502,10 +5502,10 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B420" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C420">
         <v>1</v>
@@ -5513,10 +5513,10 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B421" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C421">
         <v>1</v>
@@ -5524,10 +5524,10 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B422" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C422">
         <v>1</v>
@@ -5535,10 +5535,10 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B423" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C423">
         <v>1</v>
@@ -5546,10 +5546,10 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B424" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C424">
         <v>1</v>
@@ -5560,7 +5560,7 @@
         <v>7</v>
       </c>
       <c r="B425" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C425">
         <v>1</v>
@@ -5571,7 +5571,7 @@
         <v>29</v>
       </c>
       <c r="B426" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C426">
         <v>1</v>
@@ -5582,7 +5582,7 @@
         <v>30</v>
       </c>
       <c r="B427" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C427">
         <v>1</v>
@@ -5593,7 +5593,7 @@
         <v>31</v>
       </c>
       <c r="B428" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C428">
         <v>1</v>
@@ -5604,7 +5604,7 @@
         <v>33</v>
       </c>
       <c r="B429" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C429">
         <v>1</v>
@@ -5615,7 +5615,7 @@
         <v>4</v>
       </c>
       <c r="B430" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C430">
         <v>1</v>
@@ -5626,7 +5626,7 @@
         <v>34</v>
       </c>
       <c r="B431" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C431">
         <v>1</v>
@@ -5637,7 +5637,7 @@
         <v>35</v>
       </c>
       <c r="B432" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C432">
         <v>1</v>
@@ -5648,7 +5648,7 @@
         <v>37</v>
       </c>
       <c r="B433" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C433">
         <v>1</v>
@@ -5681,7 +5681,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5692,10 +5692,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5703,10 +5703,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -5714,10 +5714,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5725,10 +5725,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5736,10 +5736,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5747,10 +5747,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5758,10 +5758,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5769,10 +5769,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5780,10 +5780,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -5791,10 +5791,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
         <v>147</v>
-      </c>
-      <c r="B11" t="s">
-        <v>148</v>
       </c>
       <c r="C11">
         <v>1</v>

</xml_diff>

<commit_message>
some fixes, so germany case study runs
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753B6B18-2BF4-4C7F-86C8-9E9BAEDC0DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890BE4A4-1346-46AF-AAE7-E12FB18AAA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Par_TagFuelToSubsets" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Par_TagTechnologyToSubsets!$A$1:$C$433</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Par_TagTechnologyToSubsets!$A$1:$C$434</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="171">
   <si>
     <t>Technology</t>
   </si>
@@ -879,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C433"/>
+  <dimension ref="A1:C434"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
+      <selection activeCell="A363" sqref="A363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4864,7 +4864,7 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B362" t="s">
         <v>137</v>
@@ -4875,7 +4875,7 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="B363" t="s">
         <v>137</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B364" t="s">
         <v>137</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B365" t="s">
         <v>137</v>
@@ -4908,7 +4908,7 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B366" t="s">
         <v>137</v>
@@ -4919,7 +4919,7 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B367" t="s">
         <v>137</v>
@@ -4930,7 +4930,7 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B368" t="s">
         <v>137</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B369" t="s">
         <v>137</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B370" t="s">
         <v>137</v>
@@ -4963,7 +4963,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B371" t="s">
         <v>137</v>
@@ -4974,7 +4974,7 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B372" t="s">
         <v>137</v>
@@ -4985,7 +4985,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B373" t="s">
         <v>137</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B374" t="s">
         <v>137</v>
@@ -5007,7 +5007,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B375" t="s">
         <v>137</v>
@@ -5018,7 +5018,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B376" t="s">
         <v>137</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B377" t="s">
         <v>137</v>
@@ -5040,10 +5040,10 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="B378" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C378">
         <v>1</v>
@@ -5051,7 +5051,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B379" t="s">
         <v>141</v>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B380" t="s">
         <v>141</v>
@@ -5073,7 +5073,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>160</v>
+        <v>12</v>
       </c>
       <c r="B381" t="s">
         <v>141</v>
@@ -5084,7 +5084,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B382" t="s">
         <v>141</v>
@@ -5095,7 +5095,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B383" t="s">
         <v>141</v>
@@ -5106,7 +5106,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="B384" t="s">
         <v>141</v>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>158</v>
+        <v>7</v>
       </c>
       <c r="B385" t="s">
         <v>141</v>
@@ -5128,7 +5128,7 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B386" t="s">
         <v>141</v>
@@ -5139,7 +5139,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B387" t="s">
         <v>141</v>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B388" t="s">
         <v>141</v>
@@ -5161,7 +5161,7 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="B389" t="s">
         <v>141</v>
@@ -5172,7 +5172,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B390" t="s">
         <v>141</v>
@@ -5183,7 +5183,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="B391" t="s">
         <v>141</v>
@@ -5194,7 +5194,7 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B392" t="s">
         <v>141</v>
@@ -5205,7 +5205,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B393" t="s">
         <v>141</v>
@@ -5216,7 +5216,7 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B394" t="s">
         <v>141</v>
@@ -5227,7 +5227,7 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="B395" t="s">
         <v>141</v>
@@ -5238,7 +5238,7 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B396" t="s">
         <v>141</v>
@@ -5249,7 +5249,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B397" t="s">
         <v>141</v>
@@ -5260,7 +5260,7 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B398" t="s">
         <v>141</v>
@@ -5271,7 +5271,7 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="B399" t="s">
         <v>141</v>
@@ -5282,7 +5282,7 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B400" t="s">
         <v>141</v>
@@ -5293,7 +5293,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="B401" t="s">
         <v>141</v>
@@ -5304,7 +5304,7 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B402" t="s">
         <v>141</v>
@@ -5315,7 +5315,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B403" t="s">
         <v>141</v>
@@ -5326,7 +5326,7 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B404" t="s">
         <v>141</v>
@@ -5337,7 +5337,7 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="B405" t="s">
         <v>141</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B406" t="s">
         <v>141</v>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B407" t="s">
         <v>141</v>
@@ -5370,10 +5370,10 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="B408" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C408">
         <v>1</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
       <c r="B409" t="s">
         <v>142</v>
@@ -5392,7 +5392,7 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B410" t="s">
         <v>142</v>
@@ -5403,7 +5403,7 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B411" t="s">
         <v>142</v>
@@ -5414,7 +5414,7 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B412" t="s">
         <v>142</v>
@@ -5425,7 +5425,7 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="B413" t="s">
         <v>142</v>
@@ -5436,7 +5436,7 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="B414" t="s">
         <v>142</v>
@@ -5447,7 +5447,7 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B415" t="s">
         <v>142</v>
@@ -5458,7 +5458,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="B416" t="s">
         <v>142</v>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
-        <v>167</v>
+        <v>64</v>
       </c>
       <c r="B417" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C417">
         <v>1</v>
@@ -5480,7 +5480,7 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B418" t="s">
         <v>148</v>
@@ -5491,10 +5491,10 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B419" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C419">
         <v>1</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B420" t="s">
         <v>149</v>
@@ -5513,7 +5513,7 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B421" t="s">
         <v>149</v>
@@ -5524,7 +5524,7 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B422" t="s">
         <v>149</v>
@@ -5535,7 +5535,7 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B423" t="s">
         <v>149</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B424" t="s">
         <v>149</v>
@@ -5557,10 +5557,10 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="B425" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C425">
         <v>1</v>
@@ -5568,7 +5568,7 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B426" t="s">
         <v>156</v>
@@ -5579,7 +5579,7 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B427" t="s">
         <v>156</v>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B428" t="s">
         <v>156</v>
@@ -5601,7 +5601,7 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B429" t="s">
         <v>156</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B430" t="s">
         <v>156</v>
@@ -5623,7 +5623,7 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B431" t="s">
         <v>156</v>
@@ -5634,7 +5634,7 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B432" t="s">
         <v>156</v>
@@ -5645,7 +5645,7 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B433" t="s">
         <v>156</v>
@@ -5654,10 +5654,21 @@
         <v>1</v>
       </c>
     </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A434" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B434" t="s">
+        <v>156</v>
+      </c>
+      <c r="C434">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C433" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:C434" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A282:C359">
-      <sortCondition ref="A1:A433"/>
+      <sortCondition ref="A1:A434"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added heatpump geothermal surface and heaetpump geothermal deep
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jb\GENeSYS_MOD.gms\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E7FD77-2966-4668-9C00-D0436F1F1844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3A8D38-8918-4C60-AED5-CF0EA3EB7BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_TagTechnologyToSubsets" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="179">
   <si>
     <t>Technology</t>
   </si>
@@ -562,6 +562,21 @@
   </si>
   <si>
     <t>X_Alkaline_Electrolysis</t>
+  </si>
+  <si>
+    <t>HLR_Heatpump_Geo_Surface</t>
+  </si>
+  <si>
+    <t>HLR_Heatpump_Geo_Deep</t>
+  </si>
+  <si>
+    <t>P_Gas</t>
+  </si>
+  <si>
+    <t>HLR_Gas_CHP</t>
+  </si>
+  <si>
+    <t>HLI_Gas_CHP</t>
   </si>
 </sst>
 </file>
@@ -610,7 +625,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -888,20 +903,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C444"/>
+  <dimension ref="A1:C453"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C371" sqref="C371"/>
+    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
+      <selection activeCell="F448" sqref="F448"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -912,7 +926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -923,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -934,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>159</v>
       </c>
@@ -945,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -956,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -967,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -978,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -989,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1000,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1011,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1022,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1033,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1044,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>160</v>
       </c>
@@ -1055,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -1066,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -1077,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1088,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1099,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1110,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>160</v>
       </c>
@@ -1121,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -1132,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>164</v>
       </c>
@@ -1143,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>158</v>
       </c>
@@ -1165,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>159</v>
       </c>
@@ -1176,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>161</v>
       </c>
@@ -1187,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -1198,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1209,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -1220,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -1242,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>169</v>
       </c>
@@ -1253,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -1264,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>134</v>
       </c>
@@ -1275,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1286,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1297,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1308,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1319,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -1330,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1341,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1352,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1363,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1374,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1385,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1396,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1407,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1418,7 +1432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -1429,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1440,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -1451,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1462,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -1473,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -1484,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -1495,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -1506,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -1517,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -1528,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -1539,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1550,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -1561,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1572,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1583,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1594,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1605,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>93</v>
       </c>
@@ -1616,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>94</v>
       </c>
@@ -1627,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -1638,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>170</v>
       </c>
@@ -1649,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -1660,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>135</v>
       </c>
@@ -1671,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -1682,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -1693,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -1704,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -1715,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1726,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>65</v>
       </c>
@@ -1737,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>71</v>
       </c>
@@ -1748,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
@@ -1759,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
@@ -1770,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>67</v>
       </c>
@@ -1781,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>73</v>
       </c>
@@ -1792,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>69</v>
       </c>
@@ -1803,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>74</v>
       </c>
@@ -1814,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>68</v>
       </c>
@@ -1825,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>14</v>
       </c>
@@ -1836,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>70</v>
       </c>
@@ -1847,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>75</v>
       </c>
@@ -1858,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>76</v>
       </c>
@@ -1869,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>21</v>
       </c>
@@ -1880,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>22</v>
       </c>
@@ -1891,7 +1905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>25</v>
       </c>
@@ -1902,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>24</v>
       </c>
@@ -1913,7 +1927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>23</v>
       </c>
@@ -1924,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>26</v>
       </c>
@@ -1935,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>27</v>
       </c>
@@ -1946,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>28</v>
       </c>
@@ -1957,7 +1971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>53</v>
       </c>
@@ -1968,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>59</v>
       </c>
@@ -1979,7 +1993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>58</v>
       </c>
@@ -1990,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>54</v>
       </c>
@@ -2001,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>60</v>
       </c>
@@ -2012,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>56</v>
       </c>
@@ -2023,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>57</v>
       </c>
@@ -2034,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>55</v>
       </c>
@@ -2045,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>40</v>
       </c>
@@ -2056,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>43</v>
       </c>
@@ -2067,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>44</v>
       </c>
@@ -2078,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>39</v>
       </c>
@@ -2089,7 +2103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>45</v>
       </c>
@@ -2100,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>47</v>
       </c>
@@ -2111,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>41</v>
       </c>
@@ -2122,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>42</v>
       </c>
@@ -2133,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>46</v>
       </c>
@@ -2144,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
@@ -2155,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>30</v>
       </c>
@@ -2166,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>33</v>
       </c>
@@ -2177,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>29</v>
       </c>
@@ -2188,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>36</v>
       </c>
@@ -2199,7 +2213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>38</v>
       </c>
@@ -2210,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>31</v>
       </c>
@@ -2221,7 +2235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>34</v>
       </c>
@@ -2232,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>35</v>
       </c>
@@ -2243,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>32</v>
       </c>
@@ -2254,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>37</v>
       </c>
@@ -2265,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>4</v>
       </c>
@@ -2276,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>49</v>
       </c>
@@ -2287,7 +2301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>48</v>
       </c>
@@ -2298,7 +2312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>61</v>
       </c>
@@ -2309,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>50</v>
       </c>
@@ -2320,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>62</v>
       </c>
@@ -2331,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>52</v>
       </c>
@@ -2342,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>51</v>
       </c>
@@ -2353,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>64</v>
       </c>
@@ -2364,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>19</v>
       </c>
@@ -2375,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>171</v>
       </c>
@@ -2386,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>172</v>
       </c>
@@ -2397,7 +2411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>173</v>
       </c>
@@ -2408,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>17</v>
       </c>
@@ -2419,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>165</v>
       </c>
@@ -2430,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>18</v>
       </c>
@@ -2441,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>20</v>
       </c>
@@ -2452,7 +2466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>63</v>
       </c>
@@ -2463,7 +2477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>170</v>
       </c>
@@ -2474,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>77</v>
       </c>
@@ -2485,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>78</v>
       </c>
@@ -2496,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>79</v>
       </c>
@@ -2507,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>80</v>
       </c>
@@ -2518,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>81</v>
       </c>
@@ -2529,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>82</v>
       </c>
@@ -2540,7 +2554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>83</v>
       </c>
@@ -2551,7 +2565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>84</v>
       </c>
@@ -2562,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>89</v>
       </c>
@@ -2573,7 +2587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>90</v>
       </c>
@@ -2584,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>91</v>
       </c>
@@ -2595,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>92</v>
       </c>
@@ -2606,7 +2620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>93</v>
       </c>
@@ -2617,7 +2631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>94</v>
       </c>
@@ -2628,7 +2642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>95</v>
       </c>
@@ -2639,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>96</v>
       </c>
@@ -2650,7 +2664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>97</v>
       </c>
@@ -2661,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>98</v>
       </c>
@@ -2672,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>66</v>
       </c>
@@ -2683,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>67</v>
       </c>
@@ -2694,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>68</v>
       </c>
@@ -2705,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>72</v>
       </c>
@@ -2716,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>73</v>
       </c>
@@ -2727,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>14</v>
       </c>
@@ -2738,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>76</v>
       </c>
@@ -2749,7 +2763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
@@ -2760,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>66</v>
       </c>
@@ -2771,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>67</v>
       </c>
@@ -2782,7 +2796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>68</v>
       </c>
@@ -2793,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>69</v>
       </c>
@@ -2804,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>70</v>
       </c>
@@ -2815,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>71</v>
       </c>
@@ -2826,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>72</v>
       </c>
@@ -2837,7 +2851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>73</v>
       </c>
@@ -2848,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>14</v>
       </c>
@@ -2859,7 +2873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>74</v>
       </c>
@@ -2870,7 +2884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>75</v>
       </c>
@@ -2881,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>76</v>
       </c>
@@ -2892,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>100</v>
       </c>
@@ -2903,7 +2917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>101</v>
       </c>
@@ -2914,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>115</v>
       </c>
@@ -2925,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>102</v>
       </c>
@@ -2936,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>103</v>
       </c>
@@ -2947,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>104</v>
       </c>
@@ -2958,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>116</v>
       </c>
@@ -2969,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>105</v>
       </c>
@@ -2980,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>106</v>
       </c>
@@ -2991,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>107</v>
       </c>
@@ -3002,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>117</v>
       </c>
@@ -3013,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>108</v>
       </c>
@@ -3024,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>118</v>
       </c>
@@ -3035,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>109</v>
       </c>
@@ -3046,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>119</v>
       </c>
@@ -3057,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>110</v>
       </c>
@@ -3068,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>111</v>
       </c>
@@ -3079,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>112</v>
       </c>
@@ -3090,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>120</v>
       </c>
@@ -3101,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>113</v>
       </c>
@@ -3112,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>108</v>
       </c>
@@ -3123,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>118</v>
       </c>
@@ -3134,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>109</v>
       </c>
@@ -3145,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>119</v>
       </c>
@@ -3156,7 +3170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>110</v>
       </c>
@@ -3167,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>111</v>
       </c>
@@ -3178,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>112</v>
       </c>
@@ -3189,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>120</v>
       </c>
@@ -3200,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>113</v>
       </c>
@@ -3211,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>115</v>
       </c>
@@ -3222,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>102</v>
       </c>
@@ -3233,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>103</v>
       </c>
@@ -3244,7 +3258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>104</v>
       </c>
@@ -3255,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>116</v>
       </c>
@@ -3266,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>105</v>
       </c>
@@ -3277,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>106</v>
       </c>
@@ -3288,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>107</v>
       </c>
@@ -3299,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>117</v>
       </c>
@@ -3310,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>29</v>
       </c>
@@ -3321,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>30</v>
       </c>
@@ -3332,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>31</v>
       </c>
@@ -3343,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>32</v>
       </c>
@@ -3354,7 +3368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>33</v>
       </c>
@@ -3365,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>4</v>
       </c>
@@ -3376,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>34</v>
       </c>
@@ -3387,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>35</v>
       </c>
@@ -3398,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>36</v>
       </c>
@@ -3409,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>37</v>
       </c>
@@ -3420,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>39</v>
       </c>
@@ -3431,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>40</v>
       </c>
@@ -3442,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>41</v>
       </c>
@@ -3453,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>42</v>
       </c>
@@ -3464,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>43</v>
       </c>
@@ -3475,7 +3489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>5</v>
       </c>
@@ -3486,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>44</v>
       </c>
@@ -3497,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>45</v>
       </c>
@@ -3508,7 +3522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>46</v>
       </c>
@@ -3519,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>48</v>
       </c>
@@ -3530,7 +3544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
         <v>49</v>
       </c>
@@ -3541,7 +3555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
         <v>50</v>
       </c>
@@ -3552,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>51</v>
       </c>
@@ -3563,7 +3577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>52</v>
       </c>
@@ -3574,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
         <v>53</v>
       </c>
@@ -3585,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
         <v>54</v>
       </c>
@@ -3596,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
         <v>55</v>
       </c>
@@ -3607,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
         <v>56</v>
       </c>
@@ -3618,7 +3632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
         <v>57</v>
       </c>
@@ -3629,7 +3643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
         <v>58</v>
       </c>
@@ -3640,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
         <v>59</v>
       </c>
@@ -3651,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
         <v>60</v>
       </c>
@@ -3662,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
         <v>61</v>
       </c>
@@ -3673,7 +3687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
         <v>62</v>
       </c>
@@ -3684,7 +3698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
         <v>38</v>
       </c>
@@ -3695,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
         <v>47</v>
       </c>
@@ -3706,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
         <v>65</v>
       </c>
@@ -3717,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
         <v>66</v>
       </c>
@@ -3728,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
         <v>67</v>
       </c>
@@ -3739,7 +3753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
         <v>68</v>
       </c>
@@ -3750,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
         <v>69</v>
       </c>
@@ -3761,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
         <v>70</v>
       </c>
@@ -3772,7 +3786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
         <v>71</v>
       </c>
@@ -3783,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
         <v>72</v>
       </c>
@@ -3794,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="s">
         <v>73</v>
       </c>
@@ -3805,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="s">
         <v>14</v>
       </c>
@@ -3816,7 +3830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="s">
         <v>74</v>
       </c>
@@ -3827,7 +3841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
         <v>75</v>
       </c>
@@ -3838,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
         <v>76</v>
       </c>
@@ -3849,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
         <v>100</v>
       </c>
@@ -3860,7 +3874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
         <v>101</v>
       </c>
@@ -3871,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>84</v>
       </c>
@@ -3882,7 +3896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>83</v>
       </c>
@@ -3893,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>82</v>
       </c>
@@ -3904,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>128</v>
       </c>
@@ -3915,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>129</v>
       </c>
@@ -3926,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
         <v>21</v>
       </c>
@@ -3937,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="s">
         <v>22</v>
       </c>
@@ -3948,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="s">
         <v>23</v>
       </c>
@@ -3959,7 +3973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="s">
         <v>24</v>
       </c>
@@ -3970,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" s="1" t="s">
         <v>26</v>
       </c>
@@ -3981,7 +3995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" s="1" t="s">
         <v>27</v>
       </c>
@@ -3992,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" s="1" t="s">
         <v>28</v>
       </c>
@@ -4003,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" s="1" t="s">
         <v>131</v>
       </c>
@@ -4014,7 +4028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" s="1" t="s">
         <v>25</v>
       </c>
@@ -4025,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" s="1" t="s">
         <v>65</v>
       </c>
@@ -4036,7 +4050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>71</v>
       </c>
@@ -4047,7 +4061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>72</v>
       </c>
@@ -4058,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>73</v>
       </c>
@@ -4069,7 +4083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" s="1" t="s">
         <v>69</v>
       </c>
@@ -4080,7 +4094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>74</v>
       </c>
@@ -4091,7 +4105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>14</v>
       </c>
@@ -4102,7 +4116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292" s="1" t="s">
         <v>70</v>
       </c>
@@ -4113,7 +4127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A293" s="1" t="s">
         <v>75</v>
       </c>
@@ -4124,7 +4138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A294" s="1" t="s">
         <v>21</v>
       </c>
@@ -4135,7 +4149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A295" s="1" t="s">
         <v>22</v>
       </c>
@@ -4146,7 +4160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A296" s="1" t="s">
         <v>25</v>
       </c>
@@ -4157,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A297" s="1" t="s">
         <v>24</v>
       </c>
@@ -4168,7 +4182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A298" s="1" t="s">
         <v>23</v>
       </c>
@@ -4179,7 +4193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
         <v>26</v>
       </c>
@@ -4190,7 +4204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
         <v>27</v>
       </c>
@@ -4201,7 +4215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
         <v>28</v>
       </c>
@@ -4212,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
         <v>103</v>
       </c>
@@ -4223,7 +4237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
         <v>104</v>
       </c>
@@ -4234,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
         <v>106</v>
       </c>
@@ -4245,7 +4259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
         <v>105</v>
       </c>
@@ -4256,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A306" s="1" t="s">
         <v>107</v>
       </c>
@@ -4267,7 +4281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>59</v>
       </c>
@@ -4278,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A308" s="1" t="s">
         <v>58</v>
       </c>
@@ -4289,7 +4303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>60</v>
       </c>
@@ -4300,7 +4314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A310" s="1" t="s">
         <v>56</v>
       </c>
@@ -4311,7 +4325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A311" s="1" t="s">
         <v>57</v>
       </c>
@@ -4322,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A312" s="1" t="s">
         <v>55</v>
       </c>
@@ -4333,7 +4347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A313" s="1" t="s">
         <v>40</v>
       </c>
@@ -4344,7 +4358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A314" s="1" t="s">
         <v>43</v>
       </c>
@@ -4355,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A315" s="1" t="s">
         <v>44</v>
       </c>
@@ -4366,7 +4380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A316" s="1" t="s">
         <v>45</v>
       </c>
@@ -4377,7 +4391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
         <v>47</v>
       </c>
@@ -4388,7 +4402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A318" s="1" t="s">
         <v>5</v>
       </c>
@@ -4399,7 +4413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A319" s="1" t="s">
         <v>30</v>
       </c>
@@ -4410,7 +4424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A320" s="1" t="s">
         <v>33</v>
       </c>
@@ -4421,7 +4435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A321" s="1" t="s">
         <v>36</v>
       </c>
@@ -4432,7 +4446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A322" s="1" t="s">
         <v>38</v>
       </c>
@@ -4443,7 +4457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A323" s="1" t="s">
         <v>34</v>
       </c>
@@ -4454,7 +4468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A324" s="1" t="s">
         <v>35</v>
       </c>
@@ -4465,7 +4479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A325" s="1" t="s">
         <v>4</v>
       </c>
@@ -4476,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A326" s="1" t="s">
         <v>49</v>
       </c>
@@ -4487,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>61</v>
       </c>
@@ -4498,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>62</v>
       </c>
@@ -4509,7 +4523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A329" s="1" t="s">
         <v>51</v>
       </c>
@@ -4520,7 +4534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A330" s="1" t="s">
         <v>133</v>
       </c>
@@ -4531,7 +4545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>134</v>
       </c>
@@ -4542,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>93</v>
       </c>
@@ -4553,7 +4567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>94</v>
       </c>
@@ -4564,7 +4578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>95</v>
       </c>
@@ -4575,7 +4589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A335" s="1" t="s">
         <v>64</v>
       </c>
@@ -4586,7 +4600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A336" s="1" t="s">
         <v>108</v>
       </c>
@@ -4597,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A337" s="1" t="s">
         <v>109</v>
       </c>
@@ -4608,7 +4622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A338" s="1" t="s">
         <v>111</v>
       </c>
@@ -4619,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A339" s="1" t="s">
         <v>112</v>
       </c>
@@ -4630,7 +4644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A340" s="1" t="s">
         <v>113</v>
       </c>
@@ -4641,7 +4655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A341" s="1" t="s">
         <v>8</v>
       </c>
@@ -4652,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A342" s="1" t="s">
         <v>166</v>
       </c>
@@ -4663,7 +4677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A343" s="1" t="s">
         <v>167</v>
       </c>
@@ -4674,7 +4688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A344" s="1" t="s">
         <v>168</v>
       </c>
@@ -4685,7 +4699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A345" s="1" t="s">
         <v>169</v>
       </c>
@@ -4696,7 +4710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A346" s="1" t="s">
         <v>158</v>
       </c>
@@ -4707,7 +4721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A347" s="1" t="s">
         <v>7</v>
       </c>
@@ -4718,7 +4732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A348" s="1" t="s">
         <v>161</v>
       </c>
@@ -4729,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A349" s="1" t="s">
         <v>163</v>
       </c>
@@ -4740,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A350" s="1" t="s">
         <v>159</v>
       </c>
@@ -4751,7 +4765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A351" s="1" t="s">
         <v>6</v>
       </c>
@@ -4762,7 +4776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A352" s="1" t="s">
         <v>10</v>
       </c>
@@ -4773,7 +4787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A353" s="1" t="s">
         <v>11</v>
       </c>
@@ -4784,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A354" s="1" t="s">
         <v>12</v>
       </c>
@@ -4795,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A355" s="1" t="s">
         <v>162</v>
       </c>
@@ -4806,7 +4820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A356" s="1" t="s">
         <v>164</v>
       </c>
@@ -4817,7 +4831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A357" s="1" t="s">
         <v>160</v>
       </c>
@@ -4828,7 +4842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A358" s="1" t="s">
         <v>19</v>
       </c>
@@ -4839,7 +4853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>136</v>
       </c>
@@ -4850,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>135</v>
       </c>
@@ -4861,7 +4875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A361" s="1" t="s">
         <v>171</v>
       </c>
@@ -4872,7 +4886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A362" s="1" t="s">
         <v>172</v>
       </c>
@@ -4883,7 +4897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A363" s="1" t="s">
         <v>173</v>
       </c>
@@ -4894,7 +4908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A364" s="1" t="s">
         <v>17</v>
       </c>
@@ -4905,7 +4919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>170</v>
       </c>
@@ -4916,7 +4930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A366" s="1" t="s">
         <v>89</v>
       </c>
@@ -4927,7 +4941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A367" s="1" t="s">
         <v>90</v>
       </c>
@@ -4938,7 +4952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A368" s="1" t="s">
         <v>91</v>
       </c>
@@ -4949,7 +4963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A369" s="1" t="s">
         <v>92</v>
       </c>
@@ -4960,7 +4974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A370" s="1" t="s">
         <v>63</v>
       </c>
@@ -4971,7 +4985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A371" s="1" t="s">
         <v>29</v>
       </c>
@@ -4982,7 +4996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A372" s="1" t="s">
         <v>31</v>
       </c>
@@ -4993,7 +5007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A373" s="1" t="s">
         <v>32</v>
       </c>
@@ -5004,7 +5018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A374" s="1" t="s">
         <v>37</v>
       </c>
@@ -5015,7 +5029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A375" s="1" t="s">
         <v>39</v>
       </c>
@@ -5026,7 +5040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A376" s="1" t="s">
         <v>41</v>
       </c>
@@ -5037,7 +5051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A377" s="1" t="s">
         <v>42</v>
       </c>
@@ -5048,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A378" s="1" t="s">
         <v>46</v>
       </c>
@@ -5059,7 +5073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A379" s="1" t="s">
         <v>48</v>
       </c>
@@ -5070,7 +5084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A380" s="1" t="s">
         <v>50</v>
       </c>
@@ -5081,7 +5095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A381" s="1" t="s">
         <v>52</v>
       </c>
@@ -5092,7 +5106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A382" s="1" t="s">
         <v>53</v>
       </c>
@@ -5103,7 +5117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A383" s="1" t="s">
         <v>66</v>
       </c>
@@ -5114,7 +5128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A384" s="1" t="s">
         <v>67</v>
       </c>
@@ -5125,7 +5139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A385" s="1" t="s">
         <v>76</v>
       </c>
@@ -5136,7 +5150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A386" s="1" t="s">
         <v>10</v>
       </c>
@@ -5147,7 +5161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A387" s="1" t="s">
         <v>11</v>
       </c>
@@ -5158,7 +5172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A388" s="1" t="s">
         <v>12</v>
       </c>
@@ -5169,7 +5183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A389" s="1" t="s">
         <v>160</v>
       </c>
@@ -5180,7 +5194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A390" s="1" t="s">
         <v>162</v>
       </c>
@@ -5191,7 +5205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A391" s="1" t="s">
         <v>164</v>
       </c>
@@ -5202,7 +5216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A392" s="1" t="s">
         <v>7</v>
       </c>
@@ -5213,7 +5227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A393" s="1" t="s">
         <v>158</v>
       </c>
@@ -5224,7 +5238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A394" s="1" t="s">
         <v>159</v>
       </c>
@@ -5235,7 +5249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A395" s="1" t="s">
         <v>161</v>
       </c>
@@ -5246,7 +5260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A396" s="1" t="s">
         <v>163</v>
       </c>
@@ -5257,7 +5271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A397" s="1" t="s">
         <v>6</v>
       </c>
@@ -5268,7 +5282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A398" s="1" t="s">
         <v>8</v>
       </c>
@@ -5279,7 +5293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A399" s="1" t="s">
         <v>166</v>
       </c>
@@ -5290,7 +5304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A400" s="1" t="s">
         <v>168</v>
       </c>
@@ -5301,7 +5315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A401" s="1" t="s">
         <v>167</v>
       </c>
@@ -5312,7 +5326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A402" s="1" t="s">
         <v>169</v>
       </c>
@@ -5323,7 +5337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A403" s="1" t="s">
         <v>89</v>
       </c>
@@ -5334,7 +5348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A404" s="1" t="s">
         <v>90</v>
       </c>
@@ -5345,7 +5359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A405" s="1" t="s">
         <v>91</v>
       </c>
@@ -5356,7 +5370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A406" s="1" t="s">
         <v>92</v>
       </c>
@@ -5367,7 +5381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A407" s="1" t="s">
         <v>133</v>
       </c>
@@ -5378,7 +5392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A408" s="1" t="s">
         <v>134</v>
       </c>
@@ -5389,7 +5403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A409" s="1" t="s">
         <v>94</v>
       </c>
@@ -5400,7 +5414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A410" s="1" t="s">
         <v>93</v>
       </c>
@@ -5411,7 +5425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A411" s="1" t="s">
         <v>95</v>
       </c>
@@ -5422,7 +5436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A412" s="1" t="s">
         <v>64</v>
       </c>
@@ -5433,7 +5447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A413" s="1" t="s">
         <v>96</v>
       </c>
@@ -5444,7 +5458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A414" s="1" t="s">
         <v>97</v>
       </c>
@@ -5455,7 +5469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A415" s="1" t="s">
         <v>98</v>
       </c>
@@ -5466,7 +5480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A416" s="1" t="s">
         <v>165</v>
       </c>
@@ -5477,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A417" s="1" t="s">
         <v>171</v>
       </c>
@@ -5488,7 +5502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A418" s="1" t="s">
         <v>172</v>
       </c>
@@ -5499,7 +5513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A419" s="1" t="s">
         <v>173</v>
       </c>
@@ -5510,7 +5524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A420" s="1" t="s">
         <v>17</v>
       </c>
@@ -5521,7 +5535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="421" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A421" s="1" t="s">
         <v>18</v>
       </c>
@@ -5532,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A422" s="1" t="s">
         <v>44</v>
       </c>
@@ -5543,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="423" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A423" s="1" t="s">
         <v>63</v>
       </c>
@@ -5554,7 +5568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A424" s="1" t="s">
         <v>170</v>
       </c>
@@ -5565,7 +5579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A425" s="1" t="s">
         <v>19</v>
       </c>
@@ -5576,7 +5590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A426" s="1" t="s">
         <v>20</v>
       </c>
@@ -5587,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A427" s="1" t="s">
         <v>64</v>
       </c>
@@ -5598,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A428" s="1" t="s">
         <v>167</v>
       </c>
@@ -5609,7 +5623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A429" s="1" t="s">
         <v>168</v>
       </c>
@@ -5620,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A430" s="1" t="s">
         <v>150</v>
       </c>
@@ -5631,7 +5645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A431" s="1" t="s">
         <v>151</v>
       </c>
@@ -5642,7 +5656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A432" s="1" t="s">
         <v>152</v>
       </c>
@@ -5653,7 +5667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A433" s="1" t="s">
         <v>153</v>
       </c>
@@ -5664,7 +5678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A434" s="1" t="s">
         <v>154</v>
       </c>
@@ -5675,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A435" s="1" t="s">
         <v>155</v>
       </c>
@@ -5686,7 +5700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A436" s="1" t="s">
         <v>7</v>
       </c>
@@ -5697,7 +5711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="437" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A437" s="1" t="s">
         <v>29</v>
       </c>
@@ -5708,7 +5722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A438" s="1" t="s">
         <v>30</v>
       </c>
@@ -5719,7 +5733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A439" s="1" t="s">
         <v>31</v>
       </c>
@@ -5730,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A440" s="1" t="s">
         <v>33</v>
       </c>
@@ -5741,7 +5755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A441" s="1" t="s">
         <v>4</v>
       </c>
@@ -5752,7 +5766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="442" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A442" s="1" t="s">
         <v>34</v>
       </c>
@@ -5763,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A443" s="1" t="s">
         <v>35</v>
       </c>
@@ -5774,7 +5788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="444" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A444" s="1" t="s">
         <v>37</v>
       </c>
@@ -5785,13 +5799,107 @@
         <v>1</v>
       </c>
     </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A445" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B445" t="s">
+        <v>132</v>
+      </c>
+      <c r="C445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A446" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B446" t="s">
+        <v>132</v>
+      </c>
+      <c r="C446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A447" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B447" t="s">
+        <v>132</v>
+      </c>
+      <c r="C447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A448" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B448" t="s">
+        <v>132</v>
+      </c>
+      <c r="C448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A449" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B449" t="s">
+        <v>137</v>
+      </c>
+      <c r="C449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A450" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B450" t="s">
+        <v>137</v>
+      </c>
+      <c r="C450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A451" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B451" t="s">
+        <v>137</v>
+      </c>
+      <c r="C451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A452" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B452" t="s">
+        <v>137</v>
+      </c>
+      <c r="C452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A453" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B453" t="s">
+        <v>137</v>
+      </c>
+      <c r="C453">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C444" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="PhaseOutSet"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A285:C365">
       <sortCondition ref="A1:A444"/>
     </sortState>
@@ -5809,13 +5917,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -5826,7 +5934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>124</v>
       </c>
@@ -5837,7 +5945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
@@ -5848,7 +5956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -5859,7 +5967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>139</v>
       </c>
@@ -5870,7 +5978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -5881,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -5892,7 +6000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
@@ -5903,7 +6011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>144</v>
       </c>
@@ -5914,7 +6022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>145</v>
       </c>
@@ -5925,7 +6033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
-added Osterpaket and FEP to scenario data; -updates 50% heat equation to include district heating; -solved division by zero errors
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jb\GENeSYS_MOD.gms\Inputdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3A8D38-8918-4C60-AED5-CF0EA3EB7BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B538A94-42E8-4126-917C-4CC791C7F63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="15" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_TagTechnologyToSubsets" sheetId="1" r:id="rId1"/>
     <sheet name="Par_TagFuelToSubsets" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Par_TagTechnologyToSubsets!$A$1:$C$444</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Par_TagTechnologyToSubsets!$A$1:$C$453</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="179">
   <si>
     <t>Technology</t>
   </si>
@@ -625,7 +625,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -903,19 +903,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C453"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
-      <selection activeCell="F448" sqref="F448"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H456" sqref="H456"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.7265625" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -926,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -937,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -948,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>159</v>
       </c>
@@ -959,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -970,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -981,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -992,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>160</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1124,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>160</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>164</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1168,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>158</v>
       </c>
@@ -1179,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>159</v>
       </c>
@@ -1190,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>161</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1223,7 +1224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -1234,7 +1235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>169</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>134</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1322,29 +1323,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1388,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1399,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1476,7 +1477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -1487,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -1498,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -1520,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1586,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>93</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>94</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>170</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -1674,7 +1675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>135</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -1696,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -1718,7 +1719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>65</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>71</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>67</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>73</v>
       </c>
@@ -1806,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>69</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>74</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>68</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>14</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>70</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>75</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>76</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>21</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>22</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>25</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>24</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>23</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>26</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>27</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>28</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>53</v>
       </c>
@@ -1982,7 +1983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>59</v>
       </c>
@@ -1993,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>58</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>54</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>60</v>
       </c>
@@ -2026,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>56</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>57</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>55</v>
       </c>
@@ -2059,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>40</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>43</v>
       </c>
@@ -2081,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>44</v>
       </c>
@@ -2092,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>39</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>45</v>
       </c>
@@ -2114,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>47</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>41</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>42</v>
       </c>
@@ -2147,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>46</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
@@ -2169,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>30</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>33</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>29</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>36</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>38</v>
       </c>
@@ -2224,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>31</v>
       </c>
@@ -2235,29 +2236,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B121" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B122" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>32</v>
       </c>
@@ -2268,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>37</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>4</v>
       </c>
@@ -2290,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>49</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>48</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>61</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>50</v>
       </c>
@@ -2334,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>62</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>52</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>51</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>64</v>
       </c>
@@ -2378,7 +2379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>19</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>171</v>
       </c>
@@ -2400,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>172</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>173</v>
       </c>
@@ -2422,7 +2423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>17</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>165</v>
       </c>
@@ -2444,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>18</v>
       </c>
@@ -2455,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>20</v>
       </c>
@@ -2466,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>63</v>
       </c>
@@ -2477,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>170</v>
       </c>
@@ -2488,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>77</v>
       </c>
@@ -2499,7 +2500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>78</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>79</v>
       </c>
@@ -2521,7 +2522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>80</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>81</v>
       </c>
@@ -2543,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>82</v>
       </c>
@@ -2554,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>83</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>84</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>89</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>90</v>
       </c>
@@ -2598,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>91</v>
       </c>
@@ -2609,7 +2610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>92</v>
       </c>
@@ -2620,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>93</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>94</v>
       </c>
@@ -2642,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>95</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>96</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>97</v>
       </c>
@@ -2675,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>98</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>66</v>
       </c>
@@ -2697,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>67</v>
       </c>
@@ -2708,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>68</v>
       </c>
@@ -2719,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>72</v>
       </c>
@@ -2730,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>73</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>14</v>
       </c>
@@ -2752,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>76</v>
       </c>
@@ -2763,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
@@ -2774,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>66</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>67</v>
       </c>
@@ -2796,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>68</v>
       </c>
@@ -2807,7 +2808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>69</v>
       </c>
@@ -2818,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>70</v>
       </c>
@@ -2829,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>71</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>72</v>
       </c>
@@ -2851,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>73</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>14</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>74</v>
       </c>
@@ -2884,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>75</v>
       </c>
@@ -2895,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>76</v>
       </c>
@@ -2906,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>100</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>101</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>115</v>
       </c>
@@ -2939,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>102</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>103</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>104</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>116</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>105</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>106</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>107</v>
       </c>
@@ -3016,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>117</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>108</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>118</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>109</v>
       </c>
@@ -3060,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>119</v>
       </c>
@@ -3071,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>110</v>
       </c>
@@ -3082,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>111</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>112</v>
       </c>
@@ -3104,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>120</v>
       </c>
@@ -3115,7 +3116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>113</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>108</v>
       </c>
@@ -3137,7 +3138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>118</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>109</v>
       </c>
@@ -3159,7 +3160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>119</v>
       </c>
@@ -3170,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>110</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>111</v>
       </c>
@@ -3192,7 +3193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>112</v>
       </c>
@@ -3203,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>120</v>
       </c>
@@ -3214,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>113</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>115</v>
       </c>
@@ -3236,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>102</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>103</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>104</v>
       </c>
@@ -3269,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>116</v>
       </c>
@@ -3280,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>105</v>
       </c>
@@ -3291,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>106</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>107</v>
       </c>
@@ -3313,7 +3314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>117</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>29</v>
       </c>
@@ -3335,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>30</v>
       </c>
@@ -3346,7 +3347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>31</v>
       </c>
@@ -3357,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>32</v>
       </c>
@@ -3368,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>33</v>
       </c>
@@ -3379,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>4</v>
       </c>
@@ -3390,29 +3391,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B226" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C226">
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B227" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C227">
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>36</v>
       </c>
@@ -3423,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>37</v>
       </c>
@@ -3434,7 +3435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>39</v>
       </c>
@@ -3445,7 +3446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>40</v>
       </c>
@@ -3456,7 +3457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>41</v>
       </c>
@@ -3467,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>42</v>
       </c>
@@ -3478,7 +3479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>43</v>
       </c>
@@ -3489,7 +3490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>5</v>
       </c>
@@ -3500,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>44</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>45</v>
       </c>
@@ -3522,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>46</v>
       </c>
@@ -3533,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>48</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>49</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>50</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>51</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>52</v>
       </c>
@@ -3588,7 +3589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>53</v>
       </c>
@@ -3599,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>54</v>
       </c>
@@ -3610,7 +3611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>55</v>
       </c>
@@ -3621,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>56</v>
       </c>
@@ -3632,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>57</v>
       </c>
@@ -3643,7 +3644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>58</v>
       </c>
@@ -3654,7 +3655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>59</v>
       </c>
@@ -3665,7 +3666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>60</v>
       </c>
@@ -3676,7 +3677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>61</v>
       </c>
@@ -3687,7 +3688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>62</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>38</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>47</v>
       </c>
@@ -3720,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>65</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>66</v>
       </c>
@@ -3742,7 +3743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>67</v>
       </c>
@@ -3753,7 +3754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>68</v>
       </c>
@@ -3764,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>69</v>
       </c>
@@ -3775,7 +3776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>70</v>
       </c>
@@ -3786,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>71</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>72</v>
       </c>
@@ -3808,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>73</v>
       </c>
@@ -3819,7 +3820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>14</v>
       </c>
@@ -3830,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>74</v>
       </c>
@@ -3841,7 +3842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>75</v>
       </c>
@@ -3852,7 +3853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>76</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>100</v>
       </c>
@@ -3874,7 +3875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>101</v>
       </c>
@@ -3885,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>84</v>
       </c>
@@ -3896,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>83</v>
       </c>
@@ -3907,7 +3908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>82</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>128</v>
       </c>
@@ -3929,7 +3930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>129</v>
       </c>
@@ -3940,7 +3941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>21</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>22</v>
       </c>
@@ -3962,7 +3963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>23</v>
       </c>
@@ -3973,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>24</v>
       </c>
@@ -3984,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>26</v>
       </c>
@@ -3995,7 +3996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>27</v>
       </c>
@@ -4006,7 +4007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>28</v>
       </c>
@@ -4017,7 +4018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>131</v>
       </c>
@@ -4028,7 +4029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>25</v>
       </c>
@@ -4039,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>65</v>
       </c>
@@ -4050,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>71</v>
       </c>
@@ -4061,7 +4062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>72</v>
       </c>
@@ -4072,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>73</v>
       </c>
@@ -4083,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>69</v>
       </c>
@@ -4094,7 +4095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>74</v>
       </c>
@@ -4105,7 +4106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>14</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>70</v>
       </c>
@@ -4127,7 +4128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>75</v>
       </c>
@@ -4138,7 +4139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>21</v>
       </c>
@@ -4149,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>22</v>
       </c>
@@ -4160,7 +4161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>25</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>24</v>
       </c>
@@ -4182,7 +4183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>23</v>
       </c>
@@ -4193,7 +4194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>26</v>
       </c>
@@ -4204,7 +4205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>27</v>
       </c>
@@ -4215,7 +4216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>28</v>
       </c>
@@ -4226,7 +4227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>103</v>
       </c>
@@ -4237,7 +4238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>104</v>
       </c>
@@ -4248,7 +4249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>106</v>
       </c>
@@ -4259,7 +4260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>105</v>
       </c>
@@ -4270,7 +4271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>107</v>
       </c>
@@ -4281,7 +4282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>59</v>
       </c>
@@ -4292,7 +4293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>58</v>
       </c>
@@ -4303,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>60</v>
       </c>
@@ -4314,7 +4315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>56</v>
       </c>
@@ -4325,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>57</v>
       </c>
@@ -4336,7 +4337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>55</v>
       </c>
@@ -4347,7 +4348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>40</v>
       </c>
@@ -4358,7 +4359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>43</v>
       </c>
@@ -4369,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>44</v>
       </c>
@@ -4380,7 +4381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>45</v>
       </c>
@@ -4391,7 +4392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>47</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>5</v>
       </c>
@@ -4413,7 +4414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>30</v>
       </c>
@@ -4424,7 +4425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>33</v>
       </c>
@@ -4435,7 +4436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>36</v>
       </c>
@@ -4446,7 +4447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>38</v>
       </c>
@@ -4457,9 +4458,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="B323" t="s">
         <v>132</v>
@@ -4468,9 +4469,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>35</v>
+        <v>175</v>
       </c>
       <c r="B324" t="s">
         <v>132</v>
@@ -4479,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>4</v>
       </c>
@@ -4490,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>49</v>
       </c>
@@ -4501,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>61</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>62</v>
       </c>
@@ -4523,7 +4524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>51</v>
       </c>
@@ -4534,7 +4535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>133</v>
       </c>
@@ -4545,7 +4546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>134</v>
       </c>
@@ -4556,7 +4557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>93</v>
       </c>
@@ -4567,7 +4568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>94</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>95</v>
       </c>
@@ -4589,7 +4590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>64</v>
       </c>
@@ -4600,7 +4601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>108</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>109</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>111</v>
       </c>
@@ -4633,7 +4634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>112</v>
       </c>
@@ -4644,7 +4645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>113</v>
       </c>
@@ -4655,7 +4656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>8</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>166</v>
       </c>
@@ -4677,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>167</v>
       </c>
@@ -4688,7 +4689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>168</v>
       </c>
@@ -4699,7 +4700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>169</v>
       </c>
@@ -4710,7 +4711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>158</v>
       </c>
@@ -4721,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>7</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>161</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>163</v>
       </c>
@@ -4754,7 +4755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>159</v>
       </c>
@@ -4765,7 +4766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>6</v>
       </c>
@@ -4776,7 +4777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>10</v>
       </c>
@@ -4787,7 +4788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>11</v>
       </c>
@@ -4798,7 +4799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>12</v>
       </c>
@@ -4809,7 +4810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>162</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>164</v>
       </c>
@@ -4831,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>160</v>
       </c>
@@ -4842,7 +4843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>19</v>
       </c>
@@ -4853,7 +4854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>136</v>
       </c>
@@ -4864,7 +4865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>135</v>
       </c>
@@ -4875,7 +4876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>171</v>
       </c>
@@ -4886,7 +4887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>172</v>
       </c>
@@ -4897,7 +4898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:3" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>173</v>
       </c>
@@ -4908,7 +4909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>17</v>
       </c>
@@ -4919,7 +4920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>170</v>
       </c>
@@ -4930,7 +4931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>89</v>
       </c>
@@ -4941,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>90</v>
       </c>
@@ -4952,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>91</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>92</v>
       </c>
@@ -4974,7 +4975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>63</v>
       </c>
@@ -4985,7 +4986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>29</v>
       </c>
@@ -4996,7 +4997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>31</v>
       </c>
@@ -5007,7 +5008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>32</v>
       </c>
@@ -5018,7 +5019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>37</v>
       </c>
@@ -5029,7 +5030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>39</v>
       </c>
@@ -5040,7 +5041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>41</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>42</v>
       </c>
@@ -5062,7 +5063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>46</v>
       </c>
@@ -5073,7 +5074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>48</v>
       </c>
@@ -5084,7 +5085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>50</v>
       </c>
@@ -5095,7 +5096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>52</v>
       </c>
@@ -5106,7 +5107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>53</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>66</v>
       </c>
@@ -5128,7 +5129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>67</v>
       </c>
@@ -5139,7 +5140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>76</v>
       </c>
@@ -5150,7 +5151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>10</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>11</v>
       </c>
@@ -5172,7 +5173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>12</v>
       </c>
@@ -5183,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>160</v>
       </c>
@@ -5194,7 +5195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>162</v>
       </c>
@@ -5205,7 +5206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>164</v>
       </c>
@@ -5216,7 +5217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>7</v>
       </c>
@@ -5227,7 +5228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>158</v>
       </c>
@@ -5238,7 +5239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>159</v>
       </c>
@@ -5249,7 +5250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>161</v>
       </c>
@@ -5260,7 +5261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>163</v>
       </c>
@@ -5271,7 +5272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>6</v>
       </c>
@@ -5282,7 +5283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>8</v>
       </c>
@@ -5293,7 +5294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>166</v>
       </c>
@@ -5304,7 +5305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>168</v>
       </c>
@@ -5315,7 +5316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>167</v>
       </c>
@@ -5326,7 +5327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>169</v>
       </c>
@@ -5337,7 +5338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>89</v>
       </c>
@@ -5348,7 +5349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>90</v>
       </c>
@@ -5359,7 +5360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>91</v>
       </c>
@@ -5370,7 +5371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>92</v>
       </c>
@@ -5381,7 +5382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>133</v>
       </c>
@@ -5392,7 +5393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>134</v>
       </c>
@@ -5403,7 +5404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>94</v>
       </c>
@@ -5414,7 +5415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>93</v>
       </c>
@@ -5425,7 +5426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>95</v>
       </c>
@@ -5436,7 +5437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>64</v>
       </c>
@@ -5447,7 +5448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>96</v>
       </c>
@@ -5458,7 +5459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>97</v>
       </c>
@@ -5469,7 +5470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>98</v>
       </c>
@@ -5480,7 +5481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>165</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>171</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>172</v>
       </c>
@@ -5513,7 +5514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:3" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>173</v>
       </c>
@@ -5524,7 +5525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>17</v>
       </c>
@@ -5535,7 +5536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>18</v>
       </c>
@@ -5546,7 +5547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>44</v>
       </c>
@@ -5557,7 +5558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
         <v>63</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>170</v>
       </c>
@@ -5579,7 +5580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
         <v>19</v>
       </c>
@@ -5590,7 +5591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>20</v>
       </c>
@@ -5601,7 +5602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
         <v>64</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>167</v>
       </c>
@@ -5623,7 +5624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
         <v>168</v>
       </c>
@@ -5634,7 +5635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>150</v>
       </c>
@@ -5645,7 +5646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
         <v>151</v>
       </c>
@@ -5656,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
         <v>152</v>
       </c>
@@ -5667,7 +5668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
         <v>153</v>
       </c>
@@ -5678,7 +5679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
         <v>154</v>
       </c>
@@ -5689,7 +5690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
         <v>155</v>
       </c>
@@ -5700,7 +5701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
         <v>7</v>
       </c>
@@ -5711,7 +5712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
         <v>29</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
         <v>30</v>
       </c>
@@ -5733,7 +5734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
         <v>31</v>
       </c>
@@ -5744,7 +5745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>33</v>
       </c>
@@ -5755,7 +5756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
         <v>4</v>
       </c>
@@ -5766,29 +5767,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A442" s="1" t="s">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
         <v>34</v>
       </c>
       <c r="B442" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="C442">
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A443" s="1" t="s">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
         <v>35</v>
       </c>
       <c r="B443" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="C443">
         <v>1</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
         <v>37</v>
       </c>
@@ -5799,29 +5800,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
-        <v>174</v>
+        <v>34</v>
       </c>
       <c r="B445" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="C445">
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
-        <v>175</v>
+        <v>35</v>
       </c>
       <c r="B446" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="C446">
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
         <v>101</v>
       </c>
@@ -5832,7 +5833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
         <v>100</v>
       </c>
@@ -5843,7 +5844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
         <v>176</v>
       </c>
@@ -5854,7 +5855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
         <v>177</v>
       </c>
@@ -5865,7 +5866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
         <v>178</v>
       </c>
@@ -5876,7 +5877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>76</v>
       </c>
@@ -5887,7 +5888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
         <v>101</v>
       </c>
@@ -5898,10 +5899,106 @@
         <v>1</v>
       </c>
     </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A454" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B454" t="s">
+        <v>126</v>
+      </c>
+      <c r="C454">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A455" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B455" t="s">
+        <v>126</v>
+      </c>
+      <c r="C455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A456" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B456" t="s">
+        <v>156</v>
+      </c>
+      <c r="C456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A457" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B457" t="s">
+        <v>156</v>
+      </c>
+      <c r="C457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A458" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B458" t="s">
+        <v>13</v>
+      </c>
+      <c r="C458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A459" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B459" t="s">
+        <v>13</v>
+      </c>
+      <c r="C459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A460" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B460" t="s">
+        <v>16</v>
+      </c>
+      <c r="C460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A461" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B461" t="s">
+        <v>16</v>
+      </c>
+      <c r="C461">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C444" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A285:C365">
-      <sortCondition ref="A1:A444"/>
+  <autoFilter ref="A1:C453" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="HLR_Heatpump_Aerial"/>
+        <filter val="HLR_Heatpump_Geo_Deep"/>
+        <filter val="HLR_Heatpump_Geo_Surface"/>
+        <filter val="HLR_Heatpump_Ground"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:C446">
+      <sortCondition ref="B1:B453"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5917,13 +6014,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -5934,7 +6031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>124</v>
       </c>
@@ -5945,7 +6042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
@@ -5956,7 +6053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -5967,7 +6064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>139</v>
       </c>
@@ -5978,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -5989,7 +6086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -6000,7 +6097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
@@ -6011,7 +6108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>144</v>
       </c>
@@ -6022,7 +6119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>145</v>
       </c>
@@ -6033,7 +6130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
- adjusted employment constraints
</commit_message>
<xml_diff>
--- a/Inputdata/Tag_Subsets.xlsx
+++ b/Inputdata/Tag_Subsets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.gms\Inputdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhep\Documents\git\GENeSYS-MOD_GroupRepo\GENeSYS-MOD_GAMS\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42981DC4-CC28-442B-8653-E86745450AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FB2B4D-B50D-41D1-ABA8-99521F25275D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_TagTechnologyToSubsets" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -913,7 +913,7 @@
   <dimension ref="A1:C461"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E315" sqref="E315"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>70</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>73</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>14</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>66</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>73</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>69</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>74</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>68</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>14</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>70</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>75</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>76</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>34</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>175</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>174</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>35</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>34</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>175</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>174</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>35</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>65</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>71</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>72</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>73</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>69</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>74</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>14</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>70</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>75</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>34</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>175</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>174</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>35</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>66</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>67</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>76</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>76</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>65</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>71</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>69</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>74</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>70</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>34</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>175</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>174</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>35</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>65</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>71</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>66</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>72</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>67</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>73</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>69</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>74</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>68</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>14</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>70</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>75</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>76</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>34</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>175</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>174</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>35</v>
       </c>
@@ -5997,13 +5997,22 @@
   <autoFilter ref="A1:C461" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="HLR_Heatpump_Aerial"/>
-        <filter val="HLR_Heatpump_Geo_Deep"/>
-        <filter val="HLR_Heatpump_Geo_Surface"/>
-        <filter val="HLR_Heatpump_Ground"/>
+        <filter val="CHP_Biomass_Solid"/>
+        <filter val="CHP_Biomass_Solid_CCS"/>
+        <filter val="CHP_Coal_Hardcoal"/>
+        <filter val="CHP_Coal_Hardcoal_CCS"/>
+        <filter val="CHP_Coal_Lignite"/>
+        <filter val="CHP_Coal_Lignite_CCS"/>
+        <filter val="CHP_Gas_CCGT_Biogas"/>
+        <filter val="CHP_Gas_CCGT_Biogas_CCS"/>
+        <filter val="CHP_Gas_CCGT_Natural"/>
+        <filter val="CHP_Gas_CCGT_Natural_CCS"/>
+        <filter val="CHP_Gas_CCGT_SynGas"/>
+        <filter val="CHP_Hydrogen_FuelCell"/>
+        <filter val="CHP_Oil"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C461">
+    <sortState ref="A2:C461">
       <sortCondition ref="B1:B461"/>
     </sortState>
   </autoFilter>

</xml_diff>